<commit_message>
Cell Colorization for Libre Office corrected
</commit_message>
<xml_diff>
--- a/BasePlanning.xlsx
+++ b/BasePlanning.xlsx
@@ -907,25 +907,519 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="cf1" xfId="2"/>
     <cellStyle name="Prozent" xfId="1" builtinId="5" customBuiltin="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="58">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8696B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF63BE7B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF63BE7B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8696B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="2" tint="-0.24994659260841701"/>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8696B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF63BE7B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF63BE7B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8696B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="2" tint="-0.24994659260841701"/>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8696B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF63BE7B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF63BE7B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8696B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="2" tint="-0.24994659260841701"/>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF63BE7B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8696B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF63BE7B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8696B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="2" tint="-0.24994659260841701"/>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8696B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF63BE7B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8696B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="2" tint="-0.24994659260841701"/>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF63BE7B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8696B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="2" tint="-0.24994659260841701"/>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF63BE7B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8696B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749961851863155"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="2" tint="-0.24994659260841701"/>
+          <bgColor theme="2" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -976,6 +1470,7 @@
   <colors>
     <mruColors>
       <color rgb="FF63BE7B"/>
+      <color rgb="FFF8696B"/>
       <color rgb="FFFFEB84"/>
     </mruColors>
   </colors>
@@ -1273,7 +1768,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F122" sqref="F122"/>
+      <selection pane="bottomRight" activeCell="BE8" sqref="BE8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1334,10 +1829,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:122" ht="153" customHeight="1">
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="43" t="s">
         <v>210</v>
       </c>
-      <c r="C1" s="37"/>
+      <c r="C1" s="43"/>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1717,12 +2212,12 @@
         <v/>
       </c>
       <c r="F2" s="19"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="40"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="19"/>
-      <c r="L2" s="41"/>
+      <c r="L2" s="39"/>
       <c r="M2" s="19"/>
       <c r="N2" t="str">
         <f t="shared" ref="N2" si="3">IF(AND(H2="",I2=""),"",IF(H2="",0,2-H2)+IF(I2="",0,2-I2))</f>
@@ -1976,21 +2471,21 @@
       <c r="CN2" s="15"/>
     </row>
     <row r="3" spans="2:122" ht="15" customHeight="1">
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="36"/>
+      <c r="C3" s="42"/>
       <c r="E3" s="4" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F3" s="19"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="40"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="19"/>
-      <c r="L3" s="41"/>
+      <c r="L3" s="39"/>
       <c r="M3" s="19"/>
       <c r="N3" t="str">
         <f t="shared" ref="N3:N66" si="38">IF(AND(H3="",I3=""),"",IF(H3="",0,2-H3)+IF(I3="",0,2-I3))</f>
@@ -2299,12 +2794,12 @@
       <c r="F4" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="G4" s="38"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="40"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="19"/>
-      <c r="L4" s="41"/>
+      <c r="L4" s="39"/>
       <c r="M4" s="19"/>
       <c r="N4" t="str">
         <f t="shared" si="38"/>
@@ -2612,18 +3107,18 @@
       <c r="F5" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="G5" s="38">
+      <c r="G5" s="36">
         <v>9.1</v>
       </c>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="40">
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="38">
         <v>1</v>
       </c>
       <c r="K5" s="19">
         <v>1</v>
       </c>
-      <c r="L5" s="41"/>
+      <c r="L5" s="39"/>
       <c r="M5" s="19"/>
       <c r="N5" t="str">
         <f t="shared" si="38"/>
@@ -2943,24 +3438,24 @@
       <c r="F6" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="G6" s="38">
+      <c r="G6" s="36">
         <v>9.1999999999999993</v>
       </c>
-      <c r="H6" s="39" t="str">
+      <c r="H6" s="37" t="str">
         <f>IF(H5="","",H5)</f>
         <v/>
       </c>
-      <c r="I6" s="39" t="str">
+      <c r="I6" s="37" t="str">
         <f>IF(I5="","",I5)</f>
         <v/>
       </c>
-      <c r="J6" s="40">
+      <c r="J6" s="38">
         <v>1</v>
       </c>
       <c r="K6" s="19">
         <v>1</v>
       </c>
-      <c r="L6" s="41"/>
+      <c r="L6" s="39"/>
       <c r="M6" s="19">
         <v>1</v>
       </c>
@@ -3282,24 +3777,24 @@
       <c r="F7" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="G7" s="38">
+      <c r="G7" s="36">
         <v>9.3000000000000007</v>
       </c>
-      <c r="H7" s="39" t="str">
+      <c r="H7" s="37" t="str">
         <f>IF(H6="","",H6)</f>
         <v/>
       </c>
-      <c r="I7" s="39" t="str">
+      <c r="I7" s="37" t="str">
         <f>IF(I6="","",I6)</f>
         <v/>
       </c>
-      <c r="J7" s="40">
+      <c r="J7" s="38">
         <v>1</v>
       </c>
       <c r="K7" s="19">
         <v>1</v>
       </c>
-      <c r="L7" s="41"/>
+      <c r="L7" s="39"/>
       <c r="M7" s="19">
         <v>1</v>
       </c>
@@ -3467,7 +3962,9 @@
       <c r="BD7" s="5">
         <v>0</v>
       </c>
-      <c r="BE7" s="5"/>
+      <c r="BE7" s="5">
+        <v>0</v>
+      </c>
       <c r="BF7" s="5">
         <v>0</v>
       </c>
@@ -3614,12 +4111,12 @@
         <v/>
       </c>
       <c r="F8" s="19"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="40"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="38"/>
       <c r="K8" s="19"/>
-      <c r="L8" s="41"/>
+      <c r="L8" s="39"/>
       <c r="M8" s="19"/>
       <c r="N8" t="str">
         <f t="shared" si="38"/>
@@ -3942,20 +4439,20 @@
       <c r="F9" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="38">
+      <c r="G9" s="36">
         <v>10</v>
       </c>
-      <c r="H9" s="39">
+      <c r="H9" s="37">
         <v>0.89400000000000002</v>
       </c>
-      <c r="I9" s="39"/>
-      <c r="J9" s="40">
+      <c r="I9" s="37"/>
+      <c r="J9" s="38">
         <v>3</v>
       </c>
       <c r="K9" s="19">
         <v>1</v>
       </c>
-      <c r="L9" s="41"/>
+      <c r="L9" s="39"/>
       <c r="M9" s="19"/>
       <c r="N9">
         <f t="shared" si="38"/>
@@ -4291,22 +4788,22 @@
       <c r="F10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="38">
+      <c r="G10" s="36">
         <v>11</v>
       </c>
-      <c r="H10" s="39">
+      <c r="H10" s="37">
         <v>0.1</v>
       </c>
-      <c r="I10" s="39">
+      <c r="I10" s="37">
         <v>0.246</v>
       </c>
-      <c r="J10" s="40">
+      <c r="J10" s="38">
         <v>3</v>
       </c>
       <c r="K10" s="19">
         <v>1</v>
       </c>
-      <c r="L10" s="41"/>
+      <c r="L10" s="39"/>
       <c r="M10" s="19"/>
       <c r="N10">
         <f t="shared" si="38"/>
@@ -4642,22 +5139,22 @@
       <c r="F11" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="38">
-        <v>0</v>
-      </c>
-      <c r="H11" s="39">
+      <c r="G11" s="36">
+        <v>0</v>
+      </c>
+      <c r="H11" s="37">
         <v>0.47</v>
       </c>
-      <c r="I11" s="39">
+      <c r="I11" s="37">
         <v>0.5</v>
       </c>
-      <c r="J11" s="40">
+      <c r="J11" s="38">
         <v>1</v>
       </c>
       <c r="K11" s="19">
         <v>1</v>
       </c>
-      <c r="L11" s="41"/>
+      <c r="L11" s="39"/>
       <c r="M11" s="19"/>
       <c r="N11">
         <f t="shared" si="38"/>
@@ -4993,16 +5490,16 @@
       <c r="F12" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="G12" s="38">
+      <c r="G12" s="36">
         <v>210</v>
       </c>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="40"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="38"/>
       <c r="K12" s="19">
         <v>1</v>
       </c>
-      <c r="L12" s="41"/>
+      <c r="L12" s="39"/>
       <c r="M12" s="19"/>
       <c r="N12" t="str">
         <f t="shared" si="38"/>
@@ -5312,16 +5809,16 @@
       <c r="F13" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="G13" s="38">
+      <c r="G13" s="36">
         <v>200</v>
       </c>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="40"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="38"/>
       <c r="K13" s="19">
         <v>1</v>
       </c>
-      <c r="L13" s="41"/>
+      <c r="L13" s="39"/>
       <c r="M13" s="19"/>
       <c r="N13" t="str">
         <f t="shared" si="38"/>
@@ -5672,16 +6169,16 @@
       <c r="F14" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="G14" s="38">
+      <c r="G14" s="36">
         <v>200</v>
       </c>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="40"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="38"/>
       <c r="K14" s="19">
         <v>1</v>
       </c>
-      <c r="L14" s="41"/>
+      <c r="L14" s="39"/>
       <c r="M14" s="19"/>
       <c r="N14" t="str">
         <f t="shared" si="38"/>
@@ -6042,12 +6539,12 @@
         <v/>
       </c>
       <c r="F15" s="19"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="40"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="38"/>
       <c r="K15" s="19"/>
-      <c r="L15" s="41"/>
+      <c r="L15" s="39"/>
       <c r="M15" s="19"/>
       <c r="N15" t="str">
         <f t="shared" si="38"/>
@@ -6416,12 +6913,12 @@
         <v/>
       </c>
       <c r="F16" s="19"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="40"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="38"/>
       <c r="K16" s="19"/>
-      <c r="L16" s="41"/>
+      <c r="L16" s="39"/>
       <c r="M16" s="19"/>
       <c r="N16" t="str">
         <f t="shared" si="38"/>
@@ -6764,12 +7261,12 @@
         <v/>
       </c>
       <c r="F17" s="19"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="40"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="38"/>
       <c r="K17" s="19"/>
-      <c r="L17" s="41"/>
+      <c r="L17" s="39"/>
       <c r="M17" s="19"/>
       <c r="N17" t="str">
         <f t="shared" si="38"/>
@@ -7130,12 +7627,12 @@
         <v/>
       </c>
       <c r="F18" s="19"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="40"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="38"/>
       <c r="K18" s="19"/>
-      <c r="L18" s="41"/>
+      <c r="L18" s="39"/>
       <c r="M18" s="19"/>
       <c r="N18" t="str">
         <f t="shared" si="38"/>
@@ -7499,12 +7996,12 @@
       <c r="F19" s="19" t="s">
         <v>209</v>
       </c>
-      <c r="G19" s="38"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="40"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="38"/>
       <c r="K19" s="19"/>
-      <c r="L19" s="41"/>
+      <c r="L19" s="39"/>
       <c r="M19" s="19"/>
       <c r="N19" t="str">
         <f t="shared" si="38"/>
@@ -7865,22 +8362,22 @@
       <c r="F20" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="G20" s="38">
+      <c r="G20" s="36">
         <v>12</v>
       </c>
-      <c r="H20" s="39">
+      <c r="H20" s="37">
         <v>0.09</v>
       </c>
-      <c r="I20" s="39">
+      <c r="I20" s="37">
         <v>0.08</v>
       </c>
-      <c r="J20" s="40">
+      <c r="J20" s="38">
         <v>6</v>
       </c>
       <c r="K20" s="19">
         <v>2</v>
       </c>
-      <c r="L20" s="41"/>
+      <c r="L20" s="39"/>
       <c r="M20" s="19"/>
       <c r="N20">
         <f t="shared" si="38"/>
@@ -8243,22 +8740,22 @@
       <c r="F21" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="G21" s="38">
+      <c r="G21" s="36">
         <v>12</v>
       </c>
-      <c r="H21" s="39">
-        <v>0</v>
-      </c>
-      <c r="I21" s="39">
+      <c r="H21" s="37">
+        <v>0</v>
+      </c>
+      <c r="I21" s="37">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="J21" s="40">
+      <c r="J21" s="38">
         <v>6</v>
       </c>
       <c r="K21" s="19">
         <v>2</v>
       </c>
-      <c r="L21" s="41"/>
+      <c r="L21" s="39"/>
       <c r="M21" s="19"/>
       <c r="N21">
         <f t="shared" si="38"/>
@@ -8619,12 +9116,12 @@
         <v/>
       </c>
       <c r="F22" s="19"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="40"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="38"/>
       <c r="K22" s="19"/>
-      <c r="L22" s="41"/>
+      <c r="L22" s="39"/>
       <c r="M22" s="19"/>
       <c r="N22" s="30" t="str">
         <f t="shared" si="38"/>
@@ -8980,20 +9477,20 @@
       <c r="F23" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="G23" s="38">
+      <c r="G23" s="36">
         <v>101</v>
       </c>
-      <c r="H23" s="39">
+      <c r="H23" s="37">
         <v>1</v>
       </c>
-      <c r="I23" s="39">
+      <c r="I23" s="37">
         <v>1</v>
       </c>
-      <c r="J23" s="40"/>
+      <c r="J23" s="38"/>
       <c r="K23" s="19">
         <v>2</v>
       </c>
-      <c r="L23" s="41"/>
+      <c r="L23" s="39"/>
       <c r="M23" s="19"/>
       <c r="N23">
         <f t="shared" si="38"/>
@@ -9356,16 +9853,16 @@
       <c r="F24" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="G24" s="38">
+      <c r="G24" s="36">
         <v>210</v>
       </c>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="40"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="38"/>
       <c r="K24" s="19">
         <v>2</v>
       </c>
-      <c r="L24" s="41"/>
+      <c r="L24" s="39"/>
       <c r="M24" s="19"/>
       <c r="N24" t="str">
         <f t="shared" si="38"/>
@@ -9714,12 +10211,12 @@
         <v/>
       </c>
       <c r="F25" s="19"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="40"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="38"/>
       <c r="K25" s="19"/>
-      <c r="L25" s="42"/>
+      <c r="L25" s="40"/>
       <c r="M25" s="19"/>
       <c r="N25" t="str">
         <f t="shared" ref="N25" si="122">IF(AND(H25="",I25=""),"",IF(H25="",0,2-H25)+IF(I25="",0,2-I25))</f>
@@ -10066,12 +10563,12 @@
         <v/>
       </c>
       <c r="F26" s="19"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="40"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="38"/>
       <c r="K26" s="19"/>
-      <c r="L26" s="41"/>
+      <c r="L26" s="39"/>
       <c r="M26" s="19"/>
       <c r="N26" t="str">
         <f t="shared" si="38"/>
@@ -10410,12 +10907,12 @@
         <v/>
       </c>
       <c r="F27" s="19"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="39"/>
-      <c r="J27" s="40"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="38"/>
       <c r="K27" s="19"/>
-      <c r="L27" s="41"/>
+      <c r="L27" s="39"/>
       <c r="M27" s="19"/>
       <c r="N27" t="str">
         <f t="shared" si="38"/>
@@ -10765,12 +11262,12 @@
         <v/>
       </c>
       <c r="F28" s="19"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="40"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="38"/>
       <c r="K28" s="19"/>
-      <c r="L28" s="41"/>
+      <c r="L28" s="39"/>
       <c r="M28" s="19"/>
       <c r="N28" t="str">
         <f t="shared" si="38"/>
@@ -11121,12 +11618,12 @@
       <c r="F29" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="G29" s="38"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="40"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="38"/>
       <c r="K29" s="19"/>
-      <c r="L29" s="41"/>
+      <c r="L29" s="39"/>
       <c r="M29" s="19"/>
       <c r="N29" t="str">
         <f t="shared" si="38"/>
@@ -11477,12 +11974,12 @@
         <v/>
       </c>
       <c r="F30" s="19"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="40"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="38"/>
       <c r="K30" s="19"/>
-      <c r="L30" s="41"/>
+      <c r="L30" s="39"/>
       <c r="M30" s="19"/>
       <c r="N30" t="str">
         <f t="shared" si="38"/>
@@ -11774,12 +12271,12 @@
         <v/>
       </c>
       <c r="F31" s="19"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="39"/>
-      <c r="J31" s="40"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="38"/>
       <c r="K31" s="19"/>
-      <c r="L31" s="41"/>
+      <c r="L31" s="39"/>
       <c r="M31" s="19"/>
       <c r="N31" t="str">
         <f t="shared" si="38"/>
@@ -12022,20 +12519,20 @@
       <c r="F32" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="G32" s="38">
+      <c r="G32" s="36">
         <v>6.1</v>
       </c>
-      <c r="H32" s="39">
+      <c r="H32" s="37">
         <v>0.5</v>
       </c>
-      <c r="I32" s="39"/>
-      <c r="J32" s="40">
+      <c r="I32" s="37"/>
+      <c r="J32" s="38">
         <v>1</v>
       </c>
       <c r="K32" s="19">
         <v>3</v>
       </c>
-      <c r="L32" s="41"/>
+      <c r="L32" s="39"/>
       <c r="M32" s="19"/>
       <c r="N32">
         <f t="shared" si="38"/>
@@ -12255,24 +12752,24 @@
       <c r="F33" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="G33" s="38">
+      <c r="G33" s="36">
         <v>6.2</v>
       </c>
-      <c r="H33" s="39">
+      <c r="H33" s="37">
         <f>IF(H32="","",H32)</f>
         <v>0.5</v>
       </c>
-      <c r="I33" s="39" t="str">
+      <c r="I33" s="37" t="str">
         <f>IF(I32="","",I32)</f>
         <v/>
       </c>
-      <c r="J33" s="40">
+      <c r="J33" s="38">
         <v>1</v>
       </c>
       <c r="K33" s="19">
         <v>3</v>
       </c>
-      <c r="L33" s="42"/>
+      <c r="L33" s="40"/>
       <c r="M33" s="19">
         <v>1</v>
       </c>
@@ -12490,21 +12987,21 @@
       </c>
     </row>
     <row r="34" spans="2:93">
-      <c r="B34" s="36" t="s">
+      <c r="B34" s="42" t="s">
         <v>88</v>
       </c>
-      <c r="C34" s="36"/>
+      <c r="C34" s="42"/>
       <c r="E34" s="4" t="str">
         <f t="shared" ref="E34:E65" si="159">IF(P34="","",IF(AND(G34&gt;=200,G34&lt;300),100%,MIN(L34,AY34)))</f>
         <v/>
       </c>
       <c r="F34" s="19"/>
-      <c r="G34" s="38"/>
-      <c r="H34" s="39"/>
-      <c r="I34" s="39"/>
-      <c r="J34" s="40"/>
+      <c r="G34" s="36"/>
+      <c r="H34" s="37"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="38"/>
       <c r="K34" s="19"/>
-      <c r="L34" s="42"/>
+      <c r="L34" s="40"/>
       <c r="M34" s="19"/>
       <c r="N34" t="str">
         <f t="shared" si="38"/>
@@ -12728,18 +13225,18 @@
       <c r="F35" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="G35" s="38">
+      <c r="G35" s="36">
         <v>3.4</v>
       </c>
-      <c r="H35" s="39"/>
-      <c r="I35" s="39"/>
-      <c r="J35" s="40">
+      <c r="H35" s="37"/>
+      <c r="I35" s="37"/>
+      <c r="J35" s="38">
         <v>1</v>
       </c>
       <c r="K35" s="19">
         <v>3</v>
       </c>
-      <c r="L35" s="42">
+      <c r="L35" s="40">
         <v>8.9045429072610475E-5</v>
       </c>
       <c r="M35" s="19"/>
@@ -12971,24 +13468,24 @@
       <c r="F36" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G36" s="38">
+      <c r="G36" s="36">
         <v>3.1</v>
       </c>
-      <c r="H36" s="39" t="str">
+      <c r="H36" s="37" t="str">
         <f t="shared" ref="H36:I36" si="192">IF(H35="","",H35)</f>
         <v/>
       </c>
-      <c r="I36" s="39" t="str">
+      <c r="I36" s="37" t="str">
         <f t="shared" si="192"/>
         <v/>
       </c>
-      <c r="J36" s="40">
+      <c r="J36" s="38">
         <v>1</v>
       </c>
       <c r="K36" s="19">
         <v>3</v>
       </c>
-      <c r="L36" s="42">
+      <c r="L36" s="40">
         <v>1.6900918752645039E-5</v>
       </c>
       <c r="M36" s="19">
@@ -13216,24 +13713,24 @@
       <c r="F37" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="G37" s="38">
+      <c r="G37" s="36">
         <v>3.2</v>
       </c>
-      <c r="H37" s="39" t="str">
+      <c r="H37" s="37" t="str">
         <f t="shared" ref="H37:I37" si="203">IF(H36="","",H36)</f>
         <v/>
       </c>
-      <c r="I37" s="39" t="str">
+      <c r="I37" s="37" t="str">
         <f t="shared" si="203"/>
         <v/>
       </c>
-      <c r="J37" s="40">
+      <c r="J37" s="38">
         <v>1</v>
       </c>
       <c r="K37" s="19">
         <v>3</v>
       </c>
-      <c r="L37" s="42">
+      <c r="L37" s="40">
         <v>4.8582729342987897E-5</v>
       </c>
       <c r="M37" s="19">
@@ -13468,24 +13965,24 @@
       <c r="F38" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="G38" s="38">
+      <c r="G38" s="36">
         <v>3.3</v>
       </c>
-      <c r="H38" s="39" t="str">
+      <c r="H38" s="37" t="str">
         <f t="shared" ref="H38:I38" si="205">IF(H37="","",H37)</f>
         <v/>
       </c>
-      <c r="I38" s="39" t="str">
+      <c r="I38" s="37" t="str">
         <f t="shared" si="205"/>
         <v/>
       </c>
-      <c r="J38" s="40">
+      <c r="J38" s="38">
         <v>1</v>
       </c>
       <c r="K38" s="19">
         <v>3</v>
       </c>
-      <c r="L38" s="42">
+      <c r="L38" s="40">
         <v>2.9735893041913058E-4</v>
       </c>
       <c r="M38" s="19">
@@ -13720,12 +14217,12 @@
         <v/>
       </c>
       <c r="F39" s="19"/>
-      <c r="G39" s="38"/>
-      <c r="H39" s="39"/>
-      <c r="I39" s="39"/>
-      <c r="J39" s="40"/>
+      <c r="G39" s="36"/>
+      <c r="H39" s="37"/>
+      <c r="I39" s="37"/>
+      <c r="J39" s="38"/>
       <c r="K39" s="19"/>
-      <c r="L39" s="41"/>
+      <c r="L39" s="39"/>
       <c r="M39" s="19"/>
       <c r="N39" t="str">
         <f t="shared" si="38"/>
@@ -13940,18 +14437,18 @@
       <c r="F40" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="G40" s="38">
+      <c r="G40" s="36">
         <v>4.0999999999999996</v>
       </c>
-      <c r="H40" s="39"/>
-      <c r="I40" s="39"/>
-      <c r="J40" s="40">
+      <c r="H40" s="37"/>
+      <c r="I40" s="37"/>
+      <c r="J40" s="38">
         <v>0</v>
       </c>
       <c r="K40" s="19">
         <v>3</v>
       </c>
-      <c r="L40" s="41"/>
+      <c r="L40" s="39"/>
       <c r="M40" s="19"/>
       <c r="N40" t="str">
         <f t="shared" si="38"/>
@@ -14170,24 +14667,24 @@
       <c r="F41" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="G41" s="38">
+      <c r="G41" s="36">
         <v>4.2</v>
       </c>
-      <c r="H41" s="39" t="str">
+      <c r="H41" s="37" t="str">
         <f>IF(H40="","",H40)</f>
         <v/>
       </c>
-      <c r="I41" s="39" t="str">
+      <c r="I41" s="37" t="str">
         <f>IF(I40="","",I40)</f>
         <v/>
       </c>
-      <c r="J41" s="40">
+      <c r="J41" s="38">
         <v>0</v>
       </c>
       <c r="K41" s="19">
         <v>3</v>
       </c>
-      <c r="L41" s="41"/>
+      <c r="L41" s="39"/>
       <c r="M41" s="19">
         <v>1</v>
       </c>
@@ -14398,24 +14895,24 @@
       <c r="F42" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="G42" s="38">
+      <c r="G42" s="36">
         <v>4.3</v>
       </c>
-      <c r="H42" s="39" t="str">
+      <c r="H42" s="37" t="str">
         <f>IF(H41="","",H41)</f>
         <v/>
       </c>
-      <c r="I42" s="39" t="str">
+      <c r="I42" s="37" t="str">
         <f>IF(I41="","",I41)</f>
         <v/>
       </c>
-      <c r="J42" s="40">
+      <c r="J42" s="38">
         <v>0</v>
       </c>
       <c r="K42" s="19">
         <v>3</v>
       </c>
-      <c r="L42" s="41"/>
+      <c r="L42" s="39"/>
       <c r="M42" s="19">
         <v>1</v>
       </c>
@@ -14585,12 +15082,12 @@
         <v/>
       </c>
       <c r="F43" s="19"/>
-      <c r="G43" s="38"/>
-      <c r="H43" s="39"/>
-      <c r="I43" s="39"/>
-      <c r="J43" s="40"/>
+      <c r="G43" s="36"/>
+      <c r="H43" s="37"/>
+      <c r="I43" s="37"/>
+      <c r="J43" s="38"/>
       <c r="K43" s="19"/>
-      <c r="L43" s="41"/>
+      <c r="L43" s="39"/>
       <c r="M43" s="19"/>
       <c r="N43" t="str">
         <f t="shared" si="38"/>
@@ -14766,16 +15263,16 @@
       <c r="F44" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="G44" s="38">
+      <c r="G44" s="36">
         <v>210</v>
       </c>
-      <c r="H44" s="39"/>
-      <c r="I44" s="39"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="37"/>
+      <c r="I44" s="37"/>
+      <c r="J44" s="38"/>
       <c r="K44" s="19">
         <v>3</v>
       </c>
-      <c r="L44" s="41"/>
+      <c r="L44" s="39"/>
       <c r="M44" s="19"/>
       <c r="N44" t="str">
         <f t="shared" si="38"/>
@@ -14958,16 +15455,16 @@
       <c r="F45" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="G45" s="38">
+      <c r="G45" s="36">
         <v>201</v>
       </c>
-      <c r="H45" s="39"/>
-      <c r="I45" s="39"/>
-      <c r="J45" s="40"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="37"/>
+      <c r="J45" s="38"/>
       <c r="K45" s="19">
         <v>3</v>
       </c>
-      <c r="L45" s="41"/>
+      <c r="L45" s="39"/>
       <c r="M45" s="19"/>
       <c r="N45" t="str">
         <f t="shared" si="38"/>
@@ -15150,16 +15647,16 @@
       <c r="F46" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="G46" s="38">
+      <c r="G46" s="36">
         <v>202</v>
       </c>
-      <c r="H46" s="39"/>
-      <c r="I46" s="39"/>
-      <c r="J46" s="40"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="38"/>
       <c r="K46" s="19">
         <v>3</v>
       </c>
-      <c r="L46" s="41"/>
+      <c r="L46" s="39"/>
       <c r="M46" s="19"/>
       <c r="N46" t="str">
         <f t="shared" si="38"/>
@@ -15335,16 +15832,16 @@
       <c r="F47" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="G47" s="38">
+      <c r="G47" s="36">
         <v>203</v>
       </c>
-      <c r="H47" s="39"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="40"/>
+      <c r="H47" s="37"/>
+      <c r="I47" s="37"/>
+      <c r="J47" s="38"/>
       <c r="K47" s="19">
         <v>3</v>
       </c>
-      <c r="L47" s="41"/>
+      <c r="L47" s="39"/>
       <c r="M47" s="19"/>
       <c r="N47" t="str">
         <f t="shared" si="38"/>
@@ -15520,16 +16017,16 @@
       <c r="F48" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="G48" s="38">
+      <c r="G48" s="36">
         <v>204</v>
       </c>
-      <c r="H48" s="39"/>
-      <c r="I48" s="39"/>
-      <c r="J48" s="40"/>
+      <c r="H48" s="37"/>
+      <c r="I48" s="37"/>
+      <c r="J48" s="38"/>
       <c r="K48" s="19">
         <v>3</v>
       </c>
-      <c r="L48" s="41"/>
+      <c r="L48" s="39"/>
       <c r="M48" s="19"/>
       <c r="N48" t="str">
         <f t="shared" si="38"/>
@@ -15713,16 +16210,16 @@
       <c r="F49" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="G49" s="38">
+      <c r="G49" s="36">
         <v>201</v>
       </c>
-      <c r="H49" s="39"/>
-      <c r="I49" s="39"/>
-      <c r="J49" s="40"/>
+      <c r="H49" s="37"/>
+      <c r="I49" s="37"/>
+      <c r="J49" s="38"/>
       <c r="K49" s="19">
         <v>3</v>
       </c>
-      <c r="L49" s="41"/>
+      <c r="L49" s="39"/>
       <c r="M49" s="19"/>
       <c r="N49" t="str">
         <f t="shared" si="38"/>
@@ -15885,16 +16382,16 @@
       <c r="F50" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="G50" s="38">
+      <c r="G50" s="36">
         <v>202</v>
       </c>
-      <c r="H50" s="39"/>
-      <c r="I50" s="39"/>
-      <c r="J50" s="40"/>
+      <c r="H50" s="37"/>
+      <c r="I50" s="37"/>
+      <c r="J50" s="38"/>
       <c r="K50" s="19">
         <v>3</v>
       </c>
-      <c r="L50" s="41"/>
+      <c r="L50" s="39"/>
       <c r="M50" s="19"/>
       <c r="N50" t="str">
         <f t="shared" si="38"/>
@@ -16056,10 +16553,10 @@
       </c>
     </row>
     <row r="51" spans="1:63">
-      <c r="B51" s="36" t="s">
+      <c r="B51" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="C51" s="36"/>
+      <c r="C51" s="42"/>
       <c r="E51" s="4">
         <f t="shared" si="159"/>
         <v>1</v>
@@ -16067,16 +16564,16 @@
       <c r="F51" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="G51" s="38">
+      <c r="G51" s="36">
         <v>203</v>
       </c>
-      <c r="H51" s="39"/>
-      <c r="I51" s="39"/>
-      <c r="J51" s="40"/>
+      <c r="H51" s="37"/>
+      <c r="I51" s="37"/>
+      <c r="J51" s="38"/>
       <c r="K51" s="19">
         <v>3</v>
       </c>
-      <c r="L51" s="41"/>
+      <c r="L51" s="39"/>
       <c r="M51" s="19"/>
       <c r="N51" t="str">
         <f t="shared" si="38"/>
@@ -16258,16 +16755,16 @@
       <c r="F52" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="G52" s="38">
+      <c r="G52" s="36">
         <v>204</v>
       </c>
-      <c r="H52" s="39"/>
-      <c r="I52" s="39"/>
-      <c r="J52" s="40"/>
+      <c r="H52" s="37"/>
+      <c r="I52" s="37"/>
+      <c r="J52" s="38"/>
       <c r="K52" s="19">
         <v>3</v>
       </c>
-      <c r="L52" s="41"/>
+      <c r="L52" s="39"/>
       <c r="M52" s="19"/>
       <c r="N52" t="str">
         <f t="shared" si="38"/>
@@ -16446,12 +16943,12 @@
         <v/>
       </c>
       <c r="F53" s="19"/>
-      <c r="G53" s="38"/>
-      <c r="H53" s="39"/>
-      <c r="I53" s="39"/>
-      <c r="J53" s="40"/>
+      <c r="G53" s="36"/>
+      <c r="H53" s="37"/>
+      <c r="I53" s="37"/>
+      <c r="J53" s="38"/>
       <c r="K53" s="19"/>
-      <c r="L53" s="41"/>
+      <c r="L53" s="39"/>
       <c r="M53" s="19"/>
       <c r="N53" t="str">
         <f t="shared" si="38"/>
@@ -16633,12 +17130,12 @@
         <v/>
       </c>
       <c r="F54" s="19"/>
-      <c r="G54" s="38"/>
-      <c r="H54" s="39"/>
-      <c r="I54" s="39"/>
-      <c r="J54" s="40"/>
+      <c r="G54" s="36"/>
+      <c r="H54" s="37"/>
+      <c r="I54" s="37"/>
+      <c r="J54" s="38"/>
       <c r="K54" s="19"/>
-      <c r="L54" s="41"/>
+      <c r="L54" s="39"/>
       <c r="M54" s="19"/>
       <c r="N54" t="str">
         <f t="shared" si="38"/>
@@ -16821,12 +17318,12 @@
         <v/>
       </c>
       <c r="F55" s="19"/>
-      <c r="G55" s="38"/>
-      <c r="H55" s="39"/>
-      <c r="I55" s="39"/>
-      <c r="J55" s="40"/>
+      <c r="G55" s="36"/>
+      <c r="H55" s="37"/>
+      <c r="I55" s="37"/>
+      <c r="J55" s="38"/>
       <c r="K55" s="19"/>
-      <c r="L55" s="41"/>
+      <c r="L55" s="39"/>
       <c r="M55" s="19"/>
       <c r="N55" t="str">
         <f t="shared" si="38"/>
@@ -17007,12 +17504,12 @@
         <v/>
       </c>
       <c r="F56" s="19"/>
-      <c r="G56" s="38"/>
-      <c r="H56" s="39"/>
-      <c r="I56" s="39"/>
-      <c r="J56" s="40"/>
+      <c r="G56" s="36"/>
+      <c r="H56" s="37"/>
+      <c r="I56" s="37"/>
+      <c r="J56" s="38"/>
       <c r="K56" s="19"/>
-      <c r="L56" s="41"/>
+      <c r="L56" s="39"/>
       <c r="M56" s="19"/>
       <c r="N56" t="str">
         <f t="shared" si="38"/>
@@ -17182,12 +17679,12 @@
       <c r="F57" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="G57" s="38"/>
-      <c r="H57" s="39"/>
-      <c r="I57" s="39"/>
-      <c r="J57" s="40"/>
+      <c r="G57" s="36"/>
+      <c r="H57" s="37"/>
+      <c r="I57" s="37"/>
+      <c r="J57" s="38"/>
       <c r="K57" s="19"/>
-      <c r="L57" s="41"/>
+      <c r="L57" s="39"/>
       <c r="M57" s="19"/>
       <c r="N57" t="str">
         <f t="shared" si="38"/>
@@ -17362,20 +17859,20 @@
       <c r="F58" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="G58" s="38">
-        <v>0</v>
-      </c>
-      <c r="H58" s="39">
+      <c r="G58" s="36">
+        <v>0</v>
+      </c>
+      <c r="H58" s="37">
         <v>0.2</v>
       </c>
-      <c r="I58" s="39"/>
-      <c r="J58" s="40">
+      <c r="I58" s="37"/>
+      <c r="J58" s="38">
         <v>1</v>
       </c>
       <c r="K58" s="19">
         <v>4</v>
       </c>
-      <c r="L58" s="41"/>
+      <c r="L58" s="39"/>
       <c r="M58" s="19"/>
       <c r="N58">
         <f t="shared" si="38"/>
@@ -17564,12 +18061,12 @@
         <v/>
       </c>
       <c r="F59" s="19"/>
-      <c r="G59" s="38"/>
-      <c r="H59" s="39"/>
-      <c r="I59" s="39"/>
-      <c r="J59" s="40"/>
+      <c r="G59" s="36"/>
+      <c r="H59" s="37"/>
+      <c r="I59" s="37"/>
+      <c r="J59" s="38"/>
       <c r="K59" s="19"/>
-      <c r="L59" s="41"/>
+      <c r="L59" s="39"/>
       <c r="M59" s="19"/>
       <c r="N59" t="str">
         <f t="shared" si="38"/>
@@ -17758,18 +18255,18 @@
       <c r="F60" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="G60" s="38">
+      <c r="G60" s="36">
         <v>7.4</v>
       </c>
-      <c r="H60" s="39"/>
-      <c r="I60" s="39"/>
-      <c r="J60" s="40">
+      <c r="H60" s="37"/>
+      <c r="I60" s="37"/>
+      <c r="J60" s="38">
         <v>1</v>
       </c>
       <c r="K60" s="19">
         <v>4</v>
       </c>
-      <c r="L60" s="43">
+      <c r="L60" s="41">
         <f ca="1">C56</f>
         <v>4.3555555555555556E-2</v>
       </c>
@@ -17950,24 +18447,24 @@
       <c r="F61" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="G61" s="38">
+      <c r="G61" s="36">
         <v>7.5</v>
       </c>
-      <c r="H61" s="39" t="str">
+      <c r="H61" s="37" t="str">
         <f>IF(H60="","",H60)</f>
         <v/>
       </c>
-      <c r="I61" s="39" t="str">
+      <c r="I61" s="37" t="str">
         <f>IF(I60="","",I60)</f>
         <v/>
       </c>
-      <c r="J61" s="40">
+      <c r="J61" s="38">
         <v>1</v>
       </c>
       <c r="K61" s="19">
         <v>4</v>
       </c>
-      <c r="L61" s="41"/>
+      <c r="L61" s="39"/>
       <c r="M61" s="19">
         <v>1</v>
       </c>
@@ -18158,24 +18655,24 @@
       <c r="F62" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="G62" s="38">
+      <c r="G62" s="36">
         <v>7.6</v>
       </c>
-      <c r="H62" s="39" t="str">
+      <c r="H62" s="37" t="str">
         <f>IF(H61="","",H61)</f>
         <v/>
       </c>
-      <c r="I62" s="39" t="str">
+      <c r="I62" s="37" t="str">
         <f>IF(I61="","",I61)</f>
         <v/>
       </c>
-      <c r="J62" s="40">
+      <c r="J62" s="38">
         <v>0</v>
       </c>
       <c r="K62" s="19">
         <v>4</v>
       </c>
-      <c r="L62" s="41"/>
+      <c r="L62" s="39"/>
       <c r="M62" s="19">
         <v>1</v>
       </c>
@@ -18366,12 +18863,12 @@
         <v/>
       </c>
       <c r="F63" s="19"/>
-      <c r="G63" s="38"/>
-      <c r="H63" s="39"/>
-      <c r="I63" s="39"/>
-      <c r="J63" s="40"/>
+      <c r="G63" s="36"/>
+      <c r="H63" s="37"/>
+      <c r="I63" s="37"/>
+      <c r="J63" s="38"/>
       <c r="K63" s="19"/>
-      <c r="L63" s="41"/>
+      <c r="L63" s="39"/>
       <c r="M63" s="19"/>
       <c r="N63" t="str">
         <f t="shared" si="38"/>
@@ -18560,18 +19057,18 @@
       <c r="F64" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="G64" s="38">
+      <c r="G64" s="36">
         <v>8.3000000000000007</v>
       </c>
-      <c r="H64" s="39"/>
-      <c r="I64" s="39"/>
-      <c r="J64" s="40">
+      <c r="H64" s="37"/>
+      <c r="I64" s="37"/>
+      <c r="J64" s="38">
         <v>1</v>
       </c>
       <c r="K64" s="19">
         <v>4</v>
       </c>
-      <c r="L64" s="41"/>
+      <c r="L64" s="39"/>
       <c r="M64" s="19"/>
       <c r="N64" t="str">
         <f t="shared" si="38"/>
@@ -18762,24 +19259,24 @@
       <c r="F65" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="G65" s="38">
+      <c r="G65" s="36">
         <v>8.4</v>
       </c>
-      <c r="H65" s="39" t="str">
+      <c r="H65" s="37" t="str">
         <f>IF(H64="","",H64)</f>
         <v/>
       </c>
-      <c r="I65" s="39" t="str">
+      <c r="I65" s="37" t="str">
         <f>IF(I64="","",I64)</f>
         <v/>
       </c>
-      <c r="J65" s="40">
+      <c r="J65" s="38">
         <v>1</v>
       </c>
       <c r="K65" s="19">
         <v>4</v>
       </c>
-      <c r="L65" s="41"/>
+      <c r="L65" s="39"/>
       <c r="M65" s="19">
         <v>1</v>
       </c>
@@ -18942,12 +19439,12 @@
         <v/>
       </c>
       <c r="F66" s="19"/>
-      <c r="G66" s="38"/>
-      <c r="H66" s="39"/>
-      <c r="I66" s="39"/>
-      <c r="J66" s="40"/>
+      <c r="G66" s="36"/>
+      <c r="H66" s="37"/>
+      <c r="I66" s="37"/>
+      <c r="J66" s="38"/>
       <c r="K66" s="19"/>
-      <c r="L66" s="41"/>
+      <c r="L66" s="39"/>
       <c r="M66" s="19"/>
       <c r="N66" t="str">
         <f t="shared" si="38"/>
@@ -19120,16 +19617,16 @@
       <c r="F67" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="G67" s="38">
+      <c r="G67" s="36">
         <v>210</v>
       </c>
-      <c r="H67" s="39"/>
-      <c r="I67" s="39"/>
-      <c r="J67" s="40"/>
+      <c r="H67" s="37"/>
+      <c r="I67" s="37"/>
+      <c r="J67" s="38"/>
       <c r="K67" s="19">
         <v>4</v>
       </c>
-      <c r="L67" s="41"/>
+      <c r="L67" s="39"/>
       <c r="M67" s="19"/>
       <c r="N67" t="str">
         <f t="shared" ref="N67:N120" si="244">IF(AND(H67="",I67=""),"",IF(H67="",0,2-H67)+IF(I67="",0,2-I67))</f>
@@ -19299,16 +19796,16 @@
       <c r="F68" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="G68" s="38">
+      <c r="G68" s="36">
         <v>200</v>
       </c>
-      <c r="H68" s="39"/>
-      <c r="I68" s="39"/>
-      <c r="J68" s="40"/>
+      <c r="H68" s="37"/>
+      <c r="I68" s="37"/>
+      <c r="J68" s="38"/>
       <c r="K68" s="19">
         <v>4</v>
       </c>
-      <c r="L68" s="41"/>
+      <c r="L68" s="39"/>
       <c r="M68" s="19"/>
       <c r="N68" t="str">
         <f t="shared" si="244"/>
@@ -19482,12 +19979,12 @@
         <v/>
       </c>
       <c r="F69" s="19"/>
-      <c r="G69" s="38"/>
-      <c r="H69" s="39"/>
-      <c r="I69" s="39"/>
-      <c r="J69" s="40"/>
+      <c r="G69" s="36"/>
+      <c r="H69" s="37"/>
+      <c r="I69" s="37"/>
+      <c r="J69" s="38"/>
       <c r="K69" s="19"/>
-      <c r="L69" s="41"/>
+      <c r="L69" s="39"/>
       <c r="M69" s="19"/>
       <c r="N69" t="str">
         <f t="shared" si="244"/>
@@ -19698,12 +20195,12 @@
         <v/>
       </c>
       <c r="F70" s="19"/>
-      <c r="G70" s="38"/>
-      <c r="H70" s="39"/>
-      <c r="I70" s="39"/>
-      <c r="J70" s="40"/>
+      <c r="G70" s="36"/>
+      <c r="H70" s="37"/>
+      <c r="I70" s="37"/>
+      <c r="J70" s="38"/>
       <c r="K70" s="19"/>
-      <c r="L70" s="41"/>
+      <c r="L70" s="39"/>
       <c r="M70" s="19"/>
       <c r="N70" t="str">
         <f t="shared" si="244"/>
@@ -19909,12 +20406,12 @@
       <c r="F71" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="G71" s="38"/>
-      <c r="H71" s="39"/>
-      <c r="I71" s="39"/>
-      <c r="J71" s="40"/>
+      <c r="G71" s="36"/>
+      <c r="H71" s="37"/>
+      <c r="I71" s="37"/>
+      <c r="J71" s="38"/>
       <c r="K71" s="19"/>
-      <c r="L71" s="41"/>
+      <c r="L71" s="39"/>
       <c r="M71" s="19"/>
       <c r="N71" t="str">
         <f t="shared" si="244"/>
@@ -20127,16 +20624,16 @@
       <c r="F72" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="G72" s="38">
+      <c r="G72" s="36">
         <v>210</v>
       </c>
-      <c r="H72" s="39"/>
-      <c r="I72" s="39"/>
-      <c r="J72" s="40"/>
+      <c r="H72" s="37"/>
+      <c r="I72" s="37"/>
+      <c r="J72" s="38"/>
       <c r="K72" s="19">
         <v>5</v>
       </c>
-      <c r="L72" s="41"/>
+      <c r="L72" s="39"/>
       <c r="M72" s="19"/>
       <c r="N72" t="str">
         <f t="shared" si="244"/>
@@ -20349,16 +20846,16 @@
       <c r="F73" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="G73" s="38">
+      <c r="G73" s="36">
         <v>200</v>
       </c>
-      <c r="H73" s="39"/>
-      <c r="I73" s="39"/>
-      <c r="J73" s="40"/>
+      <c r="H73" s="37"/>
+      <c r="I73" s="37"/>
+      <c r="J73" s="38"/>
       <c r="K73" s="19">
         <v>5</v>
       </c>
-      <c r="L73" s="41"/>
+      <c r="L73" s="39"/>
       <c r="M73" s="19"/>
       <c r="N73" t="str">
         <f t="shared" si="244"/>
@@ -20571,16 +21068,16 @@
       <c r="F74" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="G74" s="38">
+      <c r="G74" s="36">
         <v>200</v>
       </c>
-      <c r="H74" s="39"/>
-      <c r="I74" s="39"/>
-      <c r="J74" s="40"/>
+      <c r="H74" s="37"/>
+      <c r="I74" s="37"/>
+      <c r="J74" s="38"/>
       <c r="K74" s="19">
         <v>5</v>
       </c>
-      <c r="L74" s="41"/>
+      <c r="L74" s="39"/>
       <c r="M74" s="19"/>
       <c r="N74" t="str">
         <f t="shared" si="244"/>
@@ -20750,12 +21247,12 @@
       <c r="F75" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="G75" s="38"/>
-      <c r="H75" s="39"/>
-      <c r="I75" s="39"/>
-      <c r="J75" s="40"/>
+      <c r="G75" s="36"/>
+      <c r="H75" s="37"/>
+      <c r="I75" s="37"/>
+      <c r="J75" s="38"/>
       <c r="K75" s="19"/>
-      <c r="L75" s="41"/>
+      <c r="L75" s="39"/>
       <c r="M75" s="19"/>
       <c r="N75" t="str">
         <f t="shared" si="244"/>
@@ -20921,12 +21418,12 @@
       <c r="F76" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="G76" s="38"/>
-      <c r="H76" s="39"/>
-      <c r="I76" s="39"/>
-      <c r="J76" s="40"/>
+      <c r="G76" s="36"/>
+      <c r="H76" s="37"/>
+      <c r="I76" s="37"/>
+      <c r="J76" s="38"/>
       <c r="K76" s="19"/>
-      <c r="L76" s="41"/>
+      <c r="L76" s="39"/>
       <c r="M76" s="19"/>
       <c r="N76" t="str">
         <f t="shared" si="244"/>
@@ -21133,12 +21630,12 @@
       <c r="F77" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="G77" s="38"/>
-      <c r="H77" s="39"/>
-      <c r="I77" s="39"/>
-      <c r="J77" s="40"/>
+      <c r="G77" s="36"/>
+      <c r="H77" s="37"/>
+      <c r="I77" s="37"/>
+      <c r="J77" s="38"/>
       <c r="K77" s="19"/>
-      <c r="L77" s="41"/>
+      <c r="L77" s="39"/>
       <c r="M77" s="19"/>
       <c r="N77" t="str">
         <f t="shared" si="244"/>
@@ -21344,12 +21841,12 @@
       <c r="F78" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="G78" s="38"/>
-      <c r="H78" s="39"/>
-      <c r="I78" s="39"/>
-      <c r="J78" s="40"/>
+      <c r="G78" s="36"/>
+      <c r="H78" s="37"/>
+      <c r="I78" s="37"/>
+      <c r="J78" s="38"/>
       <c r="K78" s="19"/>
-      <c r="L78" s="41"/>
+      <c r="L78" s="39"/>
       <c r="M78" s="19"/>
       <c r="N78" t="str">
         <f t="shared" si="244"/>
@@ -21555,12 +22052,12 @@
       <c r="F79" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="G79" s="38"/>
-      <c r="H79" s="39"/>
-      <c r="I79" s="39"/>
-      <c r="J79" s="40"/>
+      <c r="G79" s="36"/>
+      <c r="H79" s="37"/>
+      <c r="I79" s="37"/>
+      <c r="J79" s="38"/>
       <c r="K79" s="19"/>
-      <c r="L79" s="41"/>
+      <c r="L79" s="39"/>
       <c r="M79" s="19"/>
       <c r="N79" t="str">
         <f t="shared" si="244"/>
@@ -21764,12 +22261,12 @@
         <v/>
       </c>
       <c r="F80" s="19"/>
-      <c r="G80" s="38"/>
-      <c r="H80" s="39"/>
-      <c r="I80" s="39"/>
-      <c r="J80" s="40"/>
+      <c r="G80" s="36"/>
+      <c r="H80" s="37"/>
+      <c r="I80" s="37"/>
+      <c r="J80" s="38"/>
       <c r="K80" s="19"/>
-      <c r="L80" s="41"/>
+      <c r="L80" s="39"/>
       <c r="M80" s="19"/>
       <c r="N80" t="str">
         <f t="shared" si="244"/>
@@ -21973,12 +22470,12 @@
         <v/>
       </c>
       <c r="F81" s="19"/>
-      <c r="G81" s="38"/>
-      <c r="H81" s="39"/>
-      <c r="I81" s="39"/>
-      <c r="J81" s="40"/>
+      <c r="G81" s="36"/>
+      <c r="H81" s="37"/>
+      <c r="I81" s="37"/>
+      <c r="J81" s="38"/>
       <c r="K81" s="19"/>
-      <c r="L81" s="41"/>
+      <c r="L81" s="39"/>
       <c r="M81" s="19"/>
       <c r="N81" t="str">
         <f t="shared" si="244"/>
@@ -22139,12 +22636,12 @@
         <v/>
       </c>
       <c r="F82" s="19"/>
-      <c r="G82" s="38"/>
-      <c r="H82" s="39"/>
-      <c r="I82" s="39"/>
-      <c r="J82" s="40"/>
+      <c r="G82" s="36"/>
+      <c r="H82" s="37"/>
+      <c r="I82" s="37"/>
+      <c r="J82" s="38"/>
       <c r="K82" s="19"/>
-      <c r="L82" s="41"/>
+      <c r="L82" s="39"/>
       <c r="M82" s="19"/>
       <c r="N82" t="str">
         <f t="shared" si="244"/>
@@ -22305,12 +22802,12 @@
         <v/>
       </c>
       <c r="F83" s="19"/>
-      <c r="G83" s="38"/>
-      <c r="H83" s="39"/>
-      <c r="I83" s="39"/>
-      <c r="J83" s="40"/>
+      <c r="G83" s="36"/>
+      <c r="H83" s="37"/>
+      <c r="I83" s="37"/>
+      <c r="J83" s="38"/>
       <c r="K83" s="19"/>
-      <c r="L83" s="41"/>
+      <c r="L83" s="39"/>
       <c r="M83" s="19"/>
       <c r="N83" t="str">
         <f t="shared" si="244"/>
@@ -22471,12 +22968,12 @@
         <v/>
       </c>
       <c r="F84" s="19"/>
-      <c r="G84" s="38"/>
-      <c r="H84" s="39"/>
-      <c r="I84" s="39"/>
-      <c r="J84" s="40"/>
+      <c r="G84" s="36"/>
+      <c r="H84" s="37"/>
+      <c r="I84" s="37"/>
+      <c r="J84" s="38"/>
       <c r="K84" s="19"/>
-      <c r="L84" s="41"/>
+      <c r="L84" s="39"/>
       <c r="M84" s="19"/>
       <c r="N84" t="str">
         <f t="shared" si="244"/>
@@ -22637,12 +23134,12 @@
         <v/>
       </c>
       <c r="F85" s="19"/>
-      <c r="G85" s="38"/>
-      <c r="H85" s="39"/>
-      <c r="I85" s="39"/>
-      <c r="J85" s="40"/>
+      <c r="G85" s="36"/>
+      <c r="H85" s="37"/>
+      <c r="I85" s="37"/>
+      <c r="J85" s="38"/>
       <c r="K85" s="19"/>
-      <c r="L85" s="41"/>
+      <c r="L85" s="39"/>
       <c r="M85" s="19"/>
       <c r="N85" t="str">
         <f t="shared" si="244"/>
@@ -22803,12 +23300,12 @@
         <v/>
       </c>
       <c r="F86" s="19"/>
-      <c r="G86" s="38"/>
-      <c r="H86" s="39"/>
-      <c r="I86" s="39"/>
-      <c r="J86" s="40"/>
+      <c r="G86" s="36"/>
+      <c r="H86" s="37"/>
+      <c r="I86" s="37"/>
+      <c r="J86" s="38"/>
       <c r="K86" s="19"/>
-      <c r="L86" s="41"/>
+      <c r="L86" s="39"/>
       <c r="M86" s="19"/>
       <c r="N86" t="str">
         <f t="shared" si="244"/>
@@ -22969,12 +23466,12 @@
         <v/>
       </c>
       <c r="F87" s="19"/>
-      <c r="G87" s="38"/>
-      <c r="H87" s="39"/>
-      <c r="I87" s="39"/>
-      <c r="J87" s="40"/>
+      <c r="G87" s="36"/>
+      <c r="H87" s="37"/>
+      <c r="I87" s="37"/>
+      <c r="J87" s="38"/>
       <c r="K87" s="19"/>
-      <c r="L87" s="41"/>
+      <c r="L87" s="39"/>
       <c r="M87" s="19"/>
       <c r="N87" t="str">
         <f t="shared" si="244"/>
@@ -23135,12 +23632,12 @@
         <v/>
       </c>
       <c r="F88" s="19"/>
-      <c r="G88" s="38"/>
-      <c r="H88" s="39"/>
-      <c r="I88" s="39"/>
-      <c r="J88" s="40"/>
+      <c r="G88" s="36"/>
+      <c r="H88" s="37"/>
+      <c r="I88" s="37"/>
+      <c r="J88" s="38"/>
       <c r="K88" s="19"/>
-      <c r="L88" s="41"/>
+      <c r="L88" s="39"/>
       <c r="M88" s="19"/>
       <c r="N88" t="str">
         <f t="shared" si="244"/>
@@ -23301,12 +23798,12 @@
         <v/>
       </c>
       <c r="F89" s="19"/>
-      <c r="G89" s="38"/>
-      <c r="H89" s="39"/>
-      <c r="I89" s="39"/>
-      <c r="J89" s="40"/>
+      <c r="G89" s="36"/>
+      <c r="H89" s="37"/>
+      <c r="I89" s="37"/>
+      <c r="J89" s="38"/>
       <c r="K89" s="19"/>
-      <c r="L89" s="41"/>
+      <c r="L89" s="39"/>
       <c r="M89" s="19"/>
       <c r="N89" t="str">
         <f t="shared" si="244"/>
@@ -23467,12 +23964,12 @@
         <v/>
       </c>
       <c r="F90" s="19"/>
-      <c r="G90" s="38"/>
-      <c r="H90" s="39"/>
-      <c r="I90" s="39"/>
-      <c r="J90" s="40"/>
+      <c r="G90" s="36"/>
+      <c r="H90" s="37"/>
+      <c r="I90" s="37"/>
+      <c r="J90" s="38"/>
       <c r="K90" s="19"/>
-      <c r="L90" s="41"/>
+      <c r="L90" s="39"/>
       <c r="M90" s="19"/>
       <c r="N90" t="str">
         <f t="shared" si="244"/>
@@ -23633,12 +24130,12 @@
         <v/>
       </c>
       <c r="F91" s="19"/>
-      <c r="G91" s="38"/>
-      <c r="H91" s="39"/>
-      <c r="I91" s="39"/>
-      <c r="J91" s="40"/>
+      <c r="G91" s="36"/>
+      <c r="H91" s="37"/>
+      <c r="I91" s="37"/>
+      <c r="J91" s="38"/>
       <c r="K91" s="19"/>
-      <c r="L91" s="41"/>
+      <c r="L91" s="39"/>
       <c r="M91" s="19"/>
       <c r="N91" t="str">
         <f t="shared" si="244"/>
@@ -23799,12 +24296,12 @@
         <v/>
       </c>
       <c r="F92" s="19"/>
-      <c r="G92" s="38"/>
-      <c r="H92" s="39"/>
-      <c r="I92" s="39"/>
-      <c r="J92" s="40"/>
+      <c r="G92" s="36"/>
+      <c r="H92" s="37"/>
+      <c r="I92" s="37"/>
+      <c r="J92" s="38"/>
       <c r="K92" s="19"/>
-      <c r="L92" s="41"/>
+      <c r="L92" s="39"/>
       <c r="M92" s="19"/>
       <c r="N92" t="str">
         <f t="shared" si="244"/>
@@ -23965,12 +24462,12 @@
         <v/>
       </c>
       <c r="F93" s="19"/>
-      <c r="G93" s="38"/>
-      <c r="H93" s="39"/>
-      <c r="I93" s="39"/>
-      <c r="J93" s="40"/>
+      <c r="G93" s="36"/>
+      <c r="H93" s="37"/>
+      <c r="I93" s="37"/>
+      <c r="J93" s="38"/>
       <c r="K93" s="19"/>
-      <c r="L93" s="41"/>
+      <c r="L93" s="39"/>
       <c r="M93" s="19"/>
       <c r="N93" t="str">
         <f t="shared" si="244"/>
@@ -24131,12 +24628,12 @@
         <v/>
       </c>
       <c r="F94" s="19"/>
-      <c r="G94" s="38"/>
-      <c r="H94" s="39"/>
-      <c r="I94" s="39"/>
-      <c r="J94" s="40"/>
+      <c r="G94" s="36"/>
+      <c r="H94" s="37"/>
+      <c r="I94" s="37"/>
+      <c r="J94" s="38"/>
       <c r="K94" s="19"/>
-      <c r="L94" s="41"/>
+      <c r="L94" s="39"/>
       <c r="M94" s="19"/>
       <c r="N94" t="str">
         <f t="shared" si="244"/>
@@ -24297,12 +24794,12 @@
         <v/>
       </c>
       <c r="F95" s="19"/>
-      <c r="G95" s="38"/>
-      <c r="H95" s="39"/>
-      <c r="I95" s="39"/>
-      <c r="J95" s="40"/>
+      <c r="G95" s="36"/>
+      <c r="H95" s="37"/>
+      <c r="I95" s="37"/>
+      <c r="J95" s="38"/>
       <c r="K95" s="19"/>
-      <c r="L95" s="41"/>
+      <c r="L95" s="39"/>
       <c r="M95" s="19"/>
       <c r="N95" t="str">
         <f t="shared" si="244"/>
@@ -24463,12 +24960,12 @@
         <v/>
       </c>
       <c r="F96" s="19"/>
-      <c r="G96" s="38"/>
-      <c r="H96" s="39"/>
-      <c r="I96" s="39"/>
-      <c r="J96" s="40"/>
+      <c r="G96" s="36"/>
+      <c r="H96" s="37"/>
+      <c r="I96" s="37"/>
+      <c r="J96" s="38"/>
       <c r="K96" s="19"/>
-      <c r="L96" s="41"/>
+      <c r="L96" s="39"/>
       <c r="M96" s="19"/>
       <c r="N96" t="str">
         <f t="shared" si="244"/>
@@ -24629,12 +25126,12 @@
         <v/>
       </c>
       <c r="F97" s="19"/>
-      <c r="G97" s="38"/>
-      <c r="H97" s="39"/>
-      <c r="I97" s="39"/>
-      <c r="J97" s="40"/>
+      <c r="G97" s="36"/>
+      <c r="H97" s="37"/>
+      <c r="I97" s="37"/>
+      <c r="J97" s="38"/>
       <c r="K97" s="19"/>
-      <c r="L97" s="41"/>
+      <c r="L97" s="39"/>
       <c r="M97" s="19"/>
       <c r="N97" t="str">
         <f t="shared" si="244"/>
@@ -24795,12 +25292,12 @@
         <v/>
       </c>
       <c r="F98" s="19"/>
-      <c r="G98" s="38"/>
-      <c r="H98" s="39"/>
-      <c r="I98" s="39"/>
-      <c r="J98" s="40"/>
+      <c r="G98" s="36"/>
+      <c r="H98" s="37"/>
+      <c r="I98" s="37"/>
+      <c r="J98" s="38"/>
       <c r="K98" s="19"/>
-      <c r="L98" s="41"/>
+      <c r="L98" s="39"/>
       <c r="M98" s="19"/>
       <c r="N98" t="str">
         <f t="shared" si="244"/>
@@ -24961,12 +25458,12 @@
         <v/>
       </c>
       <c r="F99" s="19"/>
-      <c r="G99" s="38"/>
-      <c r="H99" s="39"/>
-      <c r="I99" s="39"/>
-      <c r="J99" s="40"/>
+      <c r="G99" s="36"/>
+      <c r="H99" s="37"/>
+      <c r="I99" s="37"/>
+      <c r="J99" s="38"/>
       <c r="K99" s="19"/>
-      <c r="L99" s="41"/>
+      <c r="L99" s="39"/>
       <c r="M99" s="19"/>
       <c r="N99" t="str">
         <f t="shared" si="244"/>
@@ -25127,12 +25624,12 @@
         <v/>
       </c>
       <c r="F100" s="19"/>
-      <c r="G100" s="38"/>
-      <c r="H100" s="39"/>
-      <c r="I100" s="39"/>
-      <c r="J100" s="40"/>
+      <c r="G100" s="36"/>
+      <c r="H100" s="37"/>
+      <c r="I100" s="37"/>
+      <c r="J100" s="38"/>
       <c r="K100" s="19"/>
-      <c r="L100" s="41"/>
+      <c r="L100" s="39"/>
       <c r="M100" s="19"/>
       <c r="N100" t="str">
         <f t="shared" si="244"/>
@@ -25293,12 +25790,12 @@
         <v/>
       </c>
       <c r="F101" s="19"/>
-      <c r="G101" s="38"/>
-      <c r="H101" s="39"/>
-      <c r="I101" s="39"/>
-      <c r="J101" s="40"/>
+      <c r="G101" s="36"/>
+      <c r="H101" s="37"/>
+      <c r="I101" s="37"/>
+      <c r="J101" s="38"/>
       <c r="K101" s="19"/>
-      <c r="L101" s="41"/>
+      <c r="L101" s="39"/>
       <c r="M101" s="19"/>
       <c r="N101" t="str">
         <f t="shared" si="244"/>
@@ -25459,12 +25956,12 @@
         <v/>
       </c>
       <c r="F102" s="19"/>
-      <c r="G102" s="38"/>
-      <c r="H102" s="39"/>
-      <c r="I102" s="39"/>
-      <c r="J102" s="40"/>
+      <c r="G102" s="36"/>
+      <c r="H102" s="37"/>
+      <c r="I102" s="37"/>
+      <c r="J102" s="38"/>
       <c r="K102" s="19"/>
-      <c r="L102" s="41"/>
+      <c r="L102" s="39"/>
       <c r="M102" s="19"/>
       <c r="N102" t="str">
         <f t="shared" si="244"/>
@@ -25625,12 +26122,12 @@
         <v/>
       </c>
       <c r="F103" s="19"/>
-      <c r="G103" s="38"/>
-      <c r="H103" s="39"/>
-      <c r="I103" s="39"/>
-      <c r="J103" s="40"/>
+      <c r="G103" s="36"/>
+      <c r="H103" s="37"/>
+      <c r="I103" s="37"/>
+      <c r="J103" s="38"/>
       <c r="K103" s="19"/>
-      <c r="L103" s="41"/>
+      <c r="L103" s="39"/>
       <c r="M103" s="19"/>
       <c r="N103" t="str">
         <f t="shared" si="244"/>
@@ -25791,12 +26288,12 @@
         <v/>
       </c>
       <c r="F104" s="19"/>
-      <c r="G104" s="38"/>
-      <c r="H104" s="39"/>
-      <c r="I104" s="39"/>
-      <c r="J104" s="40"/>
+      <c r="G104" s="36"/>
+      <c r="H104" s="37"/>
+      <c r="I104" s="37"/>
+      <c r="J104" s="38"/>
       <c r="K104" s="19"/>
-      <c r="L104" s="41"/>
+      <c r="L104" s="39"/>
       <c r="M104" s="19"/>
       <c r="N104" t="str">
         <f t="shared" si="244"/>
@@ -25957,12 +26454,12 @@
         <v/>
       </c>
       <c r="F105" s="19"/>
-      <c r="G105" s="38"/>
-      <c r="H105" s="39"/>
-      <c r="I105" s="39"/>
-      <c r="J105" s="40"/>
+      <c r="G105" s="36"/>
+      <c r="H105" s="37"/>
+      <c r="I105" s="37"/>
+      <c r="J105" s="38"/>
       <c r="K105" s="19"/>
-      <c r="L105" s="41"/>
+      <c r="L105" s="39"/>
       <c r="M105" s="19"/>
       <c r="N105" t="str">
         <f t="shared" si="244"/>
@@ -26123,12 +26620,12 @@
         <v/>
       </c>
       <c r="F106" s="19"/>
-      <c r="G106" s="38"/>
-      <c r="H106" s="39"/>
-      <c r="I106" s="39"/>
-      <c r="J106" s="40"/>
+      <c r="G106" s="36"/>
+      <c r="H106" s="37"/>
+      <c r="I106" s="37"/>
+      <c r="J106" s="38"/>
       <c r="K106" s="19"/>
-      <c r="L106" s="41"/>
+      <c r="L106" s="39"/>
       <c r="M106" s="19"/>
       <c r="N106" t="str">
         <f t="shared" si="244"/>
@@ -26289,12 +26786,12 @@
         <v/>
       </c>
       <c r="F107" s="19"/>
-      <c r="G107" s="38"/>
-      <c r="H107" s="39"/>
-      <c r="I107" s="39"/>
-      <c r="J107" s="40"/>
+      <c r="G107" s="36"/>
+      <c r="H107" s="37"/>
+      <c r="I107" s="37"/>
+      <c r="J107" s="38"/>
       <c r="K107" s="19"/>
-      <c r="L107" s="41"/>
+      <c r="L107" s="39"/>
       <c r="M107" s="19"/>
       <c r="N107" t="str">
         <f t="shared" si="244"/>
@@ -26455,12 +26952,12 @@
         <v/>
       </c>
       <c r="F108" s="19"/>
-      <c r="G108" s="38"/>
-      <c r="H108" s="39"/>
-      <c r="I108" s="39"/>
-      <c r="J108" s="40"/>
+      <c r="G108" s="36"/>
+      <c r="H108" s="37"/>
+      <c r="I108" s="37"/>
+      <c r="J108" s="38"/>
       <c r="K108" s="19"/>
-      <c r="L108" s="41"/>
+      <c r="L108" s="39"/>
       <c r="M108" s="19"/>
       <c r="N108" t="str">
         <f t="shared" si="244"/>
@@ -26621,12 +27118,12 @@
         <v/>
       </c>
       <c r="F109" s="19"/>
-      <c r="G109" s="38"/>
-      <c r="H109" s="39"/>
-      <c r="I109" s="39"/>
-      <c r="J109" s="40"/>
+      <c r="G109" s="36"/>
+      <c r="H109" s="37"/>
+      <c r="I109" s="37"/>
+      <c r="J109" s="38"/>
       <c r="K109" s="19"/>
-      <c r="L109" s="41"/>
+      <c r="L109" s="39"/>
       <c r="M109" s="19"/>
       <c r="N109" t="str">
         <f t="shared" si="244"/>
@@ -26787,12 +27284,12 @@
         <v/>
       </c>
       <c r="F110" s="19"/>
-      <c r="G110" s="38"/>
-      <c r="H110" s="39"/>
-      <c r="I110" s="39"/>
-      <c r="J110" s="40"/>
+      <c r="G110" s="36"/>
+      <c r="H110" s="37"/>
+      <c r="I110" s="37"/>
+      <c r="J110" s="38"/>
       <c r="K110" s="19"/>
-      <c r="L110" s="41"/>
+      <c r="L110" s="39"/>
       <c r="M110" s="19"/>
       <c r="N110" t="str">
         <f t="shared" si="244"/>
@@ -26953,12 +27450,12 @@
         <v/>
       </c>
       <c r="F111" s="19"/>
-      <c r="G111" s="38"/>
-      <c r="H111" s="39"/>
-      <c r="I111" s="39"/>
-      <c r="J111" s="40"/>
+      <c r="G111" s="36"/>
+      <c r="H111" s="37"/>
+      <c r="I111" s="37"/>
+      <c r="J111" s="38"/>
       <c r="K111" s="19"/>
-      <c r="L111" s="41"/>
+      <c r="L111" s="39"/>
       <c r="M111" s="19"/>
       <c r="N111" t="str">
         <f t="shared" si="244"/>
@@ -27119,12 +27616,12 @@
         <v/>
       </c>
       <c r="F112" s="19"/>
-      <c r="G112" s="38"/>
-      <c r="H112" s="39"/>
-      <c r="I112" s="39"/>
-      <c r="J112" s="40"/>
+      <c r="G112" s="36"/>
+      <c r="H112" s="37"/>
+      <c r="I112" s="37"/>
+      <c r="J112" s="38"/>
       <c r="K112" s="19"/>
-      <c r="L112" s="41"/>
+      <c r="L112" s="39"/>
       <c r="M112" s="19"/>
       <c r="N112" t="str">
         <f t="shared" si="244"/>
@@ -27285,12 +27782,12 @@
         <v/>
       </c>
       <c r="F113" s="19"/>
-      <c r="G113" s="38"/>
-      <c r="H113" s="39"/>
-      <c r="I113" s="39"/>
-      <c r="J113" s="40"/>
+      <c r="G113" s="36"/>
+      <c r="H113" s="37"/>
+      <c r="I113" s="37"/>
+      <c r="J113" s="38"/>
       <c r="K113" s="19"/>
-      <c r="L113" s="41"/>
+      <c r="L113" s="39"/>
       <c r="M113" s="19"/>
       <c r="N113" t="str">
         <f t="shared" si="244"/>
@@ -27451,12 +27948,12 @@
         <v/>
       </c>
       <c r="F114" s="19"/>
-      <c r="G114" s="38"/>
-      <c r="H114" s="39"/>
-      <c r="I114" s="39"/>
-      <c r="J114" s="40"/>
+      <c r="G114" s="36"/>
+      <c r="H114" s="37"/>
+      <c r="I114" s="37"/>
+      <c r="J114" s="38"/>
       <c r="K114" s="19"/>
-      <c r="L114" s="41"/>
+      <c r="L114" s="39"/>
       <c r="M114" s="19"/>
       <c r="N114" t="str">
         <f t="shared" si="244"/>
@@ -27617,12 +28114,12 @@
         <v/>
       </c>
       <c r="F115" s="19"/>
-      <c r="G115" s="38"/>
-      <c r="H115" s="39"/>
-      <c r="I115" s="39"/>
-      <c r="J115" s="40"/>
+      <c r="G115" s="36"/>
+      <c r="H115" s="37"/>
+      <c r="I115" s="37"/>
+      <c r="J115" s="38"/>
       <c r="K115" s="19"/>
-      <c r="L115" s="41"/>
+      <c r="L115" s="39"/>
       <c r="M115" s="19"/>
       <c r="N115" t="str">
         <f t="shared" si="244"/>
@@ -27783,12 +28280,12 @@
         <v/>
       </c>
       <c r="F116" s="19"/>
-      <c r="G116" s="38"/>
-      <c r="H116" s="39"/>
-      <c r="I116" s="39"/>
-      <c r="J116" s="40"/>
+      <c r="G116" s="36"/>
+      <c r="H116" s="37"/>
+      <c r="I116" s="37"/>
+      <c r="J116" s="38"/>
       <c r="K116" s="19"/>
-      <c r="L116" s="41"/>
+      <c r="L116" s="39"/>
       <c r="M116" s="19"/>
       <c r="N116" t="str">
         <f t="shared" si="244"/>
@@ -27949,12 +28446,12 @@
         <v/>
       </c>
       <c r="F117" s="19"/>
-      <c r="G117" s="38"/>
-      <c r="H117" s="39"/>
-      <c r="I117" s="39"/>
-      <c r="J117" s="40"/>
+      <c r="G117" s="36"/>
+      <c r="H117" s="37"/>
+      <c r="I117" s="37"/>
+      <c r="J117" s="38"/>
       <c r="K117" s="19"/>
-      <c r="L117" s="41"/>
+      <c r="L117" s="39"/>
       <c r="M117" s="19"/>
       <c r="N117" t="str">
         <f t="shared" si="244"/>
@@ -28115,12 +28612,12 @@
         <v/>
       </c>
       <c r="F118" s="19"/>
-      <c r="G118" s="38"/>
-      <c r="H118" s="39"/>
-      <c r="I118" s="39"/>
-      <c r="J118" s="40"/>
+      <c r="G118" s="36"/>
+      <c r="H118" s="37"/>
+      <c r="I118" s="37"/>
+      <c r="J118" s="38"/>
       <c r="K118" s="19"/>
-      <c r="L118" s="41"/>
+      <c r="L118" s="39"/>
       <c r="M118" s="19"/>
       <c r="N118" t="str">
         <f t="shared" si="244"/>
@@ -28281,12 +28778,12 @@
         <v/>
       </c>
       <c r="F119" s="19"/>
-      <c r="G119" s="38"/>
-      <c r="H119" s="39"/>
-      <c r="I119" s="39"/>
-      <c r="J119" s="40"/>
+      <c r="G119" s="36"/>
+      <c r="H119" s="37"/>
+      <c r="I119" s="37"/>
+      <c r="J119" s="38"/>
       <c r="K119" s="19"/>
-      <c r="L119" s="41"/>
+      <c r="L119" s="39"/>
       <c r="M119" s="19"/>
       <c r="N119" t="str">
         <f t="shared" si="244"/>
@@ -28447,12 +28944,12 @@
         <v/>
       </c>
       <c r="F120" s="19"/>
-      <c r="G120" s="38"/>
-      <c r="H120" s="39"/>
-      <c r="I120" s="39"/>
-      <c r="J120" s="40"/>
+      <c r="G120" s="36"/>
+      <c r="H120" s="37"/>
+      <c r="I120" s="37"/>
+      <c r="J120" s="38"/>
       <c r="K120" s="19"/>
-      <c r="L120" s="41"/>
+      <c r="L120" s="39"/>
       <c r="M120" s="19"/>
       <c r="N120" t="str">
         <f t="shared" si="244"/>
@@ -28642,13 +29139,13 @@
     <mergeCell ref="B34:C34"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="3" priority="24" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="31" operator="between">
       <formula>0</formula>
       <formula>1000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB9:BK9">
-    <cfRule type="colorScale" priority="23">
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="num" val="0.5"/>
         <cfvo type="num" val="1"/>
@@ -28660,7 +29157,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB10:BK10">
-    <cfRule type="colorScale" priority="22">
+    <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="num" val="0.5"/>
         <cfvo type="num" val="1.75"/>
@@ -28671,39 +29168,36 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BB11:BK26 BL13:BL29 C20:C22 C28:C30 C7:C18">
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
+  <conditionalFormatting sqref="BL27:BL29 C24:C26 C32">
+    <cfRule type="cellIs" priority="2" stopIfTrue="1" operator="equal">
+      <formula>""</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B72 BA13:BA18 B10:B13">
-    <cfRule type="expression" dxfId="2" priority="18">
-      <formula>"$C$15&lt;=0"</formula>
+    <cfRule type="cellIs" dxfId="13" priority="20" operator="greaterThan">
+      <formula>0</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BL27:BL29 C24:C26 C32">
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="num" val="1.0000000000000001E-30"/>
-        <cfvo type="num" val="1.0000000000000001E-30"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="lessThanOrEqual">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB51:BK55">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="11" priority="9">
       <formula>IFERROR(BB69,-1)&lt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB44:BK48">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="10" priority="8">
       <formula>IFERROR(BB69,-1)&lt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BB11:BK26 BL13:BL26 C20:C22 C28:C30 C7:C18">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="28" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="1" stopIfTrue="1" operator="equal">
+      <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.78740157500000008" bottom="0.78740157500000008" header="0.30000000000000004" footer="0.30000000000000004"/>

</xml_diff>

<commit_message>
v0.20.9 & TAC LS v0.10 Update
</commit_message>
<xml_diff>
--- a/BasePlanning.xlsx
+++ b/BasePlanning.xlsx
@@ -673,24 +673,6 @@
     <t>Base 2 is the powerhorse for Assembly. It can punch out a single 415 Tank in a bit over 6 hours. It requires Karbonite for Energygeneration and Products from Base 1</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">USI Kolonization System V0.20.8 &amp; TAC LS v0.9.x
-Base Planning Spreadsheet
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="16"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>ONLY CHANGE THE BLUE CELLS</t>
-    </r>
-  </si>
-  <si>
     <t>Is Primary</t>
   </si>
   <si>
@@ -737,6 +719,24 @@
   </si>
   <si>
     <t>Base 5 contains the logistics hub and a lot of storage for extracted resources and fuel</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">USI Kolonization System V0.20.9 &amp; TAC LS v0.10
+Base Planning Spreadsheet
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="16"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ONLY CHANGE THE BLUE CELLS</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -801,7 +801,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -829,12 +829,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -871,7 +865,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90" wrapText="1"/>
@@ -918,7 +912,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1320,10 +1313,7 @@
   <dimension ref="A1:DR124"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C81" sqref="C81"/>
+      <selection activeCell="C7" sqref="C7:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1334,9 +1324,9 @@
     <col min="4" max="4" width="3.42578125" customWidth="1"/>
     <col min="5" max="5" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.140625" style="32" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="4.7109375" style="34" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.7109375" style="33" customWidth="1"/>
+    <col min="7" max="7" width="4.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="4.7109375" style="33" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.7109375" style="32" customWidth="1"/>
     <col min="11" max="11" width="3.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.28515625" style="7" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="3.7109375" style="7" customWidth="1"/>
@@ -1382,10 +1372,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:122" ht="153" customHeight="1">
-      <c r="B1" s="43" t="s">
-        <v>206</v>
-      </c>
-      <c r="C1" s="43"/>
+      <c r="B1" s="42" t="s">
+        <v>222</v>
+      </c>
+      <c r="C1" s="42"/>
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1423,7 +1413,7 @@
         <v>5</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>118</v>
@@ -1765,12 +1755,12 @@
         <v/>
       </c>
       <c r="F2" s="19"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="37"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="36"/>
       <c r="K2" s="19"/>
-      <c r="L2" s="38"/>
+      <c r="L2" s="37"/>
       <c r="M2" s="19"/>
       <c r="N2" t="str">
         <f t="shared" ref="N2" si="3">IF(AND(H2="",I2=""),"",IF(H2="",0,2-H2)+IF(I2="",0,2-I2))</f>
@@ -1967,23 +1957,23 @@
       <c r="BV2" s="22">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="BW2" s="26">
+      <c r="BW2" s="22">
         <f>(0.039+0.0125+0.0052)/3</f>
         <v>1.89E-2</v>
       </c>
-      <c r="BX2" s="26">
+      <c r="BX2" s="22">
         <f>(0.0221+0.0088+0.0258)/3</f>
         <v>1.89E-2</v>
       </c>
-      <c r="BY2" s="26">
+      <c r="BY2" s="22">
         <f>(0.0239+0.0155+0.0173)/3</f>
         <v>1.89E-2</v>
       </c>
-      <c r="BZ2" s="26">
+      <c r="BZ2" s="22">
         <f>(0.0155+0.0173+0.0239+0.0164+0.0197+0.0206)/6</f>
         <v>1.89E-2</v>
       </c>
-      <c r="CA2" s="26">
+      <c r="CA2" s="22">
         <f>(0.039+0.0125)/2</f>
         <v>2.5750000000000002E-2</v>
       </c>
@@ -2024,21 +2014,21 @@
       <c r="CN2" s="15"/>
     </row>
     <row r="3" spans="2:122" ht="15" customHeight="1">
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="42"/>
+      <c r="C3" s="41"/>
       <c r="E3" s="4" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F3" s="19"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="37"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="36"/>
       <c r="K3" s="19"/>
-      <c r="L3" s="38"/>
+      <c r="L3" s="37"/>
       <c r="M3" s="19"/>
       <c r="N3" t="str">
         <f t="shared" ref="N3:N66" si="38">IF(AND(H3="",I3=""),"",IF(H3="",0,2-H3)+IF(I3="",0,2-I3))</f>
@@ -2232,12 +2222,27 @@
       <c r="BT3" s="13"/>
       <c r="BU3" s="13"/>
       <c r="BV3" s="13"/>
-      <c r="CE3">
+      <c r="BW3" s="7"/>
+      <c r="BX3" s="7"/>
+      <c r="BY3" s="7"/>
+      <c r="BZ3" s="7"/>
+      <c r="CA3" s="7"/>
+      <c r="CB3" s="7"/>
+      <c r="CC3" s="7"/>
+      <c r="CD3" s="7"/>
+      <c r="CE3" s="7">
         <v>-4.2500000000000001E-7</v>
       </c>
-      <c r="CF3">
+      <c r="CF3" s="7">
         <v>4.2500000000000001E-7</v>
       </c>
+      <c r="CG3" s="7"/>
+      <c r="CH3" s="7"/>
+      <c r="CI3" s="7"/>
+      <c r="CJ3" s="7"/>
+      <c r="CK3" s="7"/>
+      <c r="CL3" s="7"/>
+      <c r="CM3" s="7"/>
       <c r="CN3" s="15">
         <f>SUM(BT3:CM3)</f>
         <v>0</v>
@@ -2347,12 +2352,12 @@
       <c r="F4" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="G4" s="35"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="37"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="36"/>
       <c r="K4" s="19"/>
-      <c r="L4" s="38"/>
+      <c r="L4" s="37"/>
       <c r="M4" s="19"/>
       <c r="N4" t="str">
         <f t="shared" si="38"/>
@@ -2544,6 +2549,23 @@
       <c r="BT4" s="13"/>
       <c r="BU4" s="13"/>
       <c r="BV4" s="13"/>
+      <c r="BW4" s="7"/>
+      <c r="BX4" s="7"/>
+      <c r="BY4" s="7"/>
+      <c r="BZ4" s="7"/>
+      <c r="CA4" s="7"/>
+      <c r="CB4" s="7"/>
+      <c r="CC4" s="7"/>
+      <c r="CD4" s="7"/>
+      <c r="CE4" s="7"/>
+      <c r="CF4" s="7"/>
+      <c r="CG4" s="7"/>
+      <c r="CH4" s="7"/>
+      <c r="CI4" s="7"/>
+      <c r="CJ4" s="7"/>
+      <c r="CK4" s="7"/>
+      <c r="CL4" s="7"/>
+      <c r="CM4" s="7"/>
       <c r="CN4" s="15">
         <f t="shared" ref="CN4:CN8" si="46">SUM(BT4:CM4)</f>
         <v>0</v>
@@ -2660,18 +2682,18 @@
       <c r="F5" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="G5" s="35">
+      <c r="G5" s="34">
         <v>9.1</v>
       </c>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="37">
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="36">
         <v>1</v>
       </c>
       <c r="K5" s="19">
         <v>1</v>
       </c>
-      <c r="L5" s="38"/>
+      <c r="L5" s="37"/>
       <c r="M5" s="19"/>
       <c r="N5" t="str">
         <f t="shared" si="38"/>
@@ -2861,20 +2883,33 @@
         <v>-8.4999999999999995E-4</v>
       </c>
       <c r="BS5" s="13"/>
-      <c r="BW5">
+      <c r="BW5" s="7">
         <f>-3*0.051</f>
         <v>-0.153</v>
       </c>
-      <c r="CC5">
+      <c r="BX5" s="7"/>
+      <c r="BY5" s="7"/>
+      <c r="BZ5" s="7"/>
+      <c r="CA5" s="7"/>
+      <c r="CB5" s="7"/>
+      <c r="CC5" s="7">
         <f>0.153-0.0000002125</f>
         <v>0.15299978749999998</v>
       </c>
-      <c r="CD5">
+      <c r="CD5" s="7">
         <v>-2.125E-7</v>
       </c>
-      <c r="CF5">
+      <c r="CE5" s="7"/>
+      <c r="CF5" s="7">
         <v>4.2500000000000001E-7</v>
       </c>
+      <c r="CG5" s="7"/>
+      <c r="CH5" s="7"/>
+      <c r="CI5" s="7"/>
+      <c r="CJ5" s="7"/>
+      <c r="CK5" s="7"/>
+      <c r="CL5" s="7"/>
+      <c r="CM5" s="7"/>
       <c r="CN5" s="15">
         <f t="shared" si="46"/>
         <v>-1.3049442524958954E-17</v>
@@ -2991,24 +3026,24 @@
       <c r="F6" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="G6" s="35">
+      <c r="G6" s="34">
         <v>9.1999999999999993</v>
       </c>
-      <c r="H6" s="36" t="str">
+      <c r="H6" s="35" t="str">
         <f>IF(H5="","",H5)</f>
         <v/>
       </c>
-      <c r="I6" s="36" t="str">
+      <c r="I6" s="35" t="str">
         <f>IF(I5="","",I5)</f>
         <v/>
       </c>
-      <c r="J6" s="37">
+      <c r="J6" s="36">
         <v>1</v>
       </c>
       <c r="K6" s="19">
         <v>1</v>
       </c>
-      <c r="L6" s="38"/>
+      <c r="L6" s="37"/>
       <c r="M6" s="19">
         <v>1</v>
       </c>
@@ -3200,20 +3235,33 @@
         <v>-8.4999999999999995E-4</v>
       </c>
       <c r="BS6" s="13"/>
-      <c r="BX6">
+      <c r="BW6" s="7"/>
+      <c r="BX6" s="7">
         <f>-3*0.034</f>
         <v>-0.10200000000000001</v>
       </c>
-      <c r="CD6">
+      <c r="BY6" s="7"/>
+      <c r="BZ6" s="7"/>
+      <c r="CA6" s="7"/>
+      <c r="CB6" s="7"/>
+      <c r="CC6" s="7"/>
+      <c r="CD6" s="7">
         <f>0.102-0.0000002125</f>
         <v>0.10199978749999999</v>
       </c>
-      <c r="CE6">
+      <c r="CE6" s="7">
         <v>-2.125E-7</v>
       </c>
-      <c r="CF6">
+      <c r="CF6" s="7">
         <v>4.2500000000000001E-7</v>
       </c>
+      <c r="CG6" s="7"/>
+      <c r="CH6" s="7"/>
+      <c r="CI6" s="7"/>
+      <c r="CJ6" s="7"/>
+      <c r="CK6" s="7"/>
+      <c r="CL6" s="7"/>
+      <c r="CM6" s="7"/>
       <c r="CN6" s="15">
         <f t="shared" si="46"/>
         <v>-1.3049442524958954E-17</v>
@@ -3316,10 +3364,10 @@
       </c>
     </row>
     <row r="7" spans="2:122">
-      <c r="B7" s="44" t="s">
-        <v>214</v>
-      </c>
-      <c r="C7" s="45">
+      <c r="B7" s="43" t="s">
+        <v>213</v>
+      </c>
+      <c r="C7" s="44">
         <f ca="1">ROUNDUP(-MIN(C80:C83)/2333,1)</f>
         <v>8.1999999999999993</v>
       </c>
@@ -3330,24 +3378,24 @@
       <c r="F7" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="G7" s="35">
+      <c r="G7" s="34">
         <v>9.3000000000000007</v>
       </c>
-      <c r="H7" s="36" t="str">
+      <c r="H7" s="35" t="str">
         <f>IF(H6="","",H6)</f>
         <v/>
       </c>
-      <c r="I7" s="36" t="str">
+      <c r="I7" s="35" t="str">
         <f>IF(I6="","",I6)</f>
         <v/>
       </c>
-      <c r="J7" s="37">
+      <c r="J7" s="36">
         <v>1</v>
       </c>
       <c r="K7" s="19">
         <v>1</v>
       </c>
-      <c r="L7" s="38"/>
+      <c r="L7" s="37"/>
       <c r="M7" s="19">
         <v>1</v>
       </c>
@@ -3539,17 +3587,31 @@
         <v>-8.4999999999999995E-4</v>
       </c>
       <c r="BS7" s="13"/>
-      <c r="BY7">
+      <c r="BW7" s="7"/>
+      <c r="BX7" s="7"/>
+      <c r="BY7" s="7">
         <f>-3*0.017</f>
         <v>-5.1000000000000004E-2</v>
       </c>
-      <c r="CE7">
+      <c r="BZ7" s="7"/>
+      <c r="CA7" s="7"/>
+      <c r="CB7" s="7"/>
+      <c r="CC7" s="7"/>
+      <c r="CD7" s="7"/>
+      <c r="CE7" s="7">
         <f>0.051-0.000000425</f>
         <v>5.0999574999999998E-2</v>
       </c>
-      <c r="CF7">
+      <c r="CF7" s="7">
         <v>4.2500000000000001E-7</v>
       </c>
+      <c r="CG7" s="7"/>
+      <c r="CH7" s="7"/>
+      <c r="CI7" s="7"/>
+      <c r="CJ7" s="7"/>
+      <c r="CK7" s="7"/>
+      <c r="CL7" s="7"/>
+      <c r="CM7" s="7"/>
       <c r="CN7" s="15">
         <f t="shared" si="46"/>
         <v>-5.2822562777554271E-18</v>
@@ -3652,19 +3714,19 @@
       </c>
     </row>
     <row r="8" spans="2:122">
-      <c r="B8" s="44"/>
-      <c r="C8" s="45"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="44"/>
       <c r="E8" s="4" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="F8" s="19"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="37"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="36"/>
       <c r="K8" s="19"/>
-      <c r="L8" s="38"/>
+      <c r="L8" s="37"/>
       <c r="M8" s="19"/>
       <c r="N8" t="str">
         <f t="shared" si="38"/>
@@ -3857,20 +3919,33 @@
       <c r="BT8" s="13"/>
       <c r="BU8" s="13"/>
       <c r="BV8" s="13"/>
-      <c r="BW8">
+      <c r="BW8" s="7">
         <f>3*0.085</f>
         <v>0.255</v>
       </c>
-      <c r="CC8">
+      <c r="BX8" s="7"/>
+      <c r="BY8" s="7"/>
+      <c r="BZ8" s="7"/>
+      <c r="CA8" s="7"/>
+      <c r="CB8" s="7"/>
+      <c r="CC8" s="7">
         <v>-2.125E-7</v>
       </c>
-      <c r="CD8">
+      <c r="CD8" s="7">
         <v>-2.125E-7</v>
       </c>
-      <c r="CF8">
+      <c r="CE8" s="7"/>
+      <c r="CF8" s="7">
         <f>0.000000425-0.255</f>
         <v>-0.25499957499999998</v>
       </c>
+      <c r="CG8" s="7"/>
+      <c r="CH8" s="7"/>
+      <c r="CI8" s="7"/>
+      <c r="CJ8" s="7"/>
+      <c r="CK8" s="7"/>
+      <c r="CL8" s="7"/>
+      <c r="CM8" s="7"/>
       <c r="CN8" s="15">
         <f t="shared" si="46"/>
         <v>0</v>
@@ -3973,8 +4048,8 @@
       </c>
     </row>
     <row r="9" spans="2:122">
-      <c r="B9" s="44"/>
-      <c r="C9" s="45"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="44"/>
       <c r="E9" s="4">
         <f t="shared" ca="1" si="2"/>
         <v>1.3976999999999999</v>
@@ -3982,20 +4057,20 @@
       <c r="F9" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="35">
+      <c r="G9" s="34">
         <v>10</v>
       </c>
-      <c r="H9" s="36">
+      <c r="H9" s="35">
         <v>0.89400000000000002</v>
       </c>
-      <c r="I9" s="36"/>
-      <c r="J9" s="37">
+      <c r="I9" s="35"/>
+      <c r="J9" s="36">
         <v>3</v>
       </c>
       <c r="K9" s="19">
         <v>1</v>
       </c>
-      <c r="L9" s="38"/>
+      <c r="L9" s="37"/>
       <c r="M9" s="19"/>
       <c r="N9">
         <f t="shared" si="38"/>
@@ -4202,19 +4277,32 @@
         <v>-8.4999999999999995E-4</v>
       </c>
       <c r="BS9" s="13"/>
-      <c r="BW9">
+      <c r="BW9" s="7">
         <f>-3*0.0255</f>
         <v>-7.6499999999999999E-2</v>
       </c>
-      <c r="CC9">
+      <c r="BX9" s="7"/>
+      <c r="BY9" s="7"/>
+      <c r="BZ9" s="7"/>
+      <c r="CA9" s="7"/>
+      <c r="CB9" s="7"/>
+      <c r="CC9" s="7">
         <v>-2.125E-7</v>
       </c>
-      <c r="CD9">
+      <c r="CD9" s="7">
         <v>-2.125E-7</v>
       </c>
-      <c r="CF9">
+      <c r="CE9" s="7"/>
+      <c r="CF9" s="7">
         <v>4.2500000000000001E-7</v>
       </c>
+      <c r="CG9" s="7"/>
+      <c r="CH9" s="7"/>
+      <c r="CI9" s="7"/>
+      <c r="CJ9" s="7"/>
+      <c r="CK9" s="7"/>
+      <c r="CL9" s="7"/>
+      <c r="CM9" s="7"/>
       <c r="CN9" s="15">
         <f t="shared" ref="CN9:CN11" si="52">SUM(BT9:CM9)</f>
         <v>-7.6499999999999999E-2</v>
@@ -4331,22 +4419,22 @@
       <c r="F10" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="35">
+      <c r="G10" s="34">
         <v>11</v>
       </c>
-      <c r="H10" s="36">
+      <c r="H10" s="35">
         <v>0.1</v>
       </c>
-      <c r="I10" s="36">
+      <c r="I10" s="35">
         <v>0.246</v>
       </c>
-      <c r="J10" s="37">
+      <c r="J10" s="36">
         <v>3</v>
       </c>
       <c r="K10" s="19">
         <v>1</v>
       </c>
-      <c r="L10" s="38"/>
+      <c r="L10" s="37"/>
       <c r="M10" s="19"/>
       <c r="N10">
         <f t="shared" si="38"/>
@@ -4553,19 +4641,32 @@
         <v>-8.4999999999999995E-4</v>
       </c>
       <c r="BS10" s="13"/>
-      <c r="BX10">
+      <c r="BW10" s="7"/>
+      <c r="BX10" s="7">
         <f>-3*0.017</f>
         <v>-5.1000000000000004E-2</v>
       </c>
-      <c r="CD10">
+      <c r="BY10" s="7"/>
+      <c r="BZ10" s="7"/>
+      <c r="CA10" s="7"/>
+      <c r="CB10" s="7"/>
+      <c r="CC10" s="7"/>
+      <c r="CD10" s="7">
         <v>-2.125E-7</v>
       </c>
-      <c r="CE10">
+      <c r="CE10" s="7">
         <v>-2.125E-7</v>
       </c>
-      <c r="CF10">
+      <c r="CF10" s="7">
         <v>4.2500000000000001E-7</v>
       </c>
+      <c r="CG10" s="7"/>
+      <c r="CH10" s="7"/>
+      <c r="CI10" s="7"/>
+      <c r="CJ10" s="7"/>
+      <c r="CK10" s="7"/>
+      <c r="CL10" s="7"/>
+      <c r="CM10" s="7"/>
       <c r="CN10" s="15">
         <f t="shared" si="52"/>
         <v>-5.1000000000000004E-2</v>
@@ -4682,22 +4783,22 @@
       <c r="F11" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="35">
-        <v>0</v>
-      </c>
-      <c r="H11" s="36">
+      <c r="G11" s="34">
+        <v>0</v>
+      </c>
+      <c r="H11" s="35">
         <v>0.47</v>
       </c>
-      <c r="I11" s="36">
+      <c r="I11" s="35">
         <v>0.5</v>
       </c>
-      <c r="J11" s="37">
+      <c r="J11" s="36">
         <v>1</v>
       </c>
       <c r="K11" s="19">
         <v>1</v>
       </c>
-      <c r="L11" s="38"/>
+      <c r="L11" s="37"/>
       <c r="M11" s="19"/>
       <c r="N11">
         <f t="shared" si="38"/>
@@ -4907,16 +5008,30 @@
       <c r="BT11" s="13"/>
       <c r="BU11" s="13"/>
       <c r="BV11" s="13"/>
-      <c r="BY11">
+      <c r="BW11" s="7"/>
+      <c r="BX11" s="7"/>
+      <c r="BY11" s="7">
         <f>-3*0.0085</f>
         <v>-2.5500000000000002E-2</v>
       </c>
-      <c r="CE11">
+      <c r="BZ11" s="7"/>
+      <c r="CA11" s="7"/>
+      <c r="CB11" s="7"/>
+      <c r="CC11" s="7"/>
+      <c r="CD11" s="7"/>
+      <c r="CE11" s="7">
         <v>-4.2500000000000001E-7</v>
       </c>
-      <c r="CF11">
+      <c r="CF11" s="7">
         <v>4.2500000000000001E-7</v>
       </c>
+      <c r="CG11" s="7"/>
+      <c r="CH11" s="7"/>
+      <c r="CI11" s="7"/>
+      <c r="CJ11" s="7"/>
+      <c r="CK11" s="7"/>
+      <c r="CL11" s="7"/>
+      <c r="CM11" s="7"/>
       <c r="CN11" s="15">
         <f t="shared" si="52"/>
         <v>-2.5500000000000002E-2</v>
@@ -5033,16 +5148,16 @@
       <c r="F12" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="G12" s="35">
+      <c r="G12" s="34">
         <v>210</v>
       </c>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="37"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="36"/>
       <c r="K12" s="19">
         <v>1</v>
       </c>
-      <c r="L12" s="38"/>
+      <c r="L12" s="37"/>
       <c r="M12" s="19"/>
       <c r="N12" t="str">
         <f t="shared" si="38"/>
@@ -5215,25 +5330,35 @@
       <c r="BV12">
         <v>-0.1275</v>
       </c>
-      <c r="CB12">
+      <c r="BW12" s="7"/>
+      <c r="BX12" s="7"/>
+      <c r="BY12" s="7"/>
+      <c r="BZ12" s="7"/>
+      <c r="CA12" s="7"/>
+      <c r="CB12" s="7">
         <v>3.2452726574999999E-4</v>
       </c>
-      <c r="CC12">
+      <c r="CC12" s="7">
         <v>-2.125E-7</v>
       </c>
-      <c r="CD12">
+      <c r="CD12" s="7">
         <v>-2.125E-7</v>
       </c>
-      <c r="CF12">
+      <c r="CE12" s="7"/>
+      <c r="CF12" s="7">
         <v>4.2500000000000001E-7</v>
       </c>
-      <c r="CJ12">
+      <c r="CG12" s="7"/>
+      <c r="CH12" s="7"/>
+      <c r="CI12" s="7"/>
+      <c r="CJ12" s="7">
         <v>-6.2422730897999999E-4</v>
       </c>
-      <c r="CK12">
+      <c r="CK12" s="7">
         <v>9.0895593895410007E-2</v>
       </c>
-      <c r="CM12">
+      <c r="CL12" s="7"/>
+      <c r="CM12" s="7">
         <v>6.8629536528E-4</v>
       </c>
       <c r="CN12" s="15">
@@ -5352,16 +5477,16 @@
       <c r="F13" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="G13" s="35">
+      <c r="G13" s="34">
         <v>200</v>
       </c>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="37"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="36"/>
       <c r="K13" s="19">
         <v>1</v>
       </c>
-      <c r="L13" s="38"/>
+      <c r="L13" s="37"/>
       <c r="M13" s="19"/>
       <c r="N13" t="str">
         <f t="shared" si="38"/>
@@ -5575,25 +5700,35 @@
       <c r="BV13">
         <v>-0.1275</v>
       </c>
-      <c r="CC13">
+      <c r="BW13" s="7"/>
+      <c r="BX13" s="7"/>
+      <c r="BY13" s="7"/>
+      <c r="BZ13" s="7"/>
+      <c r="CA13" s="7"/>
+      <c r="CB13" s="7"/>
+      <c r="CC13" s="7">
         <v>-2.125E-7</v>
       </c>
-      <c r="CD13">
+      <c r="CD13" s="7">
         <v>-2.125E-7</v>
       </c>
-      <c r="CF13">
+      <c r="CE13" s="7"/>
+      <c r="CF13" s="7">
         <v>4.2500000000000001E-7</v>
       </c>
-      <c r="CG13">
+      <c r="CG13" s="7">
         <v>2.3408524086E-4</v>
       </c>
-      <c r="CJ13">
+      <c r="CH13" s="7"/>
+      <c r="CI13" s="7"/>
+      <c r="CJ13" s="7">
         <v>-6.2422730897999999E-4</v>
       </c>
-      <c r="CK13">
+      <c r="CK13" s="7">
         <v>9.0895593895410007E-2</v>
       </c>
-      <c r="CM13">
+      <c r="CL13" s="7"/>
+      <c r="CM13" s="7">
         <v>6.8629536528E-4</v>
       </c>
       <c r="CN13" s="15">
@@ -5712,16 +5847,16 @@
       <c r="F14" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="G14" s="35">
+      <c r="G14" s="34">
         <v>200</v>
       </c>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="37"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="36"/>
       <c r="K14" s="19">
         <v>1</v>
       </c>
-      <c r="L14" s="38"/>
+      <c r="L14" s="37"/>
       <c r="M14" s="19"/>
       <c r="N14" t="str">
         <f t="shared" si="38"/>
@@ -6082,12 +6217,12 @@
         <v/>
       </c>
       <c r="F15" s="19"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="37"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="36"/>
       <c r="K15" s="19"/>
-      <c r="L15" s="38"/>
+      <c r="L15" s="37"/>
       <c r="M15" s="19"/>
       <c r="N15" t="str">
         <f t="shared" si="38"/>
@@ -6456,12 +6591,12 @@
         <v/>
       </c>
       <c r="F16" s="19"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="37"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="36"/>
       <c r="K16" s="19"/>
-      <c r="L16" s="38"/>
+      <c r="L16" s="37"/>
       <c r="M16" s="19"/>
       <c r="N16" t="str">
         <f t="shared" si="38"/>
@@ -6675,21 +6810,33 @@
         <v>-8.4999999999999995E-4</v>
       </c>
       <c r="BS16" s="13"/>
-      <c r="CC16">
+      <c r="BW16" s="7"/>
+      <c r="BX16" s="7"/>
+      <c r="BY16" s="7"/>
+      <c r="BZ16" s="7"/>
+      <c r="CA16" s="7"/>
+      <c r="CB16" s="7"/>
+      <c r="CC16" s="7">
         <v>-2.125E-7</v>
       </c>
-      <c r="CD16">
+      <c r="CD16" s="7">
         <v>-2.125E-7</v>
       </c>
-      <c r="CF16">
+      <c r="CE16" s="7"/>
+      <c r="CF16" s="7">
         <v>4.2500000000000001E-7</v>
       </c>
-      <c r="CI16">
+      <c r="CG16" s="7"/>
+      <c r="CH16" s="7"/>
+      <c r="CI16" s="7">
         <v>-7.0431836926519997E-3</v>
       </c>
-      <c r="CK16">
+      <c r="CJ16" s="7"/>
+      <c r="CK16" s="7">
         <v>6.0597062596939996E-3</v>
       </c>
+      <c r="CL16" s="7"/>
+      <c r="CM16" s="7"/>
       <c r="CN16" s="15">
         <f t="shared" si="60"/>
         <v>-9.8347743295800014E-4</v>
@@ -6804,12 +6951,12 @@
         <v/>
       </c>
       <c r="F17" s="19"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="37"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="36"/>
       <c r="K17" s="19"/>
-      <c r="L17" s="38"/>
+      <c r="L17" s="37"/>
       <c r="M17" s="19"/>
       <c r="N17" t="str">
         <f t="shared" si="38"/>
@@ -7170,12 +7317,12 @@
         <v/>
       </c>
       <c r="F18" s="19"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="37"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="36"/>
       <c r="K18" s="19"/>
-      <c r="L18" s="38"/>
+      <c r="L18" s="37"/>
       <c r="M18" s="19"/>
       <c r="N18" t="str">
         <f t="shared" si="38"/>
@@ -7546,12 +7693,12 @@
       <c r="F19" s="19" t="s">
         <v>205</v>
       </c>
-      <c r="G19" s="35"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="37"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="36"/>
       <c r="K19" s="19"/>
-      <c r="L19" s="38"/>
+      <c r="L19" s="37"/>
       <c r="M19" s="19"/>
       <c r="N19" t="str">
         <f t="shared" si="38"/>
@@ -7912,22 +8059,22 @@
       <c r="F20" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="G20" s="35">
+      <c r="G20" s="34">
         <v>12</v>
       </c>
-      <c r="H20" s="36">
+      <c r="H20" s="35">
         <v>0.09</v>
       </c>
-      <c r="I20" s="36">
+      <c r="I20" s="35">
         <v>0.08</v>
       </c>
-      <c r="J20" s="37">
+      <c r="J20" s="36">
         <v>6</v>
       </c>
       <c r="K20" s="19">
         <v>2</v>
       </c>
-      <c r="L20" s="38"/>
+      <c r="L20" s="37"/>
       <c r="M20" s="19"/>
       <c r="N20">
         <f t="shared" si="38"/>
@@ -8290,22 +8437,22 @@
       <c r="F21" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="G21" s="35">
+      <c r="G21" s="34">
         <v>12</v>
       </c>
-      <c r="H21" s="36">
-        <v>0</v>
-      </c>
-      <c r="I21" s="36">
+      <c r="H21" s="35">
+        <v>0</v>
+      </c>
+      <c r="I21" s="35">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="J21" s="37">
+      <c r="J21" s="36">
         <v>6</v>
       </c>
       <c r="K21" s="19">
         <v>2</v>
       </c>
-      <c r="L21" s="38"/>
+      <c r="L21" s="37"/>
       <c r="M21" s="19"/>
       <c r="N21">
         <f t="shared" si="38"/>
@@ -8659,14 +8806,14 @@
         <v/>
       </c>
       <c r="F22" s="19"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="37"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="36"/>
       <c r="K22" s="19"/>
-      <c r="L22" s="38"/>
+      <c r="L22" s="37"/>
       <c r="M22" s="19"/>
-      <c r="N22" s="29" t="str">
+      <c r="N22" s="28" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
@@ -8884,10 +9031,10 @@
       <c r="BT22" s="22"/>
       <c r="BU22" s="22"/>
       <c r="BV22" s="22"/>
-      <c r="BW22" s="30"/>
-      <c r="BX22" s="30"/>
-      <c r="BY22" s="30"/>
-      <c r="BZ22" s="30"/>
+      <c r="BW22" s="29"/>
+      <c r="BX22" s="29"/>
+      <c r="BY22" s="29"/>
+      <c r="BZ22" s="29"/>
       <c r="CA22" s="7"/>
       <c r="CB22" s="7"/>
       <c r="CC22" s="7">
@@ -9027,20 +9174,20 @@
       <c r="F23" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="G23" s="35">
+      <c r="G23" s="34">
         <v>101</v>
       </c>
-      <c r="H23" s="36">
+      <c r="H23" s="35">
         <v>1</v>
       </c>
-      <c r="I23" s="36">
+      <c r="I23" s="35">
         <v>1</v>
       </c>
-      <c r="J23" s="37"/>
+      <c r="J23" s="36"/>
       <c r="K23" s="19">
         <v>2</v>
       </c>
-      <c r="L23" s="38"/>
+      <c r="L23" s="37"/>
       <c r="M23" s="19"/>
       <c r="N23">
         <f t="shared" si="38"/>
@@ -9261,7 +9408,7 @@
       <c r="BU23" s="22"/>
       <c r="BV23" s="22"/>
       <c r="BW23" s="7"/>
-      <c r="BX23" s="31"/>
+      <c r="BX23" s="30"/>
       <c r="BY23" s="7"/>
       <c r="BZ23" s="7"/>
       <c r="CA23" s="7"/>
@@ -9403,16 +9550,16 @@
       <c r="F24" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="G24" s="35">
+      <c r="G24" s="34">
         <v>210</v>
       </c>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="37"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="36"/>
       <c r="K24" s="19">
         <v>2</v>
       </c>
-      <c r="L24" s="38"/>
+      <c r="L24" s="37"/>
       <c r="M24" s="19"/>
       <c r="N24" t="str">
         <f t="shared" si="38"/>
@@ -9761,12 +9908,12 @@
         <v/>
       </c>
       <c r="F25" s="19"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="37"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="35"/>
+      <c r="J25" s="36"/>
       <c r="K25" s="19"/>
-      <c r="L25" s="39"/>
+      <c r="L25" s="38"/>
       <c r="M25" s="19"/>
       <c r="N25" t="str">
         <f t="shared" ref="N25" si="122">IF(AND(H25="",I25=""),"",IF(H25="",0,2-H25)+IF(I25="",0,2-I25))</f>
@@ -10106,12 +10253,12 @@
         <v/>
       </c>
       <c r="F26" s="19"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="37"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="36"/>
       <c r="K26" s="19"/>
-      <c r="L26" s="38"/>
+      <c r="L26" s="37"/>
       <c r="M26" s="19"/>
       <c r="N26" t="str">
         <f t="shared" si="38"/>
@@ -10459,12 +10606,12 @@
       <c r="F27" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="G27" s="35"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="37"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="36"/>
       <c r="K27" s="19"/>
-      <c r="L27" s="38"/>
+      <c r="L27" s="37"/>
       <c r="M27" s="19"/>
       <c r="N27" t="str">
         <f t="shared" si="38"/>
@@ -10816,18 +10963,18 @@
       <c r="F28" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="G28" s="35">
+      <c r="G28" s="34">
         <v>6.1</v>
       </c>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="37">
+      <c r="H28" s="35"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="36">
         <v>1</v>
       </c>
       <c r="K28" s="19">
         <v>3</v>
       </c>
-      <c r="L28" s="38"/>
+      <c r="L28" s="37"/>
       <c r="M28" s="19"/>
       <c r="N28" t="str">
         <f t="shared" si="38"/>
@@ -11176,12 +11323,12 @@
         <v/>
       </c>
       <c r="F29" s="19"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="37"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="36"/>
       <c r="K29" s="19"/>
-      <c r="L29" s="38"/>
+      <c r="L29" s="37"/>
       <c r="M29" s="19"/>
       <c r="N29" t="str">
         <f t="shared" si="38"/>
@@ -11527,20 +11674,20 @@
       <c r="F30" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="G30" s="35">
+      <c r="G30" s="34">
         <v>6.1</v>
       </c>
-      <c r="H30" s="36">
+      <c r="H30" s="35">
         <v>0.5</v>
       </c>
-      <c r="I30" s="36"/>
-      <c r="J30" s="37">
+      <c r="I30" s="35"/>
+      <c r="J30" s="36">
         <v>1</v>
       </c>
       <c r="K30" s="19">
         <v>3</v>
       </c>
-      <c r="L30" s="38"/>
+      <c r="L30" s="37"/>
       <c r="M30" s="19"/>
       <c r="N30">
         <f t="shared" si="38"/>
@@ -11841,24 +11988,24 @@
       <c r="F31" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="G31" s="35">
+      <c r="G31" s="34">
         <v>6.2</v>
       </c>
-      <c r="H31" s="36">
+      <c r="H31" s="35">
         <f>IF(H30="","",H30)</f>
         <v>0.5</v>
       </c>
-      <c r="I31" s="36" t="str">
+      <c r="I31" s="35" t="str">
         <f>IF(I30="","",I30)</f>
         <v/>
       </c>
-      <c r="J31" s="37">
+      <c r="J31" s="36">
         <v>1</v>
       </c>
       <c r="K31" s="19">
         <v>3</v>
       </c>
-      <c r="L31" s="39"/>
+      <c r="L31" s="38"/>
       <c r="M31" s="19">
         <v>1</v>
       </c>
@@ -12101,12 +12248,12 @@
         <v/>
       </c>
       <c r="F32" s="19"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="37"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="36"/>
       <c r="K32" s="19"/>
-      <c r="L32" s="39"/>
+      <c r="L32" s="38"/>
       <c r="M32" s="19"/>
       <c r="N32" t="str">
         <f t="shared" si="38"/>
@@ -12333,18 +12480,18 @@
       <c r="F33" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="G33" s="35">
+      <c r="G33" s="34">
         <v>3.4</v>
       </c>
-      <c r="H33" s="36"/>
-      <c r="I33" s="36"/>
-      <c r="J33" s="37">
+      <c r="H33" s="35"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="36">
         <v>1</v>
       </c>
       <c r="K33" s="19">
         <v>3</v>
       </c>
-      <c r="L33" s="39">
+      <c r="L33" s="38">
         <v>8.9347017924020636E-5</v>
       </c>
       <c r="M33" s="19"/>
@@ -12569,24 +12716,24 @@
       <c r="F34" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G34" s="35">
+      <c r="G34" s="34">
         <v>3.1</v>
       </c>
-      <c r="H34" s="36" t="str">
+      <c r="H34" s="35" t="str">
         <f t="shared" ref="H34:I34" si="160">IF(H33="","",H33)</f>
         <v/>
       </c>
-      <c r="I34" s="36" t="str">
+      <c r="I34" s="35" t="str">
         <f t="shared" si="160"/>
         <v/>
       </c>
-      <c r="J34" s="37">
+      <c r="J34" s="36">
         <v>1</v>
       </c>
       <c r="K34" s="19">
         <v>3</v>
       </c>
-      <c r="L34" s="39">
+      <c r="L34" s="38">
         <v>1.7152242271898735E-5</v>
       </c>
       <c r="M34" s="19">
@@ -12820,24 +12967,24 @@
       <c r="F35" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="G35" s="35">
+      <c r="G35" s="34">
         <v>3.2</v>
       </c>
-      <c r="H35" s="36" t="str">
+      <c r="H35" s="35" t="str">
         <f t="shared" ref="H35:I35" si="192">IF(H34="","",H34)</f>
         <v/>
       </c>
-      <c r="I35" s="36" t="str">
+      <c r="I35" s="35" t="str">
         <f t="shared" si="192"/>
         <v/>
       </c>
-      <c r="J35" s="37">
+      <c r="J35" s="36">
         <v>1</v>
       </c>
       <c r="K35" s="19">
         <v>3</v>
       </c>
-      <c r="L35" s="39">
+      <c r="L35" s="38">
         <v>4.8959715407254328E-5</v>
       </c>
       <c r="M35" s="19">
@@ -13065,24 +13212,24 @@
       <c r="F36" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="G36" s="35">
+      <c r="G36" s="34">
         <v>3.3</v>
       </c>
-      <c r="H36" s="36" t="str">
+      <c r="H36" s="35" t="str">
         <f t="shared" ref="H36:I36" si="194">IF(H35="","",H35)</f>
         <v/>
       </c>
-      <c r="I36" s="36" t="str">
+      <c r="I36" s="35" t="str">
         <f t="shared" si="194"/>
         <v/>
       </c>
-      <c r="J36" s="37">
+      <c r="J36" s="36">
         <v>1</v>
       </c>
       <c r="K36" s="19">
         <v>3</v>
       </c>
-      <c r="L36" s="39">
+      <c r="L36" s="38">
         <v>2.973589319899093E-4</v>
       </c>
       <c r="M36" s="19">
@@ -13303,21 +13450,21 @@
       </c>
     </row>
     <row r="37" spans="2:93">
-      <c r="B37" s="42" t="s">
+      <c r="B37" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="C37" s="42"/>
+      <c r="C37" s="41"/>
       <c r="E37" s="4" t="str">
         <f t="shared" si="159"/>
         <v/>
       </c>
       <c r="F37" s="19"/>
-      <c r="G37" s="35"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="37"/>
+      <c r="G37" s="34"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="36"/>
       <c r="K37" s="19"/>
-      <c r="L37" s="38"/>
+      <c r="L37" s="37"/>
       <c r="M37" s="19"/>
       <c r="N37" t="str">
         <f t="shared" si="38"/>
@@ -13542,18 +13689,18 @@
       <c r="F38" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="G38" s="35">
+      <c r="G38" s="34">
         <v>4.0999999999999996</v>
       </c>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="37">
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="36">
         <v>0</v>
       </c>
       <c r="K38" s="19">
         <v>3</v>
       </c>
-      <c r="L38" s="38"/>
+      <c r="L38" s="37"/>
       <c r="M38" s="19"/>
       <c r="N38" t="str">
         <f t="shared" si="38"/>
@@ -13785,24 +13932,24 @@
       <c r="F39" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="G39" s="35">
+      <c r="G39" s="34">
         <v>4.2</v>
       </c>
-      <c r="H39" s="36" t="str">
+      <c r="H39" s="35" t="str">
         <f>IF(H38="","",H38)</f>
         <v/>
       </c>
-      <c r="I39" s="36" t="str">
+      <c r="I39" s="35" t="str">
         <f>IF(I38="","",I38)</f>
         <v/>
       </c>
-      <c r="J39" s="37">
+      <c r="J39" s="36">
         <v>0</v>
       </c>
       <c r="K39" s="19">
         <v>3</v>
       </c>
-      <c r="L39" s="38"/>
+      <c r="L39" s="37"/>
       <c r="M39" s="19">
         <v>1</v>
       </c>
@@ -14012,24 +14159,24 @@
       <c r="F40" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="G40" s="35">
+      <c r="G40" s="34">
         <v>4.3</v>
       </c>
-      <c r="H40" s="36" t="str">
+      <c r="H40" s="35" t="str">
         <f>IF(H39="","",H39)</f>
         <v/>
       </c>
-      <c r="I40" s="36" t="str">
+      <c r="I40" s="35" t="str">
         <f>IF(I39="","",I39)</f>
         <v/>
       </c>
-      <c r="J40" s="37">
+      <c r="J40" s="36">
         <v>0</v>
       </c>
       <c r="K40" s="19">
         <v>3</v>
       </c>
-      <c r="L40" s="38"/>
+      <c r="L40" s="37"/>
       <c r="M40" s="19">
         <v>1</v>
       </c>
@@ -14248,12 +14395,12 @@
         <v/>
       </c>
       <c r="F41" s="19"/>
-      <c r="G41" s="35"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="37"/>
+      <c r="G41" s="34"/>
+      <c r="H41" s="35"/>
+      <c r="I41" s="35"/>
+      <c r="J41" s="36"/>
       <c r="K41" s="19"/>
-      <c r="L41" s="38"/>
+      <c r="L41" s="37"/>
       <c r="M41" s="19"/>
       <c r="N41" t="str">
         <f t="shared" si="38"/>
@@ -14469,16 +14616,16 @@
       <c r="F42" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="G42" s="35">
+      <c r="G42" s="34">
         <v>210</v>
       </c>
-      <c r="H42" s="36"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="37"/>
+      <c r="H42" s="35"/>
+      <c r="I42" s="35"/>
+      <c r="J42" s="36"/>
       <c r="K42" s="19">
         <v>3</v>
       </c>
-      <c r="L42" s="38"/>
+      <c r="L42" s="37"/>
       <c r="M42" s="19"/>
       <c r="N42" t="str">
         <f t="shared" si="38"/>
@@ -14648,16 +14795,16 @@
       <c r="F43" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="G43" s="35">
+      <c r="G43" s="34">
         <v>201</v>
       </c>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="37"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="36"/>
       <c r="K43" s="19">
         <v>3</v>
       </c>
-      <c r="L43" s="38"/>
+      <c r="L43" s="37"/>
       <c r="M43" s="19"/>
       <c r="N43" t="str">
         <f t="shared" si="38"/>
@@ -14833,16 +14980,16 @@
       <c r="F44" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="G44" s="35">
+      <c r="G44" s="34">
         <v>202</v>
       </c>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="37"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="36"/>
       <c r="K44" s="19">
         <v>3</v>
       </c>
-      <c r="L44" s="38"/>
+      <c r="L44" s="37"/>
       <c r="M44" s="19"/>
       <c r="N44" t="str">
         <f t="shared" si="38"/>
@@ -15018,16 +15165,16 @@
       <c r="F45" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="G45" s="35">
+      <c r="G45" s="34">
         <v>203</v>
       </c>
-      <c r="H45" s="36"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="37"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="36"/>
       <c r="K45" s="19">
         <v>3</v>
       </c>
-      <c r="L45" s="38"/>
+      <c r="L45" s="37"/>
       <c r="M45" s="19"/>
       <c r="N45" t="str">
         <f t="shared" si="38"/>
@@ -15210,16 +15357,16 @@
       <c r="F46" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="G46" s="35">
+      <c r="G46" s="34">
         <v>204</v>
       </c>
-      <c r="H46" s="36"/>
-      <c r="I46" s="36"/>
-      <c r="J46" s="37"/>
+      <c r="H46" s="35"/>
+      <c r="I46" s="35"/>
+      <c r="J46" s="36"/>
       <c r="K46" s="19">
         <v>3</v>
       </c>
-      <c r="L46" s="38"/>
+      <c r="L46" s="37"/>
       <c r="M46" s="19"/>
       <c r="N46" t="str">
         <f t="shared" si="38"/>
@@ -15402,16 +15549,16 @@
       <c r="F47" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="G47" s="35">
+      <c r="G47" s="34">
         <v>201</v>
       </c>
-      <c r="H47" s="36"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="37"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="35"/>
+      <c r="J47" s="36"/>
       <c r="K47" s="19">
         <v>3</v>
       </c>
-      <c r="L47" s="38"/>
+      <c r="L47" s="37"/>
       <c r="M47" s="19"/>
       <c r="N47" t="str">
         <f t="shared" si="38"/>
@@ -15594,16 +15741,16 @@
       <c r="F48" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="G48" s="35">
+      <c r="G48" s="34">
         <v>202</v>
       </c>
-      <c r="H48" s="36"/>
-      <c r="I48" s="36"/>
-      <c r="J48" s="37"/>
+      <c r="H48" s="35"/>
+      <c r="I48" s="35"/>
+      <c r="J48" s="36"/>
       <c r="K48" s="19">
         <v>3</v>
       </c>
-      <c r="L48" s="38"/>
+      <c r="L48" s="37"/>
       <c r="M48" s="19"/>
       <c r="N48" t="str">
         <f t="shared" si="38"/>
@@ -15796,16 +15943,16 @@
       <c r="F49" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="G49" s="35">
+      <c r="G49" s="34">
         <v>203</v>
       </c>
-      <c r="H49" s="36"/>
-      <c r="I49" s="36"/>
-      <c r="J49" s="37"/>
+      <c r="H49" s="35"/>
+      <c r="I49" s="35"/>
+      <c r="J49" s="36"/>
       <c r="K49" s="19">
         <v>3</v>
       </c>
-      <c r="L49" s="38"/>
+      <c r="L49" s="37"/>
       <c r="M49" s="19"/>
       <c r="N49" t="str">
         <f t="shared" si="38"/>
@@ -15968,16 +16115,16 @@
       <c r="F50" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="G50" s="35">
+      <c r="G50" s="34">
         <v>204</v>
       </c>
-      <c r="H50" s="36"/>
-      <c r="I50" s="36"/>
-      <c r="J50" s="37"/>
+      <c r="H50" s="35"/>
+      <c r="I50" s="35"/>
+      <c r="J50" s="36"/>
       <c r="K50" s="19">
         <v>3</v>
       </c>
-      <c r="L50" s="38"/>
+      <c r="L50" s="37"/>
       <c r="M50" s="19"/>
       <c r="N50" t="str">
         <f t="shared" si="38"/>
@@ -16144,12 +16291,12 @@
         <v/>
       </c>
       <c r="F51" s="19"/>
-      <c r="G51" s="35"/>
-      <c r="H51" s="36"/>
-      <c r="I51" s="36"/>
-      <c r="J51" s="37"/>
+      <c r="G51" s="34"/>
+      <c r="H51" s="35"/>
+      <c r="I51" s="35"/>
+      <c r="J51" s="36"/>
       <c r="K51" s="19"/>
-      <c r="L51" s="38"/>
+      <c r="L51" s="37"/>
       <c r="M51" s="19"/>
       <c r="N51" t="str">
         <f t="shared" si="38"/>
@@ -16329,12 +16476,12 @@
         <v/>
       </c>
       <c r="F52" s="19"/>
-      <c r="G52" s="35"/>
-      <c r="H52" s="36"/>
-      <c r="I52" s="36"/>
-      <c r="J52" s="37"/>
+      <c r="G52" s="34"/>
+      <c r="H52" s="35"/>
+      <c r="I52" s="35"/>
+      <c r="J52" s="36"/>
       <c r="K52" s="19"/>
-      <c r="L52" s="38"/>
+      <c r="L52" s="37"/>
       <c r="M52" s="19"/>
       <c r="N52" t="str">
         <f t="shared" si="38"/>
@@ -16512,12 +16659,12 @@
         <v/>
       </c>
       <c r="F53" s="19"/>
-      <c r="G53" s="35"/>
-      <c r="H53" s="36"/>
-      <c r="I53" s="36"/>
-      <c r="J53" s="37"/>
+      <c r="G53" s="34"/>
+      <c r="H53" s="35"/>
+      <c r="I53" s="35"/>
+      <c r="J53" s="36"/>
       <c r="K53" s="19"/>
-      <c r="L53" s="38"/>
+      <c r="L53" s="37"/>
       <c r="M53" s="19"/>
       <c r="N53" t="str">
         <f t="shared" si="38"/>
@@ -16690,21 +16837,21 @@
       <c r="BK53" s="19"/>
     </row>
     <row r="54" spans="1:63">
-      <c r="B54" s="42" t="s">
+      <c r="B54" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="C54" s="42"/>
+      <c r="C54" s="41"/>
       <c r="E54" s="4" t="str">
         <f t="shared" si="159"/>
         <v/>
       </c>
       <c r="F54" s="19"/>
-      <c r="G54" s="35"/>
-      <c r="H54" s="36"/>
-      <c r="I54" s="36"/>
-      <c r="J54" s="37"/>
+      <c r="G54" s="34"/>
+      <c r="H54" s="35"/>
+      <c r="I54" s="35"/>
+      <c r="J54" s="36"/>
       <c r="K54" s="19"/>
-      <c r="L54" s="38"/>
+      <c r="L54" s="37"/>
       <c r="M54" s="19"/>
       <c r="N54" t="str">
         <f t="shared" si="38"/>
@@ -16884,12 +17031,12 @@
       <c r="F55" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="G55" s="35"/>
-      <c r="H55" s="36"/>
-      <c r="I55" s="36"/>
-      <c r="J55" s="37"/>
+      <c r="G55" s="34"/>
+      <c r="H55" s="35"/>
+      <c r="I55" s="35"/>
+      <c r="J55" s="36"/>
       <c r="K55" s="19"/>
-      <c r="L55" s="38"/>
+      <c r="L55" s="37"/>
       <c r="M55" s="19"/>
       <c r="N55" t="str">
         <f t="shared" si="38"/>
@@ -17068,20 +17215,20 @@
       <c r="F56" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="G56" s="35">
-        <v>0</v>
-      </c>
-      <c r="H56" s="36">
+      <c r="G56" s="34">
+        <v>0</v>
+      </c>
+      <c r="H56" s="35">
         <v>0.2</v>
       </c>
-      <c r="I56" s="36"/>
-      <c r="J56" s="37">
+      <c r="I56" s="35"/>
+      <c r="J56" s="36">
         <v>1</v>
       </c>
       <c r="K56" s="19">
         <v>4</v>
       </c>
-      <c r="L56" s="38"/>
+      <c r="L56" s="37"/>
       <c r="M56" s="19"/>
       <c r="N56">
         <f t="shared" si="38"/>
@@ -17248,12 +17395,12 @@
         <v/>
       </c>
       <c r="F57" s="19"/>
-      <c r="G57" s="35"/>
-      <c r="H57" s="36"/>
-      <c r="I57" s="36"/>
-      <c r="J57" s="37"/>
+      <c r="G57" s="34"/>
+      <c r="H57" s="35"/>
+      <c r="I57" s="35"/>
+      <c r="J57" s="36"/>
       <c r="K57" s="19"/>
-      <c r="L57" s="38"/>
+      <c r="L57" s="37"/>
       <c r="M57" s="19"/>
       <c r="N57" t="str">
         <f t="shared" si="38"/>
@@ -17416,7 +17563,7 @@
       <c r="B58" t="s">
         <v>199</v>
       </c>
-      <c r="C58" s="28">
+      <c r="C58" s="27">
         <f ca="1">-(SUMIF(G:G,"&lt;&gt;7,1",AM:AM)+SUMIFS(O:O,M:M,"",G:G,7.1)*LOOKUP(100,BO:BO,CM:CM))/LOOKUP(7.1,BO:BO,CM:CM)</f>
         <v>2.6329824041168326E-18</v>
       </c>
@@ -17428,18 +17575,18 @@
       <c r="F58" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="G58" s="35">
+      <c r="G58" s="34">
         <v>7.4</v>
       </c>
-      <c r="H58" s="36"/>
-      <c r="I58" s="36"/>
-      <c r="J58" s="37">
+      <c r="H58" s="35"/>
+      <c r="I58" s="35"/>
+      <c r="J58" s="36">
         <v>1</v>
       </c>
       <c r="K58" s="19">
         <v>4</v>
       </c>
-      <c r="L58" s="40">
+      <c r="L58" s="39">
         <v>4.5936507936507942E-2</v>
       </c>
       <c r="M58" s="19"/>
@@ -17621,7 +17768,7 @@
       <c r="B59" t="s">
         <v>200</v>
       </c>
-      <c r="C59" s="28">
+      <c r="C59" s="27">
         <f ca="1">-(SUMIF(G:G,"&lt;&gt;7,4",AM:AM)+SUMIFS(O:O,M:M,"",G:G,7.4)*LOOKUP(100,BO:BO,CM:CM))/LOOKUP(7.4,BO:BO,CM:CM)</f>
         <v>4.5936507936507942E-2</v>
       </c>
@@ -17632,24 +17779,24 @@
       <c r="F59" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="G59" s="35">
+      <c r="G59" s="34">
         <v>7.5</v>
       </c>
-      <c r="H59" s="36" t="str">
+      <c r="H59" s="35" t="str">
         <f>IF(H58="","",H58)</f>
         <v/>
       </c>
-      <c r="I59" s="36" t="str">
+      <c r="I59" s="35" t="str">
         <f>IF(I58="","",I58)</f>
         <v/>
       </c>
-      <c r="J59" s="37">
+      <c r="J59" s="36">
         <v>1</v>
       </c>
       <c r="K59" s="19">
         <v>4</v>
       </c>
-      <c r="L59" s="38"/>
+      <c r="L59" s="37"/>
       <c r="M59" s="19">
         <v>1</v>
       </c>
@@ -17831,7 +17978,7 @@
       <c r="B60" t="s">
         <v>144</v>
       </c>
-      <c r="C60" s="41">
+      <c r="C60" s="40">
         <f ca="1">-(SUMIF(G:G,"&lt;&gt;3,4",AF:AF))/LOOKUP(3.4,BO:BO,CF:CF)*(1+$C$57)</f>
         <v>8.9347017924025867E-5</v>
       </c>
@@ -17842,24 +17989,24 @@
       <c r="F60" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="G60" s="35">
+      <c r="G60" s="34">
         <v>7.6</v>
       </c>
-      <c r="H60" s="36" t="str">
+      <c r="H60" s="35" t="str">
         <f>IF(H59="","",H59)</f>
         <v/>
       </c>
-      <c r="I60" s="36" t="str">
+      <c r="I60" s="35" t="str">
         <f>IF(I59="","",I59)</f>
         <v/>
       </c>
-      <c r="J60" s="37">
+      <c r="J60" s="36">
         <v>0</v>
       </c>
       <c r="K60" s="19">
         <v>4</v>
       </c>
-      <c r="L60" s="38"/>
+      <c r="L60" s="37"/>
       <c r="M60" s="19">
         <v>1</v>
       </c>
@@ -18035,7 +18182,7 @@
       <c r="B61" t="s">
         <v>146</v>
       </c>
-      <c r="C61" s="41">
+      <c r="C61" s="40">
         <f ca="1">-(SUMIF(G:G,"&lt;&gt;3,1",AC:AC))/LOOKUP(3.1,BO:BO,CC:CC)*(1+$C$57)</f>
         <v>1.7152242271900188E-5</v>
       </c>
@@ -18044,12 +18191,12 @@
         <v/>
       </c>
       <c r="F61" s="19"/>
-      <c r="G61" s="35"/>
-      <c r="H61" s="36"/>
-      <c r="I61" s="36"/>
-      <c r="J61" s="37"/>
+      <c r="G61" s="34"/>
+      <c r="H61" s="35"/>
+      <c r="I61" s="35"/>
+      <c r="J61" s="36"/>
       <c r="K61" s="19"/>
-      <c r="L61" s="38"/>
+      <c r="L61" s="37"/>
       <c r="M61" s="19"/>
       <c r="N61" t="str">
         <f t="shared" si="38"/>
@@ -18227,7 +18374,7 @@
       <c r="B62" t="s">
         <v>147</v>
       </c>
-      <c r="C62" s="41">
+      <c r="C62" s="40">
         <f ca="1">-(SUMIF(G:G,"&lt;&gt;3,2",AD:AD))/LOOKUP(3.2,BO:BO,CD:CD)*(1+$C$57)</f>
         <v>4.8959715407257384E-5</v>
       </c>
@@ -18238,18 +18385,18 @@
       <c r="F62" s="19" t="s">
         <v>203</v>
       </c>
-      <c r="G62" s="35">
+      <c r="G62" s="34">
         <v>8.3000000000000007</v>
       </c>
-      <c r="H62" s="36"/>
-      <c r="I62" s="36"/>
-      <c r="J62" s="37">
+      <c r="H62" s="35"/>
+      <c r="I62" s="35"/>
+      <c r="J62" s="36">
         <v>1</v>
       </c>
       <c r="K62" s="19">
         <v>4</v>
       </c>
-      <c r="L62" s="38"/>
+      <c r="L62" s="37"/>
       <c r="M62" s="19"/>
       <c r="N62" t="str">
         <f t="shared" si="38"/>
@@ -18429,7 +18576,7 @@
       <c r="B63" t="s">
         <v>148</v>
       </c>
-      <c r="C63" s="41">
+      <c r="C63" s="40">
         <f ca="1">-(SUMIF(G:G,"&lt;&gt;3,3",AE:AE))/LOOKUP(3.3,BO:BO,CE:CE)*(1+$C$57)</f>
         <v>2.9735893198991413E-4</v>
       </c>
@@ -18440,24 +18587,24 @@
       <c r="F63" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="G63" s="35">
+      <c r="G63" s="34">
         <v>8.4</v>
       </c>
-      <c r="H63" s="36" t="str">
+      <c r="H63" s="35" t="str">
         <f>IF(H62="","",H62)</f>
         <v/>
       </c>
-      <c r="I63" s="36" t="str">
+      <c r="I63" s="35" t="str">
         <f>IF(I62="","",I62)</f>
         <v/>
       </c>
-      <c r="J63" s="37">
+      <c r="J63" s="36">
         <v>1</v>
       </c>
       <c r="K63" s="19">
         <v>4</v>
       </c>
-      <c r="L63" s="38"/>
+      <c r="L63" s="37"/>
       <c r="M63" s="19">
         <v>1</v>
       </c>
@@ -18639,12 +18786,12 @@
         <v/>
       </c>
       <c r="F64" s="19"/>
-      <c r="G64" s="35"/>
-      <c r="H64" s="36"/>
-      <c r="I64" s="36"/>
-      <c r="J64" s="37"/>
+      <c r="G64" s="34"/>
+      <c r="H64" s="35"/>
+      <c r="I64" s="35"/>
+      <c r="J64" s="36"/>
       <c r="K64" s="19"/>
-      <c r="L64" s="38"/>
+      <c r="L64" s="37"/>
       <c r="M64" s="19"/>
       <c r="N64" t="str">
         <f t="shared" si="38"/>
@@ -18799,7 +18946,7 @@
         <v/>
       </c>
       <c r="BA64" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="BB64" s="19"/>
       <c r="BC64" s="19"/>
@@ -18818,7 +18965,7 @@
       <c r="B65" t="s">
         <v>104</v>
       </c>
-      <c r="C65" s="27">
+      <c r="C65" s="26">
         <f ca="1">$C$39/C75</f>
         <v>40656.927775221848</v>
       </c>
@@ -18829,16 +18976,16 @@
       <c r="F65" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="G65" s="35">
+      <c r="G65" s="34">
         <v>210</v>
       </c>
-      <c r="H65" s="36"/>
-      <c r="I65" s="36"/>
-      <c r="J65" s="37"/>
+      <c r="H65" s="35"/>
+      <c r="I65" s="35"/>
+      <c r="J65" s="36"/>
       <c r="K65" s="19">
         <v>4</v>
       </c>
-      <c r="L65" s="38"/>
+      <c r="L65" s="37"/>
       <c r="M65" s="19"/>
       <c r="N65" t="str">
         <f t="shared" si="38"/>
@@ -19018,7 +19165,7 @@
       <c r="B66" t="s">
         <v>105</v>
       </c>
-      <c r="C66" s="27">
+      <c r="C66" s="26">
         <f ca="1">$C$39/C76</f>
         <v>49093.258252002233</v>
       </c>
@@ -19029,16 +19176,16 @@
       <c r="F66" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="G66" s="35">
+      <c r="G66" s="34">
         <v>200</v>
       </c>
-      <c r="H66" s="36"/>
-      <c r="I66" s="36"/>
-      <c r="J66" s="37"/>
+      <c r="H66" s="35"/>
+      <c r="I66" s="35"/>
+      <c r="J66" s="36"/>
       <c r="K66" s="19">
         <v>4</v>
       </c>
-      <c r="L66" s="38"/>
+      <c r="L66" s="37"/>
       <c r="M66" s="19"/>
       <c r="N66" t="str">
         <f t="shared" si="38"/>
@@ -19197,7 +19344,7 @@
       <c r="B67" t="s">
         <v>106</v>
       </c>
-      <c r="C67" s="27">
+      <c r="C67" s="26">
         <f ca="1">$C$39/C77</f>
         <v>59170.997334388419</v>
       </c>
@@ -19206,12 +19353,12 @@
         <v/>
       </c>
       <c r="F67" s="19"/>
-      <c r="G67" s="35"/>
-      <c r="H67" s="36"/>
-      <c r="I67" s="36"/>
-      <c r="J67" s="37"/>
+      <c r="G67" s="34"/>
+      <c r="H67" s="35"/>
+      <c r="I67" s="35"/>
+      <c r="J67" s="36"/>
       <c r="K67" s="19"/>
-      <c r="L67" s="38"/>
+      <c r="L67" s="37"/>
       <c r="M67" s="19"/>
       <c r="N67" t="str">
         <f t="shared" ref="N67:N120" si="244">IF(AND(H67="",I67=""),"",IF(H67="",0,2-H67)+IF(I67="",0,2-I67))</f>
@@ -19373,7 +19520,7 @@
       <c r="B68" t="s">
         <v>107</v>
       </c>
-      <c r="C68" s="27">
+      <c r="C68" s="26">
         <f ca="1">$C$39/C78</f>
         <v>124529.40342449186</v>
       </c>
@@ -19382,12 +19529,12 @@
         <v/>
       </c>
       <c r="F68" s="19"/>
-      <c r="G68" s="35"/>
-      <c r="H68" s="36"/>
-      <c r="I68" s="36"/>
-      <c r="J68" s="37"/>
+      <c r="G68" s="34"/>
+      <c r="H68" s="35"/>
+      <c r="I68" s="35"/>
+      <c r="J68" s="36"/>
       <c r="K68" s="19"/>
-      <c r="L68" s="38"/>
+      <c r="L68" s="37"/>
       <c r="M68" s="19"/>
       <c r="N68" t="str">
         <f t="shared" si="244"/>
@@ -19548,14 +19695,14 @@
         <v/>
       </c>
       <c r="F69" s="19" t="s">
-        <v>222</v>
-      </c>
-      <c r="G69" s="35"/>
-      <c r="H69" s="36"/>
-      <c r="I69" s="36"/>
-      <c r="J69" s="37"/>
+        <v>221</v>
+      </c>
+      <c r="G69" s="34"/>
+      <c r="H69" s="35"/>
+      <c r="I69" s="35"/>
+      <c r="J69" s="36"/>
       <c r="K69" s="19"/>
-      <c r="L69" s="38"/>
+      <c r="L69" s="37"/>
       <c r="M69" s="19"/>
       <c r="N69" t="str">
         <f t="shared" si="244"/>
@@ -19731,16 +19878,16 @@
       <c r="F70" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="G70" s="35">
+      <c r="G70" s="34">
         <v>210</v>
       </c>
-      <c r="H70" s="36"/>
-      <c r="I70" s="36"/>
-      <c r="J70" s="37"/>
+      <c r="H70" s="35"/>
+      <c r="I70" s="35"/>
+      <c r="J70" s="36"/>
       <c r="K70" s="19">
         <v>5</v>
       </c>
-      <c r="L70" s="38"/>
+      <c r="L70" s="37"/>
       <c r="M70" s="19"/>
       <c r="N70" t="str">
         <f t="shared" si="244"/>
@@ -19953,16 +20100,16 @@
       <c r="F71" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="G71" s="35">
+      <c r="G71" s="34">
         <v>200</v>
       </c>
-      <c r="H71" s="36"/>
-      <c r="I71" s="36"/>
-      <c r="J71" s="37"/>
+      <c r="H71" s="35"/>
+      <c r="I71" s="35"/>
+      <c r="J71" s="36"/>
       <c r="K71" s="19">
         <v>5</v>
       </c>
-      <c r="L71" s="38"/>
+      <c r="L71" s="37"/>
       <c r="M71" s="19"/>
       <c r="N71" t="str">
         <f t="shared" si="244"/>
@@ -20175,16 +20322,16 @@
       <c r="F72" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="G72" s="35">
+      <c r="G72" s="34">
         <v>200</v>
       </c>
-      <c r="H72" s="36"/>
-      <c r="I72" s="36"/>
-      <c r="J72" s="37"/>
+      <c r="H72" s="35"/>
+      <c r="I72" s="35"/>
+      <c r="J72" s="36"/>
       <c r="K72" s="19">
         <v>5</v>
       </c>
-      <c r="L72" s="38"/>
+      <c r="L72" s="37"/>
       <c r="M72" s="19"/>
       <c r="N72" t="str">
         <f t="shared" si="244"/>
@@ -20397,12 +20544,12 @@
       <c r="F73" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="G73" s="35"/>
-      <c r="H73" s="36"/>
-      <c r="I73" s="36"/>
-      <c r="J73" s="37"/>
+      <c r="G73" s="34"/>
+      <c r="H73" s="35"/>
+      <c r="I73" s="35"/>
+      <c r="J73" s="36"/>
       <c r="K73" s="19"/>
-      <c r="L73" s="38"/>
+      <c r="L73" s="37"/>
       <c r="M73" s="19"/>
       <c r="N73" t="str">
         <f t="shared" si="244"/>
@@ -20608,12 +20755,12 @@
       <c r="F74" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="G74" s="35"/>
-      <c r="H74" s="36"/>
-      <c r="I74" s="36"/>
-      <c r="J74" s="37"/>
+      <c r="G74" s="34"/>
+      <c r="H74" s="35"/>
+      <c r="I74" s="35"/>
+      <c r="J74" s="36"/>
       <c r="K74" s="19"/>
-      <c r="L74" s="38"/>
+      <c r="L74" s="37"/>
       <c r="M74" s="19"/>
       <c r="N74" t="str">
         <f t="shared" si="244"/>
@@ -20826,12 +20973,12 @@
       <c r="F75" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="G75" s="35"/>
-      <c r="H75" s="36"/>
-      <c r="I75" s="36"/>
-      <c r="J75" s="37"/>
+      <c r="G75" s="34"/>
+      <c r="H75" s="35"/>
+      <c r="I75" s="35"/>
+      <c r="J75" s="36"/>
       <c r="K75" s="19"/>
-      <c r="L75" s="38"/>
+      <c r="L75" s="37"/>
       <c r="M75" s="19"/>
       <c r="N75" t="str">
         <f t="shared" si="244"/>
@@ -21001,16 +21148,16 @@
       <c r="F76" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="G76" s="35">
+      <c r="G76" s="34">
         <v>201</v>
       </c>
-      <c r="H76" s="36"/>
-      <c r="I76" s="36"/>
-      <c r="J76" s="37"/>
+      <c r="H76" s="35"/>
+      <c r="I76" s="35"/>
+      <c r="J76" s="36"/>
       <c r="K76" s="19">
         <v>5</v>
       </c>
-      <c r="L76" s="38"/>
+      <c r="L76" s="37"/>
       <c r="M76" s="19"/>
       <c r="N76" t="str">
         <f t="shared" si="244"/>
@@ -21183,16 +21330,16 @@
       <c r="F77" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="G77" s="35">
+      <c r="G77" s="34">
         <v>202</v>
       </c>
-      <c r="H77" s="36"/>
-      <c r="I77" s="36"/>
-      <c r="J77" s="37"/>
+      <c r="H77" s="35"/>
+      <c r="I77" s="35"/>
+      <c r="J77" s="36"/>
       <c r="K77" s="19">
         <v>5</v>
       </c>
-      <c r="L77" s="38"/>
+      <c r="L77" s="37"/>
       <c r="M77" s="19"/>
       <c r="N77" t="str">
         <f t="shared" si="244"/>
@@ -21405,16 +21552,16 @@
       <c r="F78" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="G78" s="35">
+      <c r="G78" s="34">
         <v>203</v>
       </c>
-      <c r="H78" s="36"/>
-      <c r="I78" s="36"/>
-      <c r="J78" s="37"/>
+      <c r="H78" s="35"/>
+      <c r="I78" s="35"/>
+      <c r="J78" s="36"/>
       <c r="K78" s="19">
         <v>5</v>
       </c>
-      <c r="L78" s="38"/>
+      <c r="L78" s="37"/>
       <c r="M78" s="19"/>
       <c r="N78" t="str">
         <f t="shared" si="244"/>
@@ -21620,16 +21767,16 @@
       <c r="F79" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="G79" s="35">
+      <c r="G79" s="34">
         <v>204</v>
       </c>
-      <c r="H79" s="36"/>
-      <c r="I79" s="36"/>
-      <c r="J79" s="37"/>
+      <c r="H79" s="35"/>
+      <c r="I79" s="35"/>
+      <c r="J79" s="36"/>
       <c r="K79" s="19">
         <v>5</v>
       </c>
-      <c r="L79" s="38"/>
+      <c r="L79" s="37"/>
       <c r="M79" s="19"/>
       <c r="N79" t="str">
         <f t="shared" si="244"/>
@@ -21829,7 +21976,7 @@
     </row>
     <row r="80" spans="2:63">
       <c r="B80" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C80" s="10">
         <f ca="1">SUMIF(U:U,"&lt;0")*60*60*6</f>
@@ -21840,12 +21987,12 @@
         <v/>
       </c>
       <c r="F80" s="19"/>
-      <c r="G80" s="35"/>
-      <c r="H80" s="36"/>
-      <c r="I80" s="36"/>
-      <c r="J80" s="37"/>
+      <c r="G80" s="34"/>
+      <c r="H80" s="35"/>
+      <c r="I80" s="35"/>
+      <c r="J80" s="36"/>
       <c r="K80" s="19"/>
-      <c r="L80" s="38"/>
+      <c r="L80" s="37"/>
       <c r="M80" s="19"/>
       <c r="N80" t="str">
         <f t="shared" si="244"/>
@@ -22045,7 +22192,7 @@
     </row>
     <row r="81" spans="2:63">
       <c r="B81" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C81" s="10">
         <f ca="1">SUMIF(V:V,"&lt;0")*60*60*6</f>
@@ -22056,12 +22203,12 @@
         <v/>
       </c>
       <c r="F81" s="19"/>
-      <c r="G81" s="35"/>
-      <c r="H81" s="36"/>
-      <c r="I81" s="36"/>
-      <c r="J81" s="37"/>
+      <c r="G81" s="34"/>
+      <c r="H81" s="35"/>
+      <c r="I81" s="35"/>
+      <c r="J81" s="36"/>
       <c r="K81" s="19"/>
-      <c r="L81" s="38"/>
+      <c r="L81" s="37"/>
       <c r="M81" s="19"/>
       <c r="N81" t="str">
         <f t="shared" si="244"/>
@@ -22261,7 +22408,7 @@
     </row>
     <row r="82" spans="2:63">
       <c r="B82" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C82" s="10">
         <f ca="1">SUMIF(W:W,"&lt;0")*60*60*6</f>
@@ -22272,12 +22419,12 @@
         <v/>
       </c>
       <c r="F82" s="19"/>
-      <c r="G82" s="35"/>
-      <c r="H82" s="36"/>
-      <c r="I82" s="36"/>
-      <c r="J82" s="37"/>
+      <c r="G82" s="34"/>
+      <c r="H82" s="35"/>
+      <c r="I82" s="35"/>
+      <c r="J82" s="36"/>
       <c r="K82" s="19"/>
-      <c r="L82" s="38"/>
+      <c r="L82" s="37"/>
       <c r="M82" s="19"/>
       <c r="N82" t="str">
         <f t="shared" si="244"/>
@@ -22434,7 +22581,7 @@
     </row>
     <row r="83" spans="2:63">
       <c r="B83" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C83" s="10">
         <f ca="1">SUMIF(AJ:AJ,"&lt;0")*60*60*6</f>
@@ -22445,12 +22592,12 @@
         <v/>
       </c>
       <c r="F83" s="19"/>
-      <c r="G83" s="35"/>
-      <c r="H83" s="36"/>
-      <c r="I83" s="36"/>
-      <c r="J83" s="37"/>
+      <c r="G83" s="34"/>
+      <c r="H83" s="35"/>
+      <c r="I83" s="35"/>
+      <c r="J83" s="36"/>
       <c r="K83" s="19"/>
-      <c r="L83" s="38"/>
+      <c r="L83" s="37"/>
       <c r="M83" s="19"/>
       <c r="N83" t="str">
         <f t="shared" si="244"/>
@@ -22611,12 +22758,12 @@
         <v/>
       </c>
       <c r="F84" s="19"/>
-      <c r="G84" s="35"/>
-      <c r="H84" s="36"/>
-      <c r="I84" s="36"/>
-      <c r="J84" s="37"/>
+      <c r="G84" s="34"/>
+      <c r="H84" s="35"/>
+      <c r="I84" s="35"/>
+      <c r="J84" s="36"/>
       <c r="K84" s="19"/>
-      <c r="L84" s="38"/>
+      <c r="L84" s="37"/>
       <c r="M84" s="19"/>
       <c r="N84" t="str">
         <f t="shared" si="244"/>
@@ -22777,12 +22924,12 @@
         <v/>
       </c>
       <c r="F85" s="19"/>
-      <c r="G85" s="35"/>
-      <c r="H85" s="36"/>
-      <c r="I85" s="36"/>
-      <c r="J85" s="37"/>
+      <c r="G85" s="34"/>
+      <c r="H85" s="35"/>
+      <c r="I85" s="35"/>
+      <c r="J85" s="36"/>
       <c r="K85" s="19"/>
-      <c r="L85" s="38"/>
+      <c r="L85" s="37"/>
       <c r="M85" s="19"/>
       <c r="N85" t="str">
         <f t="shared" si="244"/>
@@ -22943,12 +23090,12 @@
         <v/>
       </c>
       <c r="F86" s="19"/>
-      <c r="G86" s="35"/>
-      <c r="H86" s="36"/>
-      <c r="I86" s="36"/>
-      <c r="J86" s="37"/>
+      <c r="G86" s="34"/>
+      <c r="H86" s="35"/>
+      <c r="I86" s="35"/>
+      <c r="J86" s="36"/>
       <c r="K86" s="19"/>
-      <c r="L86" s="38"/>
+      <c r="L86" s="37"/>
       <c r="M86" s="19"/>
       <c r="N86" t="str">
         <f t="shared" si="244"/>
@@ -23109,12 +23256,12 @@
         <v/>
       </c>
       <c r="F87" s="19"/>
-      <c r="G87" s="35"/>
-      <c r="H87" s="36"/>
-      <c r="I87" s="36"/>
-      <c r="J87" s="37"/>
+      <c r="G87" s="34"/>
+      <c r="H87" s="35"/>
+      <c r="I87" s="35"/>
+      <c r="J87" s="36"/>
       <c r="K87" s="19"/>
-      <c r="L87" s="38"/>
+      <c r="L87" s="37"/>
       <c r="M87" s="19"/>
       <c r="N87" t="str">
         <f t="shared" si="244"/>
@@ -23275,12 +23422,12 @@
         <v/>
       </c>
       <c r="F88" s="19"/>
-      <c r="G88" s="35"/>
-      <c r="H88" s="36"/>
-      <c r="I88" s="36"/>
-      <c r="J88" s="37"/>
+      <c r="G88" s="34"/>
+      <c r="H88" s="35"/>
+      <c r="I88" s="35"/>
+      <c r="J88" s="36"/>
       <c r="K88" s="19"/>
-      <c r="L88" s="38"/>
+      <c r="L88" s="37"/>
       <c r="M88" s="19"/>
       <c r="N88" t="str">
         <f t="shared" si="244"/>
@@ -23441,12 +23588,12 @@
         <v/>
       </c>
       <c r="F89" s="19"/>
-      <c r="G89" s="35"/>
-      <c r="H89" s="36"/>
-      <c r="I89" s="36"/>
-      <c r="J89" s="37"/>
+      <c r="G89" s="34"/>
+      <c r="H89" s="35"/>
+      <c r="I89" s="35"/>
+      <c r="J89" s="36"/>
       <c r="K89" s="19"/>
-      <c r="L89" s="38"/>
+      <c r="L89" s="37"/>
       <c r="M89" s="19"/>
       <c r="N89" t="str">
         <f t="shared" si="244"/>
@@ -23607,12 +23754,12 @@
         <v/>
       </c>
       <c r="F90" s="19"/>
-      <c r="G90" s="35"/>
-      <c r="H90" s="36"/>
-      <c r="I90" s="36"/>
-      <c r="J90" s="37"/>
+      <c r="G90" s="34"/>
+      <c r="H90" s="35"/>
+      <c r="I90" s="35"/>
+      <c r="J90" s="36"/>
       <c r="K90" s="19"/>
-      <c r="L90" s="38"/>
+      <c r="L90" s="37"/>
       <c r="M90" s="19"/>
       <c r="N90" t="str">
         <f t="shared" si="244"/>
@@ -23773,12 +23920,12 @@
         <v/>
       </c>
       <c r="F91" s="19"/>
-      <c r="G91" s="35"/>
-      <c r="H91" s="36"/>
-      <c r="I91" s="36"/>
-      <c r="J91" s="37"/>
+      <c r="G91" s="34"/>
+      <c r="H91" s="35"/>
+      <c r="I91" s="35"/>
+      <c r="J91" s="36"/>
       <c r="K91" s="19"/>
-      <c r="L91" s="38"/>
+      <c r="L91" s="37"/>
       <c r="M91" s="19"/>
       <c r="N91" t="str">
         <f t="shared" si="244"/>
@@ -23939,12 +24086,12 @@
         <v/>
       </c>
       <c r="F92" s="19"/>
-      <c r="G92" s="35"/>
-      <c r="H92" s="36"/>
-      <c r="I92" s="36"/>
-      <c r="J92" s="37"/>
+      <c r="G92" s="34"/>
+      <c r="H92" s="35"/>
+      <c r="I92" s="35"/>
+      <c r="J92" s="36"/>
       <c r="K92" s="19"/>
-      <c r="L92" s="38"/>
+      <c r="L92" s="37"/>
       <c r="M92" s="19"/>
       <c r="N92" t="str">
         <f t="shared" si="244"/>
@@ -24105,12 +24252,12 @@
         <v/>
       </c>
       <c r="F93" s="19"/>
-      <c r="G93" s="35"/>
-      <c r="H93" s="36"/>
-      <c r="I93" s="36"/>
-      <c r="J93" s="37"/>
+      <c r="G93" s="34"/>
+      <c r="H93" s="35"/>
+      <c r="I93" s="35"/>
+      <c r="J93" s="36"/>
       <c r="K93" s="19"/>
-      <c r="L93" s="38"/>
+      <c r="L93" s="37"/>
       <c r="M93" s="19"/>
       <c r="N93" t="str">
         <f t="shared" si="244"/>
@@ -24271,12 +24418,12 @@
         <v/>
       </c>
       <c r="F94" s="19"/>
-      <c r="G94" s="35"/>
-      <c r="H94" s="36"/>
-      <c r="I94" s="36"/>
-      <c r="J94" s="37"/>
+      <c r="G94" s="34"/>
+      <c r="H94" s="35"/>
+      <c r="I94" s="35"/>
+      <c r="J94" s="36"/>
       <c r="K94" s="19"/>
-      <c r="L94" s="38"/>
+      <c r="L94" s="37"/>
       <c r="M94" s="19"/>
       <c r="N94" t="str">
         <f t="shared" si="244"/>
@@ -24437,12 +24584,12 @@
         <v/>
       </c>
       <c r="F95" s="19"/>
-      <c r="G95" s="35"/>
-      <c r="H95" s="36"/>
-      <c r="I95" s="36"/>
-      <c r="J95" s="37"/>
+      <c r="G95" s="34"/>
+      <c r="H95" s="35"/>
+      <c r="I95" s="35"/>
+      <c r="J95" s="36"/>
       <c r="K95" s="19"/>
-      <c r="L95" s="38"/>
+      <c r="L95" s="37"/>
       <c r="M95" s="19"/>
       <c r="N95" t="str">
         <f t="shared" si="244"/>
@@ -24603,12 +24750,12 @@
         <v/>
       </c>
       <c r="F96" s="19"/>
-      <c r="G96" s="35"/>
-      <c r="H96" s="36"/>
-      <c r="I96" s="36"/>
-      <c r="J96" s="37"/>
+      <c r="G96" s="34"/>
+      <c r="H96" s="35"/>
+      <c r="I96" s="35"/>
+      <c r="J96" s="36"/>
       <c r="K96" s="19"/>
-      <c r="L96" s="38"/>
+      <c r="L96" s="37"/>
       <c r="M96" s="19"/>
       <c r="N96" t="str">
         <f t="shared" si="244"/>
@@ -24769,12 +24916,12 @@
         <v/>
       </c>
       <c r="F97" s="19"/>
-      <c r="G97" s="35"/>
-      <c r="H97" s="36"/>
-      <c r="I97" s="36"/>
-      <c r="J97" s="37"/>
+      <c r="G97" s="34"/>
+      <c r="H97" s="35"/>
+      <c r="I97" s="35"/>
+      <c r="J97" s="36"/>
       <c r="K97" s="19"/>
-      <c r="L97" s="38"/>
+      <c r="L97" s="37"/>
       <c r="M97" s="19"/>
       <c r="N97" t="str">
         <f t="shared" si="244"/>
@@ -24935,12 +25082,12 @@
         <v/>
       </c>
       <c r="F98" s="19"/>
-      <c r="G98" s="35"/>
-      <c r="H98" s="36"/>
-      <c r="I98" s="36"/>
-      <c r="J98" s="37"/>
+      <c r="G98" s="34"/>
+      <c r="H98" s="35"/>
+      <c r="I98" s="35"/>
+      <c r="J98" s="36"/>
       <c r="K98" s="19"/>
-      <c r="L98" s="38"/>
+      <c r="L98" s="37"/>
       <c r="M98" s="19"/>
       <c r="N98" t="str">
         <f t="shared" si="244"/>
@@ -25101,12 +25248,12 @@
         <v/>
       </c>
       <c r="F99" s="19"/>
-      <c r="G99" s="35"/>
-      <c r="H99" s="36"/>
-      <c r="I99" s="36"/>
-      <c r="J99" s="37"/>
+      <c r="G99" s="34"/>
+      <c r="H99" s="35"/>
+      <c r="I99" s="35"/>
+      <c r="J99" s="36"/>
       <c r="K99" s="19"/>
-      <c r="L99" s="38"/>
+      <c r="L99" s="37"/>
       <c r="M99" s="19"/>
       <c r="N99" t="str">
         <f t="shared" si="244"/>
@@ -25267,12 +25414,12 @@
         <v/>
       </c>
       <c r="F100" s="19"/>
-      <c r="G100" s="35"/>
-      <c r="H100" s="36"/>
-      <c r="I100" s="36"/>
-      <c r="J100" s="37"/>
+      <c r="G100" s="34"/>
+      <c r="H100" s="35"/>
+      <c r="I100" s="35"/>
+      <c r="J100" s="36"/>
       <c r="K100" s="19"/>
-      <c r="L100" s="38"/>
+      <c r="L100" s="37"/>
       <c r="M100" s="19"/>
       <c r="N100" t="str">
         <f t="shared" si="244"/>
@@ -25433,12 +25580,12 @@
         <v/>
       </c>
       <c r="F101" s="19"/>
-      <c r="G101" s="35"/>
-      <c r="H101" s="36"/>
-      <c r="I101" s="36"/>
-      <c r="J101" s="37"/>
+      <c r="G101" s="34"/>
+      <c r="H101" s="35"/>
+      <c r="I101" s="35"/>
+      <c r="J101" s="36"/>
       <c r="K101" s="19"/>
-      <c r="L101" s="38"/>
+      <c r="L101" s="37"/>
       <c r="M101" s="19"/>
       <c r="N101" t="str">
         <f t="shared" si="244"/>
@@ -25599,12 +25746,12 @@
         <v/>
       </c>
       <c r="F102" s="19"/>
-      <c r="G102" s="35"/>
-      <c r="H102" s="36"/>
-      <c r="I102" s="36"/>
-      <c r="J102" s="37"/>
+      <c r="G102" s="34"/>
+      <c r="H102" s="35"/>
+      <c r="I102" s="35"/>
+      <c r="J102" s="36"/>
       <c r="K102" s="19"/>
-      <c r="L102" s="38"/>
+      <c r="L102" s="37"/>
       <c r="M102" s="19"/>
       <c r="N102" t="str">
         <f t="shared" si="244"/>
@@ -25765,12 +25912,12 @@
         <v/>
       </c>
       <c r="F103" s="19"/>
-      <c r="G103" s="35"/>
-      <c r="H103" s="36"/>
-      <c r="I103" s="36"/>
-      <c r="J103" s="37"/>
+      <c r="G103" s="34"/>
+      <c r="H103" s="35"/>
+      <c r="I103" s="35"/>
+      <c r="J103" s="36"/>
       <c r="K103" s="19"/>
-      <c r="L103" s="38"/>
+      <c r="L103" s="37"/>
       <c r="M103" s="19"/>
       <c r="N103" t="str">
         <f t="shared" si="244"/>
@@ -25931,12 +26078,12 @@
         <v/>
       </c>
       <c r="F104" s="19"/>
-      <c r="G104" s="35"/>
-      <c r="H104" s="36"/>
-      <c r="I104" s="36"/>
-      <c r="J104" s="37"/>
+      <c r="G104" s="34"/>
+      <c r="H104" s="35"/>
+      <c r="I104" s="35"/>
+      <c r="J104" s="36"/>
       <c r="K104" s="19"/>
-      <c r="L104" s="38"/>
+      <c r="L104" s="37"/>
       <c r="M104" s="19"/>
       <c r="N104" t="str">
         <f t="shared" si="244"/>
@@ -26097,12 +26244,12 @@
         <v/>
       </c>
       <c r="F105" s="19"/>
-      <c r="G105" s="35"/>
-      <c r="H105" s="36"/>
-      <c r="I105" s="36"/>
-      <c r="J105" s="37"/>
+      <c r="G105" s="34"/>
+      <c r="H105" s="35"/>
+      <c r="I105" s="35"/>
+      <c r="J105" s="36"/>
       <c r="K105" s="19"/>
-      <c r="L105" s="38"/>
+      <c r="L105" s="37"/>
       <c r="M105" s="19"/>
       <c r="N105" t="str">
         <f t="shared" si="244"/>
@@ -26263,12 +26410,12 @@
         <v/>
       </c>
       <c r="F106" s="19"/>
-      <c r="G106" s="35"/>
-      <c r="H106" s="36"/>
-      <c r="I106" s="36"/>
-      <c r="J106" s="37"/>
+      <c r="G106" s="34"/>
+      <c r="H106" s="35"/>
+      <c r="I106" s="35"/>
+      <c r="J106" s="36"/>
       <c r="K106" s="19"/>
-      <c r="L106" s="38"/>
+      <c r="L106" s="37"/>
       <c r="M106" s="19"/>
       <c r="N106" t="str">
         <f t="shared" si="244"/>
@@ -26429,12 +26576,12 @@
         <v/>
       </c>
       <c r="F107" s="19"/>
-      <c r="G107" s="35"/>
-      <c r="H107" s="36"/>
-      <c r="I107" s="36"/>
-      <c r="J107" s="37"/>
+      <c r="G107" s="34"/>
+      <c r="H107" s="35"/>
+      <c r="I107" s="35"/>
+      <c r="J107" s="36"/>
       <c r="K107" s="19"/>
-      <c r="L107" s="38"/>
+      <c r="L107" s="37"/>
       <c r="M107" s="19"/>
       <c r="N107" t="str">
         <f t="shared" si="244"/>
@@ -26595,12 +26742,12 @@
         <v/>
       </c>
       <c r="F108" s="19"/>
-      <c r="G108" s="35"/>
-      <c r="H108" s="36"/>
-      <c r="I108" s="36"/>
-      <c r="J108" s="37"/>
+      <c r="G108" s="34"/>
+      <c r="H108" s="35"/>
+      <c r="I108" s="35"/>
+      <c r="J108" s="36"/>
       <c r="K108" s="19"/>
-      <c r="L108" s="38"/>
+      <c r="L108" s="37"/>
       <c r="M108" s="19"/>
       <c r="N108" t="str">
         <f t="shared" si="244"/>
@@ -26761,12 +26908,12 @@
         <v/>
       </c>
       <c r="F109" s="19"/>
-      <c r="G109" s="35"/>
-      <c r="H109" s="36"/>
-      <c r="I109" s="36"/>
-      <c r="J109" s="37"/>
+      <c r="G109" s="34"/>
+      <c r="H109" s="35"/>
+      <c r="I109" s="35"/>
+      <c r="J109" s="36"/>
       <c r="K109" s="19"/>
-      <c r="L109" s="38"/>
+      <c r="L109" s="37"/>
       <c r="M109" s="19"/>
       <c r="N109" t="str">
         <f t="shared" si="244"/>
@@ -26927,12 +27074,12 @@
         <v/>
       </c>
       <c r="F110" s="19"/>
-      <c r="G110" s="35"/>
-      <c r="H110" s="36"/>
-      <c r="I110" s="36"/>
-      <c r="J110" s="37"/>
+      <c r="G110" s="34"/>
+      <c r="H110" s="35"/>
+      <c r="I110" s="35"/>
+      <c r="J110" s="36"/>
       <c r="K110" s="19"/>
-      <c r="L110" s="38"/>
+      <c r="L110" s="37"/>
       <c r="M110" s="19"/>
       <c r="N110" t="str">
         <f t="shared" si="244"/>
@@ -27093,12 +27240,12 @@
         <v/>
       </c>
       <c r="F111" s="19"/>
-      <c r="G111" s="35"/>
-      <c r="H111" s="36"/>
-      <c r="I111" s="36"/>
-      <c r="J111" s="37"/>
+      <c r="G111" s="34"/>
+      <c r="H111" s="35"/>
+      <c r="I111" s="35"/>
+      <c r="J111" s="36"/>
       <c r="K111" s="19"/>
-      <c r="L111" s="38"/>
+      <c r="L111" s="37"/>
       <c r="M111" s="19"/>
       <c r="N111" t="str">
         <f t="shared" si="244"/>
@@ -27259,12 +27406,12 @@
         <v/>
       </c>
       <c r="F112" s="19"/>
-      <c r="G112" s="35"/>
-      <c r="H112" s="36"/>
-      <c r="I112" s="36"/>
-      <c r="J112" s="37"/>
+      <c r="G112" s="34"/>
+      <c r="H112" s="35"/>
+      <c r="I112" s="35"/>
+      <c r="J112" s="36"/>
       <c r="K112" s="19"/>
-      <c r="L112" s="38"/>
+      <c r="L112" s="37"/>
       <c r="M112" s="19"/>
       <c r="N112" t="str">
         <f t="shared" si="244"/>
@@ -27425,12 +27572,12 @@
         <v/>
       </c>
       <c r="F113" s="19"/>
-      <c r="G113" s="35"/>
-      <c r="H113" s="36"/>
-      <c r="I113" s="36"/>
-      <c r="J113" s="37"/>
+      <c r="G113" s="34"/>
+      <c r="H113" s="35"/>
+      <c r="I113" s="35"/>
+      <c r="J113" s="36"/>
       <c r="K113" s="19"/>
-      <c r="L113" s="38"/>
+      <c r="L113" s="37"/>
       <c r="M113" s="19"/>
       <c r="N113" t="str">
         <f t="shared" si="244"/>
@@ -27591,12 +27738,12 @@
         <v/>
       </c>
       <c r="F114" s="19"/>
-      <c r="G114" s="35"/>
-      <c r="H114" s="36"/>
-      <c r="I114" s="36"/>
-      <c r="J114" s="37"/>
+      <c r="G114" s="34"/>
+      <c r="H114" s="35"/>
+      <c r="I114" s="35"/>
+      <c r="J114" s="36"/>
       <c r="K114" s="19"/>
-      <c r="L114" s="38"/>
+      <c r="L114" s="37"/>
       <c r="M114" s="19"/>
       <c r="N114" t="str">
         <f t="shared" si="244"/>
@@ -27757,12 +27904,12 @@
         <v/>
       </c>
       <c r="F115" s="19"/>
-      <c r="G115" s="35"/>
-      <c r="H115" s="36"/>
-      <c r="I115" s="36"/>
-      <c r="J115" s="37"/>
+      <c r="G115" s="34"/>
+      <c r="H115" s="35"/>
+      <c r="I115" s="35"/>
+      <c r="J115" s="36"/>
       <c r="K115" s="19"/>
-      <c r="L115" s="38"/>
+      <c r="L115" s="37"/>
       <c r="M115" s="19"/>
       <c r="N115" t="str">
         <f t="shared" si="244"/>
@@ -27923,12 +28070,12 @@
         <v/>
       </c>
       <c r="F116" s="19"/>
-      <c r="G116" s="35"/>
-      <c r="H116" s="36"/>
-      <c r="I116" s="36"/>
-      <c r="J116" s="37"/>
+      <c r="G116" s="34"/>
+      <c r="H116" s="35"/>
+      <c r="I116" s="35"/>
+      <c r="J116" s="36"/>
       <c r="K116" s="19"/>
-      <c r="L116" s="38"/>
+      <c r="L116" s="37"/>
       <c r="M116" s="19"/>
       <c r="N116" t="str">
         <f t="shared" si="244"/>
@@ -28089,12 +28236,12 @@
         <v/>
       </c>
       <c r="F117" s="19"/>
-      <c r="G117" s="35"/>
-      <c r="H117" s="36"/>
-      <c r="I117" s="36"/>
-      <c r="J117" s="37"/>
+      <c r="G117" s="34"/>
+      <c r="H117" s="35"/>
+      <c r="I117" s="35"/>
+      <c r="J117" s="36"/>
       <c r="K117" s="19"/>
-      <c r="L117" s="38"/>
+      <c r="L117" s="37"/>
       <c r="M117" s="19"/>
       <c r="N117" t="str">
         <f t="shared" si="244"/>
@@ -28255,12 +28402,12 @@
         <v/>
       </c>
       <c r="F118" s="19"/>
-      <c r="G118" s="35"/>
-      <c r="H118" s="36"/>
-      <c r="I118" s="36"/>
-      <c r="J118" s="37"/>
+      <c r="G118" s="34"/>
+      <c r="H118" s="35"/>
+      <c r="I118" s="35"/>
+      <c r="J118" s="36"/>
       <c r="K118" s="19"/>
-      <c r="L118" s="38"/>
+      <c r="L118" s="37"/>
       <c r="M118" s="19"/>
       <c r="N118" t="str">
         <f t="shared" si="244"/>
@@ -28421,12 +28568,12 @@
         <v/>
       </c>
       <c r="F119" s="19"/>
-      <c r="G119" s="35"/>
-      <c r="H119" s="36"/>
-      <c r="I119" s="36"/>
-      <c r="J119" s="37"/>
+      <c r="G119" s="34"/>
+      <c r="H119" s="35"/>
+      <c r="I119" s="35"/>
+      <c r="J119" s="36"/>
       <c r="K119" s="19"/>
-      <c r="L119" s="38"/>
+      <c r="L119" s="37"/>
       <c r="M119" s="19"/>
       <c r="N119" t="str">
         <f t="shared" si="244"/>
@@ -28587,12 +28734,12 @@
         <v/>
       </c>
       <c r="F120" s="19"/>
-      <c r="G120" s="35"/>
-      <c r="H120" s="36"/>
-      <c r="I120" s="36"/>
-      <c r="J120" s="37"/>
+      <c r="G120" s="34"/>
+      <c r="H120" s="35"/>
+      <c r="I120" s="35"/>
+      <c r="J120" s="36"/>
       <c r="K120" s="19"/>
-      <c r="L120" s="38"/>
+      <c r="L120" s="37"/>
       <c r="M120" s="19"/>
       <c r="N120" t="str">
         <f t="shared" si="244"/>
@@ -28749,7 +28896,7 @@
     </row>
     <row r="121" spans="5:51">
       <c r="F121" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="N121" t="str">
         <f t="shared" ref="N121:N124" si="294">IF(AND(H121="",I121=""),"",IF(H121="",0,2-H121)+IF(I121="",0,2-I121))</f>
@@ -28863,22 +29010,22 @@
   <sheetData>
     <row r="3" spans="2:7">
       <c r="B3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C3" t="s">
         <v>215</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>216</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>217</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>218</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>219</v>
-      </c>
-      <c r="G3" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="4" spans="2:7">
@@ -28949,7 +29096,7 @@
         <v>985</v>
       </c>
       <c r="F7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G7">
         <f>E7-E6</f>

</xml_diff>

<commit_message>
Readme update and densities adjustment
</commit_message>
<xml_diff>
--- a/BasePlanning.xlsx
+++ b/BasePlanning.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="222">
   <si>
     <t>Efficiency of this module</t>
   </si>
@@ -614,9 +614,6 @@
   </si>
   <si>
     <t>Kerbal 0.10</t>
-  </si>
-  <si>
-    <t>Kerbal 0.9</t>
   </si>
   <si>
     <t>OKS Aeroponics Purify</t>
@@ -1312,8 +1309,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:DR124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:C9"/>
+    <sheetView tabSelected="1" topLeftCell="BN1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="CB13" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="BN1" sqref="BN1"/>
+      <selection pane="topRight" activeCell="BP1" sqref="BP1"/>
+      <selection pane="bottomLeft" activeCell="BN2" sqref="BN2"/>
+      <selection pane="bottomRight" activeCell="CI33" sqref="CI33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1336,8 +1337,9 @@
     <col min="19" max="25" width="5.28515625" hidden="1" customWidth="1"/>
     <col min="26" max="26" width="7.28515625" hidden="1" customWidth="1"/>
     <col min="27" max="27" width="5.28515625" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="8.42578125" hidden="1" customWidth="1"/>
-    <col min="29" max="39" width="9" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="8.42578125" customWidth="1"/>
+    <col min="29" max="32" width="9" hidden="1" customWidth="1"/>
+    <col min="33" max="39" width="9" customWidth="1"/>
     <col min="40" max="40" width="3.7109375" hidden="1" customWidth="1"/>
     <col min="41" max="41" width="7.5703125" hidden="1" customWidth="1"/>
     <col min="42" max="43" width="7.7109375" hidden="1" customWidth="1"/>
@@ -1373,7 +1375,7 @@
   <sheetData>
     <row r="1" spans="2:122" ht="153" customHeight="1">
       <c r="B1" s="42" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C1" s="42"/>
       <c r="E1" s="1" t="s">
@@ -1413,7 +1415,7 @@
         <v>5</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>118</v>
@@ -1646,7 +1648,7 @@
         <v>37</v>
       </c>
       <c r="CO1" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="CP1" s="12"/>
       <c r="CQ1" s="12" t="s">
@@ -1994,7 +1996,7 @@
       </c>
       <c r="CG2" s="7"/>
       <c r="CH2" s="7">
-        <v>1E-3</v>
+        <v>2.8102905982906002E-4</v>
       </c>
       <c r="CI2" s="7">
         <v>1.4100000000000001E-6</v>
@@ -2006,10 +2008,10 @@
         <v>1.951E-6</v>
       </c>
       <c r="CL2" s="7">
-        <v>1E-3</v>
+        <v>7.5000000000000002E-4</v>
       </c>
       <c r="CM2" s="7">
-        <v>1E-3</v>
+        <v>1.005E-3</v>
       </c>
       <c r="CN2" s="15"/>
     </row>
@@ -2848,7 +2850,7 @@
         <v>1.125</v>
       </c>
       <c r="BA5" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="BB5" s="5">
         <v>0</v>
@@ -3200,7 +3202,7 @@
         <v>1.125</v>
       </c>
       <c r="BA6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="BB6" s="5">
         <v>0</v>
@@ -3365,7 +3367,7 @@
     </row>
     <row r="7" spans="2:122">
       <c r="B7" s="43" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C7" s="44">
         <f ca="1">ROUNDUP(-MIN(C80:C83)/2333,1)</f>
@@ -4154,27 +4156,27 @@
       </c>
       <c r="AH9" s="15">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.0817575525E-5</v>
+        <v>-1.6927083333000001E-5</v>
       </c>
       <c r="AI9" s="15">
         <f t="shared" ca="1" si="23"/>
-        <v>-3.5215918463259999E-3</v>
+        <v>-1.7135375623849999E-3</v>
       </c>
       <c r="AJ9" s="15">
         <f t="shared" ca="1" si="24"/>
-        <v>-2.0807576966E-5</v>
+        <v>-1.1188078703999999E-5</v>
       </c>
       <c r="AK9" s="15">
         <f t="shared" ca="1" si="25"/>
-        <v>3.0298531298469998E-3</v>
+        <v>1.4801288987600001E-3</v>
       </c>
       <c r="AL9" s="15">
         <f t="shared" ca="1" si="26"/>
-        <v>7.8028413620000008E-6</v>
+        <v>1.5393518520000001E-6</v>
       </c>
       <c r="AM9" s="15">
         <f t="shared" ca="1" si="27"/>
-        <v>2.2876512175999999E-5</v>
+        <v>1.4247685185E-5</v>
       </c>
       <c r="AN9">
         <f t="shared" ca="1" si="28"/>
@@ -4518,27 +4520,27 @@
       </c>
       <c r="AH10" s="15">
         <f t="shared" ca="1" si="22"/>
-        <v>-2.1635151050000001E-5</v>
+        <v>-3.3854166666000003E-5</v>
       </c>
       <c r="AI10" s="15">
         <f t="shared" ca="1" si="23"/>
-        <v>-7.0431836926519997E-3</v>
+        <v>-3.4270751247699998E-3</v>
       </c>
       <c r="AJ10" s="15">
         <f t="shared" ca="1" si="24"/>
-        <v>-4.1615153932E-5</v>
+        <v>-2.2376157407999999E-5</v>
       </c>
       <c r="AK10" s="15">
         <f t="shared" ca="1" si="25"/>
-        <v>6.0597062596939996E-3</v>
+        <v>2.9602577975200001E-3</v>
       </c>
       <c r="AL10" s="15">
         <f t="shared" ca="1" si="26"/>
-        <v>1.5605682724000002E-5</v>
+        <v>3.0787037040000002E-6</v>
       </c>
       <c r="AM10" s="15">
         <f t="shared" ca="1" si="27"/>
-        <v>4.5753024351999997E-5</v>
+        <v>2.849537037E-5</v>
       </c>
       <c r="AN10">
         <f t="shared" ca="1" si="28"/>
@@ -4882,27 +4884,27 @@
       </c>
       <c r="AH11" s="15">
         <f t="shared" ca="1" si="22"/>
-        <v>-2.1635151050000001E-5</v>
+        <v>-3.3854166666000003E-5</v>
       </c>
       <c r="AI11" s="15">
         <f t="shared" ca="1" si="23"/>
-        <v>-7.0431836926519997E-3</v>
+        <v>-3.4270751247699998E-3</v>
       </c>
       <c r="AJ11" s="15">
         <f t="shared" ca="1" si="24"/>
-        <v>-4.1615153932E-5</v>
+        <v>-2.2376157407999999E-5</v>
       </c>
       <c r="AK11" s="15">
         <f t="shared" ca="1" si="25"/>
-        <v>6.0597062596939996E-3</v>
+        <v>2.9602577975200001E-3</v>
       </c>
       <c r="AL11" s="15">
         <f t="shared" ca="1" si="26"/>
-        <v>1.5605682724000002E-5</v>
+        <v>3.0787037040000002E-6</v>
       </c>
       <c r="AM11" s="15">
         <f t="shared" ca="1" si="27"/>
-        <v>4.5753024351999997E-5</v>
+        <v>2.849537037E-5</v>
       </c>
       <c r="AN11">
         <f t="shared" ca="1" si="28"/>
@@ -5367,7 +5369,7 @@
       </c>
       <c r="CO12">
         <f t="shared" si="44"/>
-        <v>-1.0181691038565104E-3</v>
+        <v>-1.018165672379684E-3</v>
       </c>
       <c r="CR12">
         <f t="shared" si="47"/>
@@ -5737,7 +5739,7 @@
       </c>
       <c r="CO13">
         <f t="shared" si="44"/>
-        <v>-1.0240105946400103E-3</v>
+        <v>-1.0240071631631839E-3</v>
       </c>
       <c r="CR13">
         <f t="shared" si="47"/>
@@ -6058,7 +6060,7 @@
         <v>1.4975555555555558</v>
       </c>
       <c r="BN14" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="BO14" s="7">
         <v>7.1</v>
@@ -6109,7 +6111,7 @@
       </c>
       <c r="CO14">
         <f t="shared" si="44"/>
-        <v>-6.1120416889999949E-6</v>
+        <v>-6.2149859937919963E-6</v>
       </c>
       <c r="CR14">
         <f t="shared" si="47"/>
@@ -6424,7 +6426,7 @@
         <v>5.3105227272727271</v>
       </c>
       <c r="BN15" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="BO15" s="7">
         <v>7.2</v>
@@ -6483,7 +6485,7 @@
       </c>
       <c r="CO15">
         <f>SUMPRODUCT($BR$2:$CM$2,BR15:CM15)</f>
-        <v>-3.8583210085860222E-6</v>
+        <v>-3.8580922434642624E-6</v>
       </c>
       <c r="CR15">
         <f t="shared" si="47"/>
@@ -6798,7 +6800,7 @@
         <v>3.0880477528089885</v>
       </c>
       <c r="BN16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="BO16">
         <v>7.3</v>
@@ -7158,13 +7160,13 @@
         <v>1.9948363095238095</v>
       </c>
       <c r="BN17" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="BO17" s="7">
         <v>7.4</v>
       </c>
       <c r="BP17" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="BQ17" s="7">
         <v>-6.25</v>
@@ -7209,7 +7211,7 @@
       </c>
       <c r="CO17">
         <f t="shared" si="86"/>
-        <v>-8.9051042224999984E-6</v>
+        <v>-9.1624649844799949E-6</v>
       </c>
       <c r="CR17">
         <f t="shared" si="47"/>
@@ -7524,13 +7526,13 @@
         <v>2.9579759196502988E-2</v>
       </c>
       <c r="BN18" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="BO18" s="7">
         <v>7.5</v>
       </c>
       <c r="BP18" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="BQ18" s="7">
         <v>-12.5</v>
@@ -7583,7 +7585,7 @@
       </c>
       <c r="CO18">
         <f t="shared" si="86"/>
-        <v>-3.2708025214650599E-6</v>
+        <v>-3.2702306086606596E-6</v>
       </c>
       <c r="CR18">
         <f t="shared" si="47"/>
@@ -7691,7 +7693,7 @@
         <v/>
       </c>
       <c r="F19" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G19" s="34"/>
       <c r="H19" s="35"/>
@@ -7900,13 +7902,13 @@
         <v>2.4276106109028472E-2</v>
       </c>
       <c r="BN19" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="BO19" s="7">
         <v>7.6</v>
       </c>
       <c r="BP19" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="BQ19" s="7"/>
       <c r="BR19" s="22">
@@ -8158,27 +8160,27 @@
       </c>
       <c r="AH20" s="15">
         <f t="shared" ca="1" si="22"/>
-        <v>-2.1635151050000001E-5</v>
+        <v>-3.3854166666000003E-5</v>
       </c>
       <c r="AI20" s="15">
         <f t="shared" ca="1" si="23"/>
-        <v>-7.0431836926519997E-3</v>
+        <v>-3.4270751247699998E-3</v>
       </c>
       <c r="AJ20" s="15">
         <f t="shared" ca="1" si="24"/>
-        <v>-4.1615153932E-5</v>
+        <v>-2.2376157407999999E-5</v>
       </c>
       <c r="AK20" s="15">
         <f t="shared" ca="1" si="25"/>
-        <v>6.0597062596939996E-3</v>
+        <v>2.9602577975200001E-3</v>
       </c>
       <c r="AL20" s="15">
         <f t="shared" ca="1" si="26"/>
-        <v>1.5605682724000002E-5</v>
+        <v>3.0787037040000002E-6</v>
       </c>
       <c r="AM20" s="15">
         <f t="shared" ca="1" si="27"/>
-        <v>4.5753024351999997E-5</v>
+        <v>2.849537037E-5</v>
       </c>
       <c r="AN20">
         <f t="shared" ca="1" si="28"/>
@@ -8276,7 +8278,7 @@
         <v>5.861947194468504E-3</v>
       </c>
       <c r="BN20" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="BO20" s="7">
         <v>8.1</v>
@@ -8327,7 +8329,7 @@
       </c>
       <c r="CO20">
         <f t="shared" si="86"/>
-        <v>-4.2656056827239992E-6</v>
+        <v>-4.2617042620429994E-6</v>
       </c>
       <c r="CR20">
         <f t="shared" si="47"/>
@@ -8536,27 +8538,27 @@
       </c>
       <c r="AH21" s="15">
         <f t="shared" ca="1" si="22"/>
-        <v>-2.1635151050000001E-5</v>
+        <v>-3.3854166666000003E-5</v>
       </c>
       <c r="AI21" s="15">
         <f t="shared" ca="1" si="23"/>
-        <v>-7.0431836926519997E-3</v>
+        <v>-3.4270751247699998E-3</v>
       </c>
       <c r="AJ21" s="15">
         <f t="shared" ca="1" si="24"/>
-        <v>-4.1615153932E-5</v>
+        <v>-2.2376157407999999E-5</v>
       </c>
       <c r="AK21" s="15">
         <f t="shared" ca="1" si="25"/>
-        <v>6.0597062596939996E-3</v>
+        <v>2.9602577975200001E-3</v>
       </c>
       <c r="AL21" s="15">
         <f t="shared" ca="1" si="26"/>
-        <v>1.5605682724000002E-5</v>
+        <v>3.0787037040000002E-6</v>
       </c>
       <c r="AM21" s="15">
         <f t="shared" ca="1" si="27"/>
-        <v>4.5753024351999997E-5</v>
+        <v>2.849537037E-5</v>
       </c>
       <c r="AN21">
         <f t="shared" ca="1" si="28"/>
@@ -8654,7 +8656,7 @@
         <v>0.11240718750000001</v>
       </c>
       <c r="BN21" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="BO21" s="7">
         <v>8.1999999999999993</v>
@@ -8705,7 +8707,7 @@
       </c>
       <c r="CO21">
         <f t="shared" si="86"/>
-        <v>-4.6177975678499987E-6</v>
+        <v>-4.6333526127411581E-6</v>
       </c>
       <c r="CR21">
         <f t="shared" si="47"/>
@@ -9013,13 +9015,13 @@
         <v>1.3715140397767858E-4</v>
       </c>
       <c r="BN22" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="BO22" s="7">
         <v>8.3000000000000007</v>
       </c>
       <c r="BP22" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="BQ22" s="7">
         <v>-6.25</v>
@@ -9064,7 +9066,7 @@
       </c>
       <c r="CO22">
         <f t="shared" si="86"/>
-        <v>-4.3280284136199988E-6</v>
+        <v>-4.3085213102149989E-6</v>
       </c>
       <c r="CR22">
         <f t="shared" si="47"/>
@@ -9165,7 +9167,7 @@
       </c>
       <c r="C23">
         <f ca="1">SUM(AH:AH)</f>
-        <v>2.1635151050000028E-5</v>
+        <v>1.0447518242100002E-4</v>
       </c>
       <c r="E23" s="4">
         <f t="shared" si="2"/>
@@ -9271,27 +9273,27 @@
       </c>
       <c r="AH23" s="15">
         <f t="shared" si="22"/>
-        <v>-2.1635151050000001E-5</v>
+        <v>-3.3854166666000003E-5</v>
       </c>
       <c r="AI23" s="15">
         <f t="shared" si="23"/>
-        <v>-7.0431836926519997E-3</v>
+        <v>-3.4270751247699998E-3</v>
       </c>
       <c r="AJ23" s="15">
         <f t="shared" si="24"/>
-        <v>-4.1615153932E-5</v>
+        <v>-2.2376157407999999E-5</v>
       </c>
       <c r="AK23" s="15">
         <f t="shared" si="25"/>
-        <v>6.0597062596939996E-3</v>
+        <v>2.9602577975200001E-3</v>
       </c>
       <c r="AL23" s="15">
         <f t="shared" si="26"/>
-        <v>1.5605682724000002E-5</v>
+        <v>3.0787037040000002E-6</v>
       </c>
       <c r="AM23" s="15">
         <f t="shared" si="27"/>
-        <v>4.5753024351999997E-5</v>
+        <v>2.849537037E-5</v>
       </c>
       <c r="AN23" t="str">
         <f t="shared" si="28"/>
@@ -9389,13 +9391,13 @@
         <v>2.0621795028142855E-4</v>
       </c>
       <c r="BN23" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="BO23" s="7">
         <v>8.4</v>
       </c>
       <c r="BP23" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="BQ23" s="7">
         <v>-12.5</v>
@@ -9440,7 +9442,7 @@
       </c>
       <c r="CO23">
         <f t="shared" si="86"/>
-        <v>-6.0889878392499985E-6</v>
+        <v>-6.1667630637057931E-6</v>
       </c>
       <c r="CR23">
         <f t="shared" si="47"/>
@@ -9541,7 +9543,7 @@
       </c>
       <c r="C24">
         <f ca="1">SUM(AI:AI)</f>
-        <v>1.5847163308466999E-2</v>
+        <v>3.9351868999699995E-2</v>
       </c>
       <c r="E24" s="4">
         <f t="shared" si="2"/>
@@ -9718,19 +9720,19 @@
       </c>
       <c r="BB24" s="15">
         <f t="shared" ref="BB24:BK24" ca="1" si="97">IF(BB$31=1,SUMIF($K:$K,BB$1,$AH:$AH),"")</f>
-        <v>-5.4087877625000002E-5</v>
+        <v>-8.4635416665000007E-5</v>
       </c>
       <c r="BC24" s="15">
         <f t="shared" ca="1" si="97"/>
-        <v>-6.4905453150000003E-5</v>
+        <v>-1.0156249999800001E-4</v>
       </c>
       <c r="BD24" s="15">
         <f t="shared" ca="1" si="97"/>
-        <v>-1.0817575525E-5</v>
+        <v>-1.6927083333000001E-5</v>
       </c>
       <c r="BE24" s="15">
         <f t="shared" ca="1" si="97"/>
-        <v>1.5144605735000003E-4</v>
+        <v>1.4533654954200002E-4</v>
       </c>
       <c r="BF24" s="15">
         <f t="shared" ca="1" si="97"/>
@@ -9758,7 +9760,7 @@
       </c>
       <c r="BL24" s="15">
         <f t="shared" ca="1" si="94"/>
-        <v>2.1635151050000028E-5</v>
+        <v>-5.7788450453999997E-5</v>
       </c>
       <c r="BN24" s="7" t="s">
         <v>115</v>
@@ -9901,7 +9903,7 @@
       </c>
       <c r="C25">
         <f ca="1">ROUND(SUM(AJ:AJ),15)</f>
-        <v>0</v>
+        <v>1.2505347740600001E-4</v>
       </c>
       <c r="E25" s="4" t="str">
         <f t="shared" si="2"/>
@@ -10072,19 +10074,19 @@
       </c>
       <c r="BB25" s="15">
         <f t="shared" ref="BB25:BK25" ca="1" si="150">IF(BB$31=1,SUMIF($K:$K,BB$1,$AI:$AI),"")</f>
-        <v>-1.7607959231629999E-2</v>
+        <v>-8.5676878119250004E-3</v>
       </c>
       <c r="BC25" s="15">
         <f t="shared" ca="1" si="150"/>
-        <v>-2.1129551077955999E-2</v>
+        <v>-1.0281225374309999E-2</v>
       </c>
       <c r="BD25" s="15">
         <f t="shared" ca="1" si="150"/>
-        <v>-3.5215918463259999E-3</v>
+        <v>-1.7135375623849999E-3</v>
       </c>
       <c r="BE25" s="15">
         <f t="shared" ca="1" si="150"/>
-        <v>5.8106265464378998E-2</v>
+        <v>5.9914319748319997E-2</v>
       </c>
       <c r="BF25" s="15">
         <f t="shared" ca="1" si="150"/>
@@ -10112,7 +10114,7 @@
       </c>
       <c r="BL25" s="15">
         <f t="shared" ca="1" si="94"/>
-        <v>1.5847163308466999E-2</v>
+        <v>3.9351868999699995E-2</v>
       </c>
       <c r="BN25" s="7" t="s">
         <v>116</v>
@@ -10417,19 +10419,19 @@
       </c>
       <c r="BB26" s="15">
         <f t="shared" ref="BB26:BK26" ca="1" si="151">IF(BB$31=1,SUMIF($K:$K,BB$1,$AJ:$AJ),"")</f>
-        <v>-1.0403788482999999E-4</v>
+        <v>-5.5940393520000003E-5</v>
       </c>
       <c r="BC26" s="15">
         <f t="shared" ca="1" si="151"/>
-        <v>-1.2484546179599999E-4</v>
+        <v>-6.7128472224E-5</v>
       </c>
       <c r="BD26" s="15">
         <f t="shared" ca="1" si="151"/>
-        <v>-1.5367881844888572E-3</v>
+        <v>-1.5271686862268572E-3</v>
       </c>
       <c r="BE26" s="15">
         <f t="shared" ca="1" si="151"/>
-        <v>1.7656715311148573E-3</v>
+        <v>1.7752910293768573E-3</v>
       </c>
       <c r="BF26" s="15">
         <f t="shared" ca="1" si="151"/>
@@ -10457,7 +10459,7 @@
       </c>
       <c r="BL26" s="15">
         <f t="shared" ca="1" si="94"/>
-        <v>0</v>
+        <v>1.2505347740600012E-4</v>
       </c>
       <c r="BN26" s="7" t="s">
         <v>117</v>
@@ -10597,7 +10599,7 @@
       </c>
       <c r="C27">
         <f ca="1">SUM(AK:AK)</f>
-        <v>0.20711210323311277</v>
+        <v>0.1869656882289818</v>
       </c>
       <c r="E27" s="4" t="str">
         <f t="shared" si="2"/>
@@ -10770,19 +10772,19 @@
       </c>
       <c r="BB27" s="15">
         <f t="shared" ref="BB27:BK27" ca="1" si="152">IF(BB$31=1,SUMIF($K:$K,BB$1,$AK:$AK),"")</f>
-        <v>1.5149265649234998E-2</v>
+        <v>7.4006444938000005E-3</v>
       </c>
       <c r="BC27" s="15">
         <f t="shared" ca="1" si="152"/>
-        <v>1.8179118779081998E-2</v>
+        <v>8.8807733925599999E-3</v>
       </c>
       <c r="BD27" s="15">
         <f t="shared" ca="1" si="152"/>
-        <v>0.22377629544727129</v>
+        <v>0.22222657121618433</v>
       </c>
       <c r="BE27" s="15">
         <f t="shared" ca="1" si="152"/>
-        <v>-4.99925766424755E-2</v>
+        <v>-5.1542300873562499E-2</v>
       </c>
       <c r="BF27" s="15">
         <f t="shared" ca="1" si="152"/>
@@ -10810,7 +10812,7 @@
       </c>
       <c r="BL27" s="15">
         <f t="shared" ca="1" si="94"/>
-        <v>0.20711210323311277</v>
+        <v>0.18696568822898185</v>
       </c>
       <c r="BN27" s="7" t="s">
         <v>33</v>
@@ -10954,7 +10956,7 @@
       </c>
       <c r="C28">
         <f ca="1">SUM(AL:AL)</f>
-        <v>-1.5605682723999998E-5</v>
+        <v>-9.7031046353999998E-5</v>
       </c>
       <c r="E28" s="4">
         <f t="shared" ca="1" si="2"/>
@@ -11133,19 +11135,19 @@
       </c>
       <c r="BB28" s="15">
         <f t="shared" ref="BB28:BK28" ca="1" si="153">IF(BB$31=1,SUMIF($K:$K,BB$1,$AL:$AL),"")</f>
-        <v>3.9014206810000009E-5</v>
+        <v>7.6967592600000006E-6</v>
       </c>
       <c r="BC28" s="15">
         <f t="shared" ca="1" si="153"/>
-        <v>4.6817048172000008E-5</v>
+        <v>9.236111112E-6</v>
       </c>
       <c r="BD28" s="15">
         <f t="shared" ca="1" si="153"/>
-        <v>7.8028413620000008E-6</v>
+        <v>1.5393518520000001E-6</v>
       </c>
       <c r="BE28" s="15">
         <f t="shared" ca="1" si="153"/>
-        <v>-1.09239779068E-4</v>
+        <v>-1.15503268578E-4</v>
       </c>
       <c r="BF28" s="15">
         <f t="shared" ca="1" si="153"/>
@@ -11173,7 +11175,7 @@
       </c>
       <c r="BL28" s="15">
         <f t="shared" ca="1" si="94"/>
-        <v>-1.5605682723999985E-5</v>
+        <v>-9.7031046354000011E-5</v>
       </c>
       <c r="BN28" s="7" t="s">
         <v>34</v>
@@ -11316,7 +11318,7 @@
       </c>
       <c r="C29">
         <f ca="1">ROUND(SUM(AM:AM),15)</f>
-        <v>0</v>
+        <v>-1.12174750883E-4</v>
       </c>
       <c r="E29" s="4" t="str">
         <f t="shared" si="2"/>
@@ -11487,19 +11489,19 @@
       </c>
       <c r="BB29" s="15">
         <f t="shared" ref="BB29:BK29" ca="1" si="154">IF(BB$31=1,SUMIF($K:$K,BB$1,$AM:$AM),"")</f>
-        <v>1.1438256087999999E-4</v>
+        <v>7.1238425924999993E-5</v>
       </c>
       <c r="BC29" s="15">
         <f t="shared" ca="1" si="154"/>
-        <v>1.3725907305599998E-4</v>
+        <v>8.5486111109999999E-5</v>
       </c>
       <c r="BD29" s="15">
         <f t="shared" ca="1" si="154"/>
-        <v>1.689593827856E-3</v>
+        <v>1.6809650008649999E-3</v>
       </c>
       <c r="BE29" s="15">
         <f t="shared" ca="1" si="154"/>
-        <v>-1.941235461792E-3</v>
+        <v>-1.9498642887830001E-3</v>
       </c>
       <c r="BF29" s="15">
         <f t="shared" ca="1" si="154"/>
@@ -11527,7 +11529,7 @@
       </c>
       <c r="BL29" s="15">
         <f t="shared" ca="1" si="94"/>
-        <v>0</v>
+        <v>-1.1217475088300013E-4</v>
       </c>
       <c r="BN29" s="7" t="s">
         <v>36</v>
@@ -11771,27 +11773,27 @@
       </c>
       <c r="AH30" s="15">
         <f t="shared" ca="1" si="22"/>
-        <v>-1.0817575525E-5</v>
+        <v>-1.6927083333000001E-5</v>
       </c>
       <c r="AI30" s="15">
         <f t="shared" ca="1" si="23"/>
-        <v>-3.5215918463259999E-3</v>
+        <v>-1.7135375623849999E-3</v>
       </c>
       <c r="AJ30" s="15">
         <f t="shared" ca="1" si="24"/>
-        <v>-6.2274105348242856E-4</v>
+        <v>-6.1312155522042855E-4</v>
       </c>
       <c r="AK30" s="15">
         <f t="shared" ca="1" si="25"/>
-        <v>9.067917581470665E-2</v>
+        <v>8.9129451583619651E-2</v>
       </c>
       <c r="AL30" s="15">
         <f t="shared" ca="1" si="26"/>
-        <v>7.8028413620000008E-6</v>
+        <v>1.5393518520000001E-6</v>
       </c>
       <c r="AM30" s="15">
         <f t="shared" ca="1" si="27"/>
-        <v>6.8466132869600003E-4</v>
+        <v>6.7603250170500005E-4</v>
       </c>
       <c r="AN30">
         <f t="shared" ca="1" si="28"/>
@@ -11842,7 +11844,7 @@
         <v>0.9642857142857143</v>
       </c>
       <c r="BN30" s="7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="BO30" s="7">
         <v>100</v>
@@ -11851,34 +11853,31 @@
         <f>-0.0277777777777778-0.0138888888888889</f>
         <v>-4.1666666666666699E-2</v>
       </c>
-      <c r="BT30" s="15"/>
-      <c r="BU30" s="15"/>
-      <c r="BV30" s="15"/>
-      <c r="CH30" s="15">
-        <v>-1.0817575525E-5</v>
+      <c r="CH30">
+        <v>-1.6927083333000001E-5</v>
       </c>
       <c r="CI30">
-        <v>-3.5215918463259999E-3</v>
-      </c>
-      <c r="CJ30" s="15">
-        <v>-2.0807576966E-5</v>
+        <v>-1.7135375623849999E-3</v>
+      </c>
+      <c r="CJ30">
+        <v>-1.1188078703999999E-5</v>
       </c>
       <c r="CK30">
-        <v>3.0298531298469998E-3</v>
-      </c>
-      <c r="CL30" s="15">
-        <v>7.8028413620000008E-6</v>
-      </c>
-      <c r="CM30" s="15">
-        <v>2.2876512175999999E-5</v>
+        <v>1.4801288987600001E-3</v>
+      </c>
+      <c r="CL30">
+        <v>1.5393518520000001E-6</v>
+      </c>
+      <c r="CM30">
+        <v>1.4247685185E-5</v>
       </c>
       <c r="CN30" s="15">
         <f>SUM(BT30:CM30)</f>
-        <v>-4.9268451543199988E-4</v>
+        <v>-2.4573678862499976E-4</v>
       </c>
       <c r="CO30">
         <f t="shared" si="86"/>
-        <v>1.1838608926858932E-20</v>
+        <v>-2.7822881647711128E-19</v>
       </c>
       <c r="CR30">
         <f t="shared" si="99"/>
@@ -11950,27 +11949,27 @@
       </c>
       <c r="DI30">
         <f t="shared" si="116"/>
-        <v>-0.23365963134000003</v>
+        <v>-0.36562499999280001</v>
       </c>
       <c r="DJ30">
         <f t="shared" si="117"/>
-        <v>-76.066383880641609</v>
+        <v>-37.012411347515993</v>
       </c>
       <c r="DK30">
         <f t="shared" si="118"/>
-        <v>-0.44944366246560002</v>
+        <v>-0.24166250000639999</v>
       </c>
       <c r="DL30">
         <f t="shared" si="119"/>
-        <v>65.444827604695206</v>
+        <v>31.970784213216</v>
       </c>
       <c r="DM30">
         <f t="shared" si="120"/>
-        <v>0.1685413734192</v>
+        <v>3.3250000003200005E-2</v>
       </c>
       <c r="DN30">
         <f t="shared" si="121"/>
-        <v>0.49413266300159997</v>
+        <v>0.30774999999600006</v>
       </c>
     </row>
     <row r="31" spans="2:119">
@@ -12205,34 +12204,18 @@
         <v>0</v>
       </c>
       <c r="BN31" s="7" t="s">
-        <v>186</v>
-      </c>
-      <c r="BO31" s="7"/>
-      <c r="CH31">
-        <v>-1.6927083333000001E-5</v>
-      </c>
-      <c r="CI31">
-        <v>-1.7135375623849999E-3</v>
-      </c>
-      <c r="CJ31">
-        <v>-1.1188078703999999E-5</v>
-      </c>
-      <c r="CK31">
-        <v>1.4801288987600001E-3</v>
-      </c>
-      <c r="CL31">
-        <v>1.5393518520000001E-6</v>
-      </c>
-      <c r="CM31">
-        <v>1.4247685185E-5</v>
+        <v>99</v>
+      </c>
+      <c r="BO31" s="7">
+        <v>101</v>
       </c>
       <c r="CN31" s="15">
         <f t="shared" ref="CN31:CN38" si="156">SUM(BT31:CM31)</f>
-        <v>-2.4573678862499976E-4</v>
+        <v>0</v>
       </c>
       <c r="CO31">
         <f t="shared" si="86"/>
-        <v>-1.1856481481482095E-8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:119">
@@ -12451,10 +12434,13 @@
         <v>0</v>
       </c>
       <c r="BN32" s="7" t="s">
-        <v>99</v>
+        <v>163</v>
       </c>
       <c r="BO32" s="7">
-        <v>101</v>
+        <v>200</v>
+      </c>
+      <c r="BQ32">
+        <v>-2.5</v>
       </c>
       <c r="CN32" s="15">
         <f t="shared" si="156"/>
@@ -12465,7 +12451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:93">
+    <row r="33" spans="2:113">
       <c r="B33" t="s">
         <v>130</v>
       </c>
@@ -12691,10 +12677,10 @@
         <v>0</v>
       </c>
       <c r="BN33" s="7" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="BO33" s="7">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="BQ33">
         <v>-2.5</v>
@@ -12707,8 +12693,12 @@
         <f t="shared" si="86"/>
         <v>0</v>
       </c>
+      <c r="DI33">
+        <f>DI30/DI21</f>
+        <v>-0.78238803574241733</v>
+      </c>
     </row>
-    <row r="34" spans="2:93">
+    <row r="34" spans="2:113">
       <c r="E34" s="4">
         <f t="shared" ref="E34:E65" ca="1" si="159">IF(P34="","",IF(AND(G34&gt;=200,G34&lt;300),100%,MIN(L34,AY34)))</f>
         <v>1.7152242271898735E-5</v>
@@ -12935,14 +12925,15 @@
         <v>0</v>
       </c>
       <c r="BN34" s="7" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="BO34" s="7">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="BQ34">
         <v>-2.5</v>
       </c>
+      <c r="CI34" s="15"/>
       <c r="CN34" s="15">
         <f t="shared" si="156"/>
         <v>0</v>
@@ -12951,8 +12942,12 @@
         <f t="shared" si="86"/>
         <v>0</v>
       </c>
+      <c r="DI34">
+        <f>DC21/DC15</f>
+        <v>-1</v>
+      </c>
     </row>
-    <row r="35" spans="2:93">
+    <row r="35" spans="2:113">
       <c r="B35" t="s">
         <v>131</v>
       </c>
@@ -13186,15 +13181,15 @@
         <v>0</v>
       </c>
       <c r="BN35" s="7" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="BO35" s="7">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="BQ35">
         <v>-2.5</v>
       </c>
-      <c r="CI35" s="15"/>
+      <c r="CL35" s="15"/>
       <c r="CN35" s="15">
         <f t="shared" si="156"/>
         <v>0</v>
@@ -13203,8 +13198,12 @@
         <f t="shared" si="86"/>
         <v>0</v>
       </c>
+      <c r="DI35">
+        <f>DH15/DH20</f>
+        <v>-1</v>
+      </c>
     </row>
-    <row r="36" spans="2:93">
+    <row r="36" spans="2:113">
       <c r="E36" s="4">
         <f t="shared" ca="1" si="159"/>
         <v>2.973589319899093E-4</v>
@@ -13431,10 +13430,10 @@
         <v>0</v>
       </c>
       <c r="BN36" s="7" t="s">
-        <v>150</v>
+        <v>169</v>
       </c>
       <c r="BO36" s="7">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="BQ36">
         <v>-2.5</v>
@@ -13448,8 +13447,12 @@
         <f t="shared" si="86"/>
         <v>0</v>
       </c>
+      <c r="DI36">
+        <f>DM20/DM30</f>
+        <v>-10.137826971607787</v>
+      </c>
     </row>
-    <row r="37" spans="2:93">
+    <row r="37" spans="2:113">
       <c r="B37" s="41" t="s">
         <v>88</v>
       </c>
@@ -13662,25 +13665,31 @@
         <v>0</v>
       </c>
       <c r="BN37" s="7" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="BO37" s="7">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="BQ37">
-        <v>-2.5</v>
-      </c>
-      <c r="CL37" s="15"/>
+        <v>100</v>
+      </c>
+      <c r="BS37">
+        <v>-0.2</v>
+      </c>
       <c r="CN37" s="15">
         <f t="shared" si="156"/>
         <v>0</v>
       </c>
       <c r="CO37">
         <f t="shared" si="86"/>
-        <v>0</v>
+        <v>-2.5000000000000005E-3</v>
+      </c>
+      <c r="DI37">
+        <f>DI36*DI33</f>
+        <v>7.9317145310127151</v>
       </c>
     </row>
-    <row r="38" spans="2:93">
+    <row r="38" spans="2:113">
       <c r="B38" s="25"/>
       <c r="E38" s="4">
         <f t="shared" ca="1" si="159"/>
@@ -13897,28 +13906,18 @@
         <f t="shared" si="207"/>
         <v>0</v>
       </c>
-      <c r="BN38" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="BO38" s="7">
-        <v>210</v>
-      </c>
-      <c r="BQ38">
-        <v>100</v>
-      </c>
-      <c r="BS38">
-        <v>-0.2</v>
-      </c>
+      <c r="BN38" s="7"/>
+      <c r="BO38" s="7"/>
       <c r="CN38" s="15">
         <f t="shared" si="156"/>
         <v>0</v>
       </c>
       <c r="CO38">
         <f t="shared" si="86"/>
-        <v>-2.5000000000000005E-3</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:93">
+    <row r="39" spans="2:113">
       <c r="B39" t="s">
         <v>51</v>
       </c>
@@ -14151,7 +14150,7 @@
       <c r="BN39" s="7"/>
       <c r="BO39" s="7"/>
     </row>
-    <row r="40" spans="2:93">
+    <row r="40" spans="2:113">
       <c r="E40" s="4">
         <f t="shared" ca="1" si="159"/>
         <v>0.5</v>
@@ -14382,7 +14381,7 @@
       <c r="CL40" s="15"/>
       <c r="CM40" s="15"/>
     </row>
-    <row r="41" spans="2:93">
+    <row r="41" spans="2:113">
       <c r="B41" t="s">
         <v>89</v>
       </c>
@@ -14601,7 +14600,7 @@
       <c r="BO41" s="7"/>
       <c r="CM41" s="15"/>
     </row>
-    <row r="42" spans="2:93">
+    <row r="42" spans="2:113">
       <c r="B42" t="s">
         <v>90</v>
       </c>
@@ -14780,7 +14779,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:93">
+    <row r="43" spans="2:113">
       <c r="B43" t="s">
         <v>91</v>
       </c>
@@ -14965,7 +14964,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="44" spans="2:93">
+    <row r="44" spans="2:113">
       <c r="B44" t="s">
         <v>92</v>
       </c>
@@ -15157,7 +15156,7 @@
       <c r="BJ44" s="19"/>
       <c r="BK44" s="19"/>
     </row>
-    <row r="45" spans="2:93">
+    <row r="45" spans="2:113">
       <c r="E45" s="4">
         <f t="shared" si="159"/>
         <v>1</v>
@@ -15342,7 +15341,7 @@
       <c r="BJ45" s="19"/>
       <c r="BK45" s="19"/>
     </row>
-    <row r="46" spans="2:93">
+    <row r="46" spans="2:113">
       <c r="B46" t="s">
         <v>93</v>
       </c>
@@ -15534,7 +15533,7 @@
       <c r="BJ46" s="19"/>
       <c r="BK46" s="19"/>
     </row>
-    <row r="47" spans="2:93">
+    <row r="47" spans="2:113">
       <c r="B47" t="s">
         <v>94</v>
       </c>
@@ -15726,7 +15725,7 @@
       <c r="BJ47" s="19"/>
       <c r="BK47" s="19"/>
     </row>
-    <row r="48" spans="2:93">
+    <row r="48" spans="2:113">
       <c r="B48" t="s">
         <v>95</v>
       </c>
@@ -17312,27 +17311,27 @@
       </c>
       <c r="AH56" s="15">
         <f t="shared" ca="1" si="177"/>
-        <v>-1.0817575525E-5</v>
+        <v>-1.6927083333000001E-5</v>
       </c>
       <c r="AI56" s="15">
         <f t="shared" ca="1" si="178"/>
-        <v>-3.5215918463259999E-3</v>
+        <v>-1.7135375623849999E-3</v>
       </c>
       <c r="AJ56" s="15">
         <f t="shared" ca="1" si="179"/>
-        <v>-2.0807576966E-5</v>
+        <v>-1.1188078703999999E-5</v>
       </c>
       <c r="AK56" s="15">
         <f t="shared" ca="1" si="180"/>
-        <v>3.0298531298469998E-3</v>
+        <v>1.4801288987600001E-3</v>
       </c>
       <c r="AL56" s="15">
         <f t="shared" ca="1" si="181"/>
-        <v>7.8028413620000008E-6</v>
+        <v>1.5393518520000001E-6</v>
       </c>
       <c r="AM56" s="15">
         <f t="shared" ca="1" si="182"/>
-        <v>2.2876512175999999E-5</v>
+        <v>1.4247685185E-5</v>
       </c>
       <c r="AN56">
         <f t="shared" ca="1" si="183"/>
@@ -17561,11 +17560,11 @@
     <row r="58" spans="1:63">
       <c r="A58" s="1"/>
       <c r="B58" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C58" s="27">
         <f ca="1">-(SUMIF(G:G,"&lt;&gt;7,1",AM:AM)+SUMIFS(O:O,M:M,"",G:G,7.1)*LOOKUP(100,BO:BO,CM:CM))/LOOKUP(7.1,BO:BO,CM:CM)</f>
-        <v>2.6329824041168326E-18</v>
+        <v>-5.4483223287412584E-3</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="4">
@@ -17573,7 +17572,7 @@
         <v>4.5936507936507942E-2</v>
       </c>
       <c r="F58" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G58" s="34">
         <v>7.4</v>
@@ -17766,18 +17765,18 @@
     </row>
     <row r="59" spans="1:63">
       <c r="B59" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C59" s="27">
         <f ca="1">-(SUMIF(G:G,"&lt;&gt;7,4",AM:AM)+SUMIFS(O:O,M:M,"",G:G,7.4)*LOOKUP(100,BO:BO,CM:CM))/LOOKUP(7.4,BO:BO,CM:CM)</f>
-        <v>4.5936507936507942E-2</v>
+        <v>4.3757179005011436E-2</v>
       </c>
       <c r="E59" s="4">
         <f t="shared" ca="1" si="159"/>
         <v>3.5</v>
       </c>
       <c r="F59" s="19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G59" s="34">
         <v>7.5</v>
@@ -17987,7 +17986,7 @@
         <v>3.5</v>
       </c>
       <c r="F60" s="19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G60" s="34">
         <v>7.6</v>
@@ -18383,7 +18382,7 @@
         <v>1.5</v>
       </c>
       <c r="F62" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G62" s="34">
         <v>8.3000000000000007</v>
@@ -18585,7 +18584,7 @@
         <v>1.5</v>
       </c>
       <c r="F63" s="19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G63" s="34">
         <v>8.4</v>
@@ -18873,9 +18872,9 @@
         <f t="shared" si="176"/>
         <v/>
       </c>
-      <c r="AH64" s="15" t="str">
-        <f t="shared" si="177"/>
-        <v/>
+      <c r="AH64" s="15">
+        <f ca="1">$J63*LOOKUP($G63,$BO:$BO,CH:CH)*$E63</f>
+        <v>1.6226363287500002E-4</v>
       </c>
       <c r="AI64" s="15" t="str">
         <f t="shared" si="178"/>
@@ -18946,7 +18945,7 @@
         <v/>
       </c>
       <c r="BA64" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="BB64" s="19"/>
       <c r="BC64" s="19"/>
@@ -19695,7 +19694,7 @@
         <v/>
       </c>
       <c r="F69" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G69" s="34"/>
       <c r="H69" s="35"/>
@@ -21976,7 +21975,7 @@
     </row>
     <row r="80" spans="2:63">
       <c r="B80" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C80" s="10">
         <f ca="1">SUMIF(U:U,"&lt;0")*60*60*6</f>
@@ -22192,7 +22191,7 @@
     </row>
     <row r="81" spans="2:63">
       <c r="B81" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C81" s="10">
         <f ca="1">SUMIF(V:V,"&lt;0")*60*60*6</f>
@@ -22408,7 +22407,7 @@
     </row>
     <row r="82" spans="2:63">
       <c r="B82" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C82" s="10">
         <f ca="1">SUMIF(W:W,"&lt;0")*60*60*6</f>
@@ -22581,11 +22580,11 @@
     </row>
     <row r="83" spans="2:63">
       <c r="B83" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C83" s="10">
         <f ca="1">SUMIF(AJ:AJ,"&lt;0")*60*60*6</f>
-        <v>-46.453212827694514</v>
+        <v>-43.752057715724916</v>
       </c>
       <c r="E83" s="4" t="str">
         <f t="shared" si="213"/>
@@ -28896,7 +28895,7 @@
     </row>
     <row r="121" spans="5:51">
       <c r="F121" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="N121" t="str">
         <f t="shared" ref="N121:N124" si="294">IF(AND(H121="",I121=""),"",IF(H121="",0,2-H121)+IF(I121="",0,2-I121))</f>
@@ -29010,22 +29009,22 @@
   <sheetData>
     <row r="3" spans="2:7">
       <c r="B3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C3" t="s">
         <v>214</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>215</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>216</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>217</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>218</v>
-      </c>
-      <c r="G3" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="4" spans="2:7">
@@ -29096,7 +29095,7 @@
         <v>985</v>
       </c>
       <c r="F7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G7">
         <f>E7-E6</f>

</xml_diff>

<commit_message>
Corrected Life Support Numbers
</commit_message>
<xml_diff>
--- a/BasePlanning.xlsx
+++ b/BasePlanning.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="USI_Efficiency" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -53,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="215">
   <si>
     <t>Efficiency of this module</t>
   </si>
@@ -694,27 +693,6 @@
     <t>Minimal Number of Mining ILMs to run smoothly on Rails</t>
   </si>
   <si>
-    <t>Min</t>
-  </si>
-  <si>
-    <t>Sec</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Metal</t>
-  </si>
-  <si>
-    <t>Delta Time</t>
-  </si>
-  <si>
-    <t>Delta Metal</t>
-  </si>
-  <si>
-    <t>..</t>
-  </si>
-  <si>
     <t>Base 5 contains the logistics hub and a lot of storage for extracted resources and fuel</t>
   </si>
   <si>
@@ -1310,10 +1288,10 @@
   <dimension ref="A1:DR124"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="L61" sqref="L61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1366,15 +1344,16 @@
     <col min="70" max="78" width="9.42578125" customWidth="1"/>
     <col min="79" max="79" width="10.42578125" customWidth="1"/>
     <col min="80" max="80" width="12.85546875" customWidth="1"/>
-    <col min="81" max="82" width="11.42578125" customWidth="1"/>
-    <col min="83" max="91" width="12.85546875" customWidth="1"/>
+    <col min="81" max="82" width="11.42578125" hidden="1" customWidth="1"/>
+    <col min="83" max="84" width="12.85546875" hidden="1" customWidth="1"/>
+    <col min="85" max="91" width="12.85546875" customWidth="1"/>
     <col min="92" max="92" width="15.7109375" customWidth="1"/>
     <col min="93" max="118" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:122" ht="153" customHeight="1">
       <c r="B1" s="42" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="C1" s="42"/>
       <c r="E1" s="1" t="s">
@@ -4411,7 +4390,7 @@
       </c>
       <c r="C10">
         <f ca="1">MIN(BB11:BK11)</f>
-        <v>23.271230158730162</v>
+        <v>25.771230158730162</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" ca="1" si="2"/>
@@ -4775,7 +4754,7 @@
       </c>
       <c r="C11">
         <f ca="1">SUM(S:S)</f>
-        <v>3.5285870858746828E-2</v>
+        <v>3.5285896755121782E-2</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" ca="1" si="2"/>
@@ -4966,11 +4945,11 @@
       </c>
       <c r="BD11" s="9">
         <f t="shared" ca="1" si="55"/>
-        <v>67.814575116774478</v>
+        <v>67.81465025331201</v>
       </c>
       <c r="BE11" s="9">
         <f t="shared" ca="1" si="55"/>
-        <v>23.271230158730162</v>
+        <v>25.771230158730162</v>
       </c>
       <c r="BF11" s="9">
         <f t="shared" ca="1" si="55"/>
@@ -5140,7 +5119,7 @@
       </c>
       <c r="C12">
         <f ca="1">SUM(T:T)</f>
-        <v>1.4975555555555555</v>
+        <v>0.99804444444444451</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="2"/>
@@ -5337,38 +5316,32 @@
       <c r="BZ12" s="7"/>
       <c r="CA12" s="7"/>
       <c r="CB12" s="7">
-        <v>3.2452726574999999E-4</v>
-      </c>
-      <c r="CC12" s="7">
-        <v>-2.125E-7</v>
-      </c>
-      <c r="CD12" s="7">
-        <v>-2.125E-7</v>
-      </c>
+        <v>5.0781249998999999E-4</v>
+      </c>
+      <c r="CC12" s="7"/>
+      <c r="CD12" s="7"/>
       <c r="CE12" s="7"/>
-      <c r="CF12" s="7">
-        <v>4.2500000000000001E-7</v>
-      </c>
+      <c r="CF12" s="7"/>
       <c r="CG12" s="7"/>
       <c r="CH12" s="7"/>
       <c r="CI12" s="7"/>
       <c r="CJ12" s="7">
-        <v>-6.2422730897999999E-4</v>
+        <v>-3.3564236111999999E-4</v>
       </c>
       <c r="CK12" s="7">
-        <v>9.0895593895410007E-2</v>
+        <v>4.44038669628E-2</v>
       </c>
       <c r="CL12" s="7"/>
       <c r="CM12" s="7">
-        <v>6.8629536528E-4</v>
+        <v>4.2743055555000001E-4</v>
       </c>
       <c r="CN12" s="15">
         <f>SUM(BT12:CM12)</f>
-        <v>-3.6217810782540043E-2</v>
+        <v>-8.249653234278001E-2</v>
       </c>
       <c r="CO12">
         <f t="shared" si="44"/>
-        <v>-1.018165672379684E-3</v>
+        <v>-1.0149288177085276E-3</v>
       </c>
       <c r="CR12">
         <f t="shared" si="47"/>
@@ -5416,15 +5389,15 @@
       </c>
       <c r="DC12">
         <f t="shared" si="56"/>
-        <v>7.0097889402</v>
+        <v>10.968749999783999</v>
       </c>
       <c r="DD12">
         <f t="shared" si="56"/>
-        <v>-4.5899999999999995E-3</v>
+        <v>0</v>
       </c>
       <c r="DE12">
         <f t="shared" si="56"/>
-        <v>-4.5899999999999995E-3</v>
+        <v>0</v>
       </c>
       <c r="DF12">
         <f t="shared" si="56"/>
@@ -5432,7 +5405,7 @@
       </c>
       <c r="DG12">
         <f t="shared" si="56"/>
-        <v>9.1799999999999989E-3</v>
+        <v>0</v>
       </c>
       <c r="DH12">
         <f t="shared" si="56"/>
@@ -5448,11 +5421,11 @@
       </c>
       <c r="DK12">
         <f t="shared" si="56"/>
-        <v>-13.483309873968</v>
+        <v>-7.2498750001920005</v>
       </c>
       <c r="DL12">
         <f t="shared" si="56"/>
-        <v>1963.3448281408562</v>
+        <v>959.12352639647997</v>
       </c>
       <c r="DM12">
         <f t="shared" si="56"/>
@@ -5460,7 +5433,7 @@
       </c>
       <c r="DN12">
         <f t="shared" ref="DN12:DN23" si="57">CM12 * 60 * 60 * 6</f>
-        <v>14.823979890047998</v>
+        <v>9.2324999998799999</v>
       </c>
     </row>
     <row r="13" spans="2:122">
@@ -5654,7 +5627,7 @@
       </c>
       <c r="BD13" s="15">
         <f t="shared" ca="1" si="58"/>
-        <v>-2.0646706095071685E-3</v>
+        <v>-2.0646447131322126E-3</v>
       </c>
       <c r="BE13" s="15">
         <f t="shared" ca="1" si="58"/>
@@ -5683,7 +5656,7 @@
       </c>
       <c r="BL13" s="15">
         <f t="shared" ref="BL13:BL14" ca="1" si="59">SUM(BB13:BK13)</f>
-        <v>3.5285870858746821E-2</v>
+        <v>3.5285896755121782E-2</v>
       </c>
       <c r="BN13" t="s">
         <v>52</v>
@@ -5707,38 +5680,32 @@
       <c r="BZ13" s="7"/>
       <c r="CA13" s="7"/>
       <c r="CB13" s="7"/>
-      <c r="CC13" s="7">
-        <v>-2.125E-7</v>
-      </c>
-      <c r="CD13" s="7">
-        <v>-2.125E-7</v>
-      </c>
+      <c r="CC13" s="7"/>
+      <c r="CD13" s="7"/>
       <c r="CE13" s="7"/>
-      <c r="CF13" s="7">
-        <v>4.2500000000000001E-7</v>
-      </c>
+      <c r="CF13" s="7"/>
       <c r="CG13" s="7">
-        <v>2.3408524086E-4</v>
+        <v>4.6180555559999997E-5</v>
       </c>
       <c r="CH13" s="7"/>
       <c r="CI13" s="7"/>
       <c r="CJ13" s="7">
-        <v>-6.2422730897999999E-4</v>
+        <v>-3.3564236111999999E-4</v>
       </c>
       <c r="CK13" s="7">
-        <v>9.0895593895410007E-2</v>
+        <v>4.44038669628E-2</v>
       </c>
       <c r="CL13" s="7"/>
       <c r="CM13" s="7">
-        <v>6.8629536528E-4</v>
+        <v>4.2743055555000001E-4</v>
       </c>
       <c r="CN13" s="15">
         <f t="shared" ref="CN13:CN17" si="60">SUM(BT13:CM13)</f>
-        <v>-3.6308252807430046E-2</v>
+        <v>-8.2958164287210007E-2</v>
       </c>
       <c r="CO13">
         <f t="shared" si="44"/>
-        <v>-1.0240071631631839E-3</v>
+        <v>-1.0240694427083477E-3</v>
       </c>
       <c r="CR13">
         <f t="shared" si="47"/>
@@ -5790,11 +5757,11 @@
       </c>
       <c r="DD13">
         <f t="shared" ref="DD13:DD23" si="72">CC13 * 60 * 60 * 6</f>
-        <v>-4.5899999999999995E-3</v>
+        <v>0</v>
       </c>
       <c r="DE13">
         <f t="shared" ref="DE13:DE23" si="73">CD13 * 60 * 60 * 6</f>
-        <v>-4.5899999999999995E-3</v>
+        <v>0</v>
       </c>
       <c r="DF13">
         <f t="shared" ref="DF13:DF23" si="74">CE13 * 60 * 60 * 6</f>
@@ -5802,11 +5769,11 @@
       </c>
       <c r="DG13">
         <f t="shared" ref="DG13:DG23" si="75">CF13 * 60 * 60 * 6</f>
-        <v>9.1799999999999989E-3</v>
+        <v>0</v>
       </c>
       <c r="DH13">
         <f t="shared" ref="DH13:DH23" si="76">CG13 * 60 * 60 * 6</f>
-        <v>5.0562412025759995</v>
+        <v>0.99750000009599993</v>
       </c>
       <c r="DI13">
         <f t="shared" ref="DI13:DI23" si="77">CH13 * 60 * 60 * 6</f>
@@ -5818,11 +5785,11 @@
       </c>
       <c r="DK13">
         <f t="shared" ref="DK13:DK23" si="79">CJ13 * 60 * 60 * 6</f>
-        <v>-13.483309873968</v>
+        <v>-7.2498750001920005</v>
       </c>
       <c r="DL13">
         <f t="shared" ref="DL13:DL23" si="80">CK13 * 60 * 60 * 6</f>
-        <v>1963.3448281408562</v>
+        <v>959.12352639647997</v>
       </c>
       <c r="DM13">
         <f t="shared" ref="DM13:DM23" si="81">CL13 * 60 * 60 * 6</f>
@@ -5830,7 +5797,7 @@
       </c>
       <c r="DN13">
         <f t="shared" si="57"/>
-        <v>14.823979890047998</v>
+        <v>9.2324999998799999</v>
       </c>
     </row>
     <row r="14" spans="2:122">
@@ -6028,7 +5995,7 @@
       </c>
       <c r="BE14" s="15">
         <f t="shared" ca="1" si="82"/>
-        <v>0.29951111111111112</v>
+        <v>-0.2</v>
       </c>
       <c r="BF14" s="15">
         <f t="shared" ca="1" si="82"/>
@@ -6056,7 +6023,7 @@
       </c>
       <c r="BL14" s="15">
         <f t="shared" ca="1" si="59"/>
-        <v>1.4975555555555558</v>
+        <v>0.99804444444444462</v>
       </c>
       <c r="BN14" s="7" t="s">
         <v>194</v>
@@ -6097,20 +6064,20 @@
       <c r="CH14" s="7"/>
       <c r="CI14" s="7"/>
       <c r="CJ14" s="22">
-        <v>1.8726819269400001E-2</v>
+        <v>1.00692708336E-2</v>
       </c>
       <c r="CK14" s="7"/>
       <c r="CL14" s="7"/>
       <c r="CM14" s="7">
-        <v>-2.0588860958399999E-2</v>
+        <v>-1.2822916666499999E-2</v>
       </c>
       <c r="CN14" s="23">
         <f t="shared" si="60"/>
-        <v>-1.8620416889999977E-3</v>
+        <v>-2.7536458328999997E-3</v>
       </c>
       <c r="CO14">
         <f t="shared" si="44"/>
-        <v>-6.2149859937919963E-6</v>
+        <v>-7.0677604162324986E-6</v>
       </c>
       <c r="CR14">
         <f t="shared" si="47"/>
@@ -6190,7 +6157,7 @@
       </c>
       <c r="DK14">
         <f t="shared" si="79"/>
-        <v>404.49929621903999</v>
+        <v>217.49625000576</v>
       </c>
       <c r="DL14">
         <f t="shared" si="80"/>
@@ -6202,7 +6169,7 @@
       </c>
       <c r="DN14">
         <f t="shared" si="57"/>
-        <v>-444.71939670144002</v>
+        <v>-276.97499999640002</v>
       </c>
     </row>
     <row r="15" spans="2:122">
@@ -6449,42 +6416,36 @@
       <c r="BZ15" s="7"/>
       <c r="CA15" s="7"/>
       <c r="CB15" s="7">
-        <v>2.1635151050000001E-5</v>
-      </c>
-      <c r="CC15" s="7">
-        <v>-2.125E-7</v>
-      </c>
-      <c r="CD15" s="7">
-        <v>-2.125E-7</v>
-      </c>
+        <v>3.3854166666000003E-5</v>
+      </c>
+      <c r="CC15" s="7"/>
+      <c r="CD15" s="7"/>
       <c r="CE15" s="7"/>
-      <c r="CF15" s="7">
-        <v>4.2500000000000001E-7</v>
-      </c>
+      <c r="CF15" s="7"/>
       <c r="CG15" s="7">
-        <v>-1.5605682724000002E-5</v>
+        <v>-3.0787037040000002E-6</v>
       </c>
       <c r="CH15" s="7"/>
       <c r="CI15" s="7">
-        <v>7.0431836926519997E-3</v>
+        <v>3.4270751247699998E-3</v>
       </c>
       <c r="CJ15" s="22">
-        <v>-4.1615153932E-5</v>
+        <v>-2.2376157407999999E-5</v>
       </c>
       <c r="CK15" s="7">
-        <v>-6.0597062596939996E-3</v>
+        <v>-2.9602577975200001E-3</v>
       </c>
       <c r="CL15" s="7"/>
       <c r="CM15" s="7">
-        <v>4.5753024351999997E-5</v>
+        <v>2.849537037E-5</v>
       </c>
       <c r="CN15" s="23">
         <f t="shared" si="60"/>
-        <v>9.9364477170399987E-4</v>
+        <v>5.0371200317399982E-4</v>
       </c>
       <c r="CO15">
         <f>SUMPRODUCT($BR$2:$CM$2,BR15:CM15)</f>
-        <v>-3.8580922434642624E-6</v>
+        <v>-3.6353065972351853E-6</v>
       </c>
       <c r="CR15">
         <f t="shared" si="47"/>
@@ -6532,15 +6493,15 @@
       </c>
       <c r="DC15">
         <f t="shared" si="71"/>
-        <v>0.46731926268000007</v>
+        <v>0.73124999998560003</v>
       </c>
       <c r="DD15">
         <f t="shared" si="72"/>
-        <v>-4.5899999999999995E-3</v>
+        <v>0</v>
       </c>
       <c r="DE15">
         <f t="shared" si="73"/>
-        <v>-4.5899999999999995E-3</v>
+        <v>0</v>
       </c>
       <c r="DF15">
         <f t="shared" si="74"/>
@@ -6548,11 +6509,11 @@
       </c>
       <c r="DG15">
         <f t="shared" si="75"/>
-        <v>9.1799999999999989E-3</v>
+        <v>0</v>
       </c>
       <c r="DH15">
         <f t="shared" si="76"/>
-        <v>-0.3370827468384</v>
+        <v>-6.6500000006400009E-2</v>
       </c>
       <c r="DI15">
         <f t="shared" si="77"/>
@@ -6560,15 +6521,15 @@
       </c>
       <c r="DJ15">
         <f t="shared" si="78"/>
-        <v>152.13276776128322</v>
+        <v>74.024822695031986</v>
       </c>
       <c r="DK15">
         <f t="shared" si="79"/>
-        <v>-0.89888732493120005</v>
+        <v>-0.48332500001279999</v>
       </c>
       <c r="DL15">
         <f t="shared" si="80"/>
-        <v>-130.88965520939041</v>
+        <v>-63.941568426431999</v>
       </c>
       <c r="DM15">
         <f t="shared" si="81"/>
@@ -6576,7 +6537,7 @@
       </c>
       <c r="DN15">
         <f t="shared" si="57"/>
-        <v>0.98826532600319994</v>
+        <v>0.61549999999200011</v>
       </c>
     </row>
     <row r="16" spans="2:122">
@@ -6585,7 +6546,7 @@
       </c>
       <c r="C16">
         <f ca="1">SUM(X:X)</f>
-        <v>2.9579759196502988E-2</v>
+        <v>2.9578499372624762E-2</v>
       </c>
       <c r="E16" s="4" t="str">
         <f t="shared" si="2"/>
@@ -6817,34 +6778,28 @@
       <c r="BZ16" s="7"/>
       <c r="CA16" s="7"/>
       <c r="CB16" s="7"/>
-      <c r="CC16" s="7">
-        <v>-2.125E-7</v>
-      </c>
-      <c r="CD16" s="7">
-        <v>-2.125E-7</v>
-      </c>
+      <c r="CC16" s="7"/>
+      <c r="CD16" s="7"/>
       <c r="CE16" s="7"/>
-      <c r="CF16" s="7">
-        <v>4.2500000000000001E-7</v>
-      </c>
+      <c r="CF16" s="7"/>
       <c r="CG16" s="7"/>
       <c r="CH16" s="7"/>
       <c r="CI16" s="7">
-        <v>-7.0431836926519997E-3</v>
+        <v>-3.4270751247699998E-3</v>
       </c>
       <c r="CJ16" s="7"/>
       <c r="CK16" s="7">
-        <v>6.0597062596939996E-3</v>
+        <v>2.9602577975200001E-3</v>
       </c>
       <c r="CL16" s="7"/>
       <c r="CM16" s="7"/>
       <c r="CN16" s="15">
         <f t="shared" si="60"/>
-        <v>-9.8347743295800014E-4</v>
+        <v>-4.6681732724999968E-4</v>
       </c>
       <c r="CO16">
         <f t="shared" ref="CO16:CO38" si="86">SUMPRODUCT($BR$2:$CM$2,BR16:CM16)</f>
-        <v>-4.2481084020939756E-6</v>
+        <v>-4.249056712962964E-6</v>
       </c>
       <c r="CR16">
         <f t="shared" si="47"/>
@@ -6896,11 +6851,11 @@
       </c>
       <c r="DD16">
         <f t="shared" si="72"/>
-        <v>-4.5899999999999995E-3</v>
+        <v>0</v>
       </c>
       <c r="DE16">
         <f t="shared" si="73"/>
-        <v>-4.5899999999999995E-3</v>
+        <v>0</v>
       </c>
       <c r="DF16">
         <f t="shared" si="74"/>
@@ -6908,7 +6863,7 @@
       </c>
       <c r="DG16">
         <f t="shared" si="75"/>
-        <v>9.1799999999999989E-3</v>
+        <v>0</v>
       </c>
       <c r="DH16">
         <f t="shared" si="76"/>
@@ -6920,7 +6875,7 @@
       </c>
       <c r="DJ16">
         <f t="shared" si="78"/>
-        <v>-152.13276776128322</v>
+        <v>-74.024822695031986</v>
       </c>
       <c r="DK16">
         <f t="shared" si="79"/>
@@ -6928,7 +6883,7 @@
       </c>
       <c r="DL16">
         <f t="shared" si="80"/>
-        <v>130.88965520939041</v>
+        <v>63.941568426431999</v>
       </c>
       <c r="DM16">
         <f t="shared" si="81"/>
@@ -6945,7 +6900,7 @@
       </c>
       <c r="C17">
         <f ca="1">SUM(Y:Y)</f>
-        <v>2.4276106109028472E-2</v>
+        <v>2.427736593308168E-2</v>
       </c>
       <c r="E17" s="4" t="str">
         <f t="shared" si="2"/>
@@ -7197,20 +7152,20 @@
       <c r="CH17" s="7"/>
       <c r="CI17" s="7"/>
       <c r="CJ17" s="7">
-        <v>4.6817048173499999E-2</v>
+        <v>2.5173177083999999E-2</v>
       </c>
       <c r="CK17" s="7"/>
       <c r="CL17" s="7"/>
       <c r="CM17" s="7">
-        <v>-5.1472152395999997E-2</v>
+        <v>-3.2057291666250001E-2</v>
       </c>
       <c r="CN17" s="23">
         <f t="shared" si="60"/>
-        <v>-4.6551042224999978E-3</v>
+        <v>-6.8841145822500019E-3</v>
       </c>
       <c r="CO17">
         <f t="shared" si="86"/>
-        <v>-9.1624649844799949E-6</v>
+        <v>-1.1294401040581255E-5</v>
       </c>
       <c r="CR17">
         <f t="shared" si="47"/>
@@ -7290,7 +7245,7 @@
       </c>
       <c r="DK17">
         <f t="shared" si="79"/>
-        <v>1011.2482405476001</v>
+        <v>543.74062501439994</v>
       </c>
       <c r="DL17">
         <f t="shared" si="80"/>
@@ -7302,7 +7257,7 @@
       </c>
       <c r="DN17">
         <f t="shared" si="57"/>
-        <v>-1111.7984917536</v>
+        <v>-692.43749999099998</v>
       </c>
     </row>
     <row r="18" spans="2:119">
@@ -7490,7 +7445,7 @@
       </c>
       <c r="BD18" s="15">
         <f t="shared" ca="1" si="88"/>
-        <v>2.0159196503024757E-5</v>
+        <v>1.8899372624797097E-5</v>
       </c>
       <c r="BE18" s="15">
         <f t="shared" ca="1" si="88"/>
@@ -7522,7 +7477,7 @@
       </c>
       <c r="BL18" s="15">
         <f t="shared" ca="1" si="84"/>
-        <v>2.9579759196502988E-2</v>
+        <v>2.9578499372624762E-2</v>
       </c>
       <c r="BN18" s="7" t="s">
         <v>188</v>
@@ -7549,42 +7504,36 @@
       <c r="BZ18" s="7"/>
       <c r="CA18" s="7"/>
       <c r="CB18" s="7">
-        <v>5.4087877625000002E-5</v>
-      </c>
-      <c r="CC18" s="7">
-        <v>-2.125E-7</v>
-      </c>
-      <c r="CD18" s="7">
-        <v>-2.125E-7</v>
-      </c>
+        <v>8.4635416664999993E-5</v>
+      </c>
+      <c r="CC18" s="7"/>
+      <c r="CD18" s="7"/>
       <c r="CE18" s="7"/>
-      <c r="CF18" s="7">
-        <v>4.2500000000000001E-7</v>
-      </c>
+      <c r="CF18" s="7"/>
       <c r="CG18" s="7">
-        <v>-3.9014206810000002E-5</v>
+        <v>-7.6967592600000006E-6</v>
       </c>
       <c r="CH18" s="7"/>
       <c r="CI18" s="7">
-        <v>1.7607959231629999E-2</v>
+        <v>8.5676878119250004E-3</v>
       </c>
       <c r="CJ18" s="7">
-        <v>-1.0403788482999999E-4</v>
+        <v>-5.5940393520000003E-5</v>
       </c>
       <c r="CK18" s="7">
-        <v>-1.5149265649234999E-2</v>
+        <v>-7.4006444937999996E-3</v>
       </c>
       <c r="CL18" s="7"/>
       <c r="CM18" s="7">
-        <v>1.1438256088E-4</v>
+        <v>7.1238425925000006E-5</v>
       </c>
       <c r="CN18" s="23">
         <f t="shared" ref="CN18:CN22" si="89">SUM(BT18:CM18)</f>
-        <v>2.4841119292600029E-3</v>
+        <v>1.259280007935001E-3</v>
       </c>
       <c r="CO18">
         <f t="shared" si="86"/>
-        <v>-3.2702306086606596E-6</v>
+        <v>-2.713266493087965E-6</v>
       </c>
       <c r="CR18">
         <f t="shared" si="47"/>
@@ -7632,15 +7581,15 @@
       </c>
       <c r="DC18">
         <f t="shared" si="71"/>
-        <v>1.1682981567000001</v>
+        <v>1.8281249999639999</v>
       </c>
       <c r="DD18">
         <f t="shared" si="72"/>
-        <v>-4.5899999999999995E-3</v>
+        <v>0</v>
       </c>
       <c r="DE18">
         <f t="shared" si="73"/>
-        <v>-4.5899999999999995E-3</v>
+        <v>0</v>
       </c>
       <c r="DF18">
         <f t="shared" si="74"/>
@@ -7648,11 +7597,11 @@
       </c>
       <c r="DG18">
         <f t="shared" si="75"/>
-        <v>9.1799999999999989E-3</v>
+        <v>0</v>
       </c>
       <c r="DH18">
         <f t="shared" si="76"/>
-        <v>-0.84270686709600007</v>
+        <v>-0.16625000001600002</v>
       </c>
       <c r="DI18">
         <f t="shared" si="77"/>
@@ -7660,15 +7609,15 @@
       </c>
       <c r="DJ18">
         <f t="shared" si="78"/>
-        <v>380.33191940320796</v>
+        <v>185.06205673758001</v>
       </c>
       <c r="DK18">
         <f t="shared" si="79"/>
-        <v>-2.2472183123280001</v>
+        <v>-1.2083125000320001</v>
       </c>
       <c r="DL18">
         <f t="shared" si="80"/>
-        <v>-327.22413802347597</v>
+        <v>-159.85392106607998</v>
       </c>
       <c r="DM18">
         <f t="shared" si="81"/>
@@ -7676,7 +7625,7 @@
       </c>
       <c r="DN18">
         <f t="shared" si="57"/>
-        <v>2.4706633150079997</v>
+        <v>1.5387499999800001</v>
       </c>
     </row>
     <row r="19" spans="2:119">
@@ -7866,7 +7815,7 @@
       </c>
       <c r="BD19" s="15">
         <f t="shared" ca="1" si="90"/>
-        <v>-4.9938909715399421E-6</v>
+        <v>-3.7340669183353798E-6</v>
       </c>
       <c r="BE19" s="15">
         <f t="shared" ca="1" si="90"/>
@@ -7898,7 +7847,7 @@
       </c>
       <c r="BL19" s="15">
         <f t="shared" ca="1" si="84"/>
-        <v>2.4276106109028472E-2</v>
+        <v>2.427736593308168E-2</v>
       </c>
       <c r="BN19" s="7" t="s">
         <v>189</v>
@@ -7923,34 +7872,28 @@
       <c r="BZ19" s="7"/>
       <c r="CA19" s="7"/>
       <c r="CB19" s="7"/>
-      <c r="CC19" s="7">
-        <v>-2.125E-7</v>
-      </c>
-      <c r="CD19" s="7">
-        <v>-2.125E-7</v>
-      </c>
+      <c r="CC19" s="7"/>
+      <c r="CD19" s="7"/>
       <c r="CE19" s="7"/>
-      <c r="CF19" s="7">
-        <v>4.2500000000000001E-7</v>
-      </c>
+      <c r="CF19" s="7"/>
       <c r="CG19" s="7"/>
       <c r="CH19" s="7"/>
       <c r="CI19" s="7">
-        <v>-1.7607959231629999E-2</v>
+        <v>-8.5676878119250004E-3</v>
       </c>
       <c r="CJ19" s="7"/>
       <c r="CK19" s="7">
-        <v>1.5149265649234999E-2</v>
+        <v>7.4006444937999996E-3</v>
       </c>
       <c r="CL19" s="7"/>
       <c r="CM19" s="7"/>
       <c r="CN19" s="23">
         <f t="shared" si="89"/>
-        <v>-2.4586935823949999E-3</v>
+        <v>-1.1670433181250007E-3</v>
       </c>
       <c r="CO19">
         <f t="shared" si="86"/>
-        <v>-4.2452710052349403E-6</v>
+        <v>-4.2476417824074109E-6</v>
       </c>
       <c r="CR19">
         <f t="shared" si="47"/>
@@ -8002,11 +7945,11 @@
       </c>
       <c r="DD19">
         <f t="shared" si="72"/>
-        <v>-4.5899999999999995E-3</v>
+        <v>0</v>
       </c>
       <c r="DE19">
         <f t="shared" si="73"/>
-        <v>-4.5899999999999995E-3</v>
+        <v>0</v>
       </c>
       <c r="DF19">
         <f t="shared" si="74"/>
@@ -8014,7 +7957,7 @@
       </c>
       <c r="DG19">
         <f t="shared" si="75"/>
-        <v>9.1799999999999989E-3</v>
+        <v>0</v>
       </c>
       <c r="DH19">
         <f t="shared" si="76"/>
@@ -8026,7 +7969,7 @@
       </c>
       <c r="DJ19">
         <f t="shared" si="78"/>
-        <v>-380.33191940320796</v>
+        <v>-185.06205673758001</v>
       </c>
       <c r="DK19">
         <f t="shared" si="79"/>
@@ -8034,7 +7977,7 @@
       </c>
       <c r="DL19">
         <f t="shared" si="80"/>
-        <v>327.22413802347597</v>
+        <v>159.85392106607998</v>
       </c>
       <c r="DM19">
         <f t="shared" si="81"/>
@@ -8051,7 +7994,7 @@
       </c>
       <c r="C20">
         <f ca="1">SUM(AB:AB)</f>
-        <v>1.3715140397767858E-4</v>
+        <v>4.2080712363482139E-4</v>
       </c>
       <c r="E20" s="4">
         <f t="shared" ca="1" si="2"/>
@@ -8242,7 +8185,7 @@
       </c>
       <c r="BD20" s="15">
         <f t="shared" ca="1" si="91"/>
-        <v>-1.5165305531485375E-5</v>
+        <v>-1.5165305531485621E-5</v>
       </c>
       <c r="BE20" s="15">
         <f t="shared" ca="1" si="91"/>
@@ -8301,25 +8244,19 @@
       <c r="BZ20" s="7"/>
       <c r="CA20" s="7"/>
       <c r="CB20" s="7"/>
-      <c r="CC20" s="7">
-        <v>-2.125E-7</v>
-      </c>
-      <c r="CD20" s="7">
-        <v>-2.125E-7</v>
-      </c>
+      <c r="CC20" s="7"/>
+      <c r="CD20" s="7"/>
       <c r="CE20" s="7"/>
-      <c r="CF20" s="7">
-        <v>4.2500000000000001E-7</v>
-      </c>
+      <c r="CF20" s="7"/>
       <c r="CG20" s="7">
-        <v>1.5605682724000002E-5</v>
+        <v>3.0787037040000002E-6</v>
       </c>
       <c r="CH20" s="7"/>
       <c r="CI20" s="7"/>
       <c r="CJ20" s="7"/>
       <c r="CK20" s="7"/>
       <c r="CL20" s="7">
-        <v>-1.5605682724000002E-5</v>
+        <v>-3.0787037040000002E-6</v>
       </c>
       <c r="CM20" s="7"/>
       <c r="CN20" s="15">
@@ -8328,7 +8265,7 @@
       </c>
       <c r="CO20">
         <f t="shared" si="86"/>
-        <v>-4.2617042620429994E-6</v>
+        <v>-4.2523090277780004E-6</v>
       </c>
       <c r="CR20">
         <f t="shared" si="47"/>
@@ -8380,11 +8317,11 @@
       </c>
       <c r="DD20">
         <f t="shared" si="72"/>
-        <v>-4.5899999999999995E-3</v>
+        <v>0</v>
       </c>
       <c r="DE20">
         <f t="shared" si="73"/>
-        <v>-4.5899999999999995E-3</v>
+        <v>0</v>
       </c>
       <c r="DF20">
         <f t="shared" si="74"/>
@@ -8392,11 +8329,11 @@
       </c>
       <c r="DG20">
         <f t="shared" si="75"/>
-        <v>9.1799999999999989E-3</v>
+        <v>0</v>
       </c>
       <c r="DH20">
         <f t="shared" si="76"/>
-        <v>0.3370827468384</v>
+        <v>6.6500000006400009E-2</v>
       </c>
       <c r="DI20">
         <f t="shared" si="77"/>
@@ -8416,7 +8353,7 @@
       </c>
       <c r="DM20">
         <f t="shared" si="81"/>
-        <v>-0.3370827468384</v>
+        <v>-6.6500000006400009E-2</v>
       </c>
       <c r="DN20">
         <f t="shared" si="57"/>
@@ -8429,7 +8366,7 @@
       </c>
       <c r="C21">
         <f ca="1">SUM(AG:AG)</f>
-        <v>2.0621795028142855E-4</v>
+        <v>4.0682870374285707E-5</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" ca="1" si="2"/>
@@ -8679,21 +8616,15 @@
       <c r="BZ21" s="7"/>
       <c r="CA21" s="7"/>
       <c r="CB21" s="7">
-        <v>-2.1635151050000001E-5</v>
-      </c>
-      <c r="CC21" s="7">
-        <v>-2.125E-7</v>
-      </c>
-      <c r="CD21" s="7">
-        <v>-2.125E-7</v>
-      </c>
+        <v>-3.3854166666000003E-5</v>
+      </c>
+      <c r="CC21" s="7"/>
+      <c r="CD21" s="7"/>
       <c r="CE21" s="7"/>
-      <c r="CF21" s="7">
-        <v>4.2500000000000001E-7</v>
-      </c>
+      <c r="CF21" s="7"/>
       <c r="CG21" s="7"/>
       <c r="CH21" s="7">
-        <v>2.1635151050000001E-5</v>
+        <v>3.3854166666000003E-5</v>
       </c>
       <c r="CI21" s="7"/>
       <c r="CJ21" s="7"/>
@@ -8706,7 +8637,7 @@
       </c>
       <c r="CO21">
         <f t="shared" si="86"/>
-        <v>-4.6333526127411581E-6</v>
+        <v>-4.8498609953585575E-6</v>
       </c>
       <c r="CR21">
         <f t="shared" si="47"/>
@@ -8754,15 +8685,15 @@
       </c>
       <c r="DC21">
         <f t="shared" si="71"/>
-        <v>-0.46731926268000007</v>
+        <v>-0.73124999998560003</v>
       </c>
       <c r="DD21">
         <f t="shared" si="72"/>
-        <v>-4.5899999999999995E-3</v>
+        <v>0</v>
       </c>
       <c r="DE21">
         <f t="shared" si="73"/>
-        <v>-4.5899999999999995E-3</v>
+        <v>0</v>
       </c>
       <c r="DF21">
         <f t="shared" si="74"/>
@@ -8770,7 +8701,7 @@
       </c>
       <c r="DG21">
         <f t="shared" si="75"/>
-        <v>9.1799999999999989E-3</v>
+        <v>0</v>
       </c>
       <c r="DH21">
         <f t="shared" si="76"/>
@@ -8778,7 +8709,7 @@
       </c>
       <c r="DI21">
         <f t="shared" si="77"/>
-        <v>0.46731926268000007</v>
+        <v>0.73124999998560003</v>
       </c>
       <c r="DJ21">
         <f t="shared" si="78"/>
@@ -8979,11 +8910,11 @@
       </c>
       <c r="BD22" s="15">
         <f t="shared" ca="1" si="95"/>
-        <v>4.7520063913392857E-4</v>
+        <v>7.435825892710714E-4</v>
       </c>
       <c r="BE22" s="15">
         <f t="shared" ca="1" si="95"/>
-        <v>2.7043938812499994E-5</v>
+        <v>4.2317708332499963E-5</v>
       </c>
       <c r="BF22" s="15">
         <f t="shared" ca="1" si="95"/>
@@ -9011,7 +8942,7 @@
       </c>
       <c r="BL22" s="15">
         <f t="shared" ca="1" si="94"/>
-        <v>1.3715140397767858E-4</v>
+        <v>4.2080712363482139E-4</v>
       </c>
       <c r="BN22" s="7" t="s">
         <v>192</v>
@@ -9049,14 +8980,14 @@
         <v>4.2500000000000001E-7</v>
       </c>
       <c r="CG22" s="7">
-        <v>7.8028413620000005E-5</v>
+        <v>1.5393518520000001E-5</v>
       </c>
       <c r="CH22" s="7"/>
       <c r="CI22" s="7"/>
       <c r="CJ22" s="7"/>
       <c r="CK22" s="7"/>
       <c r="CL22" s="7">
-        <v>-7.8028413620000005E-5</v>
+        <v>-1.5393518520000001E-5</v>
       </c>
       <c r="CM22" s="7"/>
       <c r="CN22" s="15">
@@ -9065,7 +8996,7 @@
       </c>
       <c r="CO22">
         <f t="shared" si="86"/>
-        <v>-4.3085213102149989E-6</v>
+        <v>-4.2615451388899994E-6</v>
       </c>
       <c r="CR22">
         <f t="shared" si="47"/>
@@ -9133,7 +9064,7 @@
       </c>
       <c r="DH22">
         <f t="shared" si="76"/>
-        <v>1.6854137341920001</v>
+        <v>0.33250000003200003</v>
       </c>
       <c r="DI22">
         <f t="shared" si="77"/>
@@ -9153,7 +9084,7 @@
       </c>
       <c r="DM22">
         <f t="shared" si="81"/>
-        <v>-1.6854137341920001</v>
+        <v>-0.33250000003200003</v>
       </c>
       <c r="DN22">
         <f t="shared" si="57"/>
@@ -9166,7 +9097,7 @@
       </c>
       <c r="C23">
         <f ca="1">SUM(AH:AH)</f>
-        <v>1.0447518242100002E-4</v>
+        <v>3.3854166665999976E-5</v>
       </c>
       <c r="E23" s="4">
         <f t="shared" si="2"/>
@@ -9355,11 +9286,11 @@
       </c>
       <c r="BD23" s="15">
         <f t="shared" ca="1" si="96"/>
-        <v>2.2572505368642856E-4</v>
+        <v>4.453125000428571E-5</v>
       </c>
       <c r="BE23" s="15">
         <f t="shared" ca="1" si="96"/>
-        <v>-1.9507103405000018E-5</v>
+        <v>-3.8483796300000003E-6</v>
       </c>
       <c r="BF23" s="15">
         <f t="shared" ca="1" si="96"/>
@@ -9387,7 +9318,7 @@
       </c>
       <c r="BL23" s="15">
         <f t="shared" ca="1" si="94"/>
-        <v>2.0621795028142855E-4</v>
+        <v>4.0682870374285707E-5</v>
       </c>
       <c r="BN23" s="7" t="s">
         <v>193</v>
@@ -9414,7 +9345,7 @@
       <c r="BZ23" s="7"/>
       <c r="CA23" s="7"/>
       <c r="CB23" s="7">
-        <v>-1.0817575525E-4</v>
+        <v>-1.6927083332999999E-4</v>
       </c>
       <c r="CC23" s="7">
         <v>-2.125E-7</v>
@@ -9428,7 +9359,7 @@
       </c>
       <c r="CG23" s="7"/>
       <c r="CH23" s="7">
-        <v>1.0817575525E-4</v>
+        <v>1.6927083332999999E-4</v>
       </c>
       <c r="CI23" s="7"/>
       <c r="CJ23" s="7"/>
@@ -9441,7 +9372,7 @@
       </c>
       <c r="CO23">
         <f t="shared" si="86"/>
-        <v>-6.1667630637057931E-6</v>
+        <v>-7.2493049767927869E-6</v>
       </c>
       <c r="CR23">
         <f t="shared" si="47"/>
@@ -9489,7 +9420,7 @@
       </c>
       <c r="DC23">
         <f t="shared" si="71"/>
-        <v>-2.3365963134000003</v>
+        <v>-3.6562499999279998</v>
       </c>
       <c r="DD23">
         <f t="shared" si="72"/>
@@ -9513,7 +9444,7 @@
       </c>
       <c r="DI23">
         <f t="shared" si="77"/>
-        <v>2.3365963134000003</v>
+        <v>3.6562499999279998</v>
       </c>
       <c r="DJ23">
         <f t="shared" si="78"/>
@@ -9542,7 +9473,7 @@
       </c>
       <c r="C24">
         <f ca="1">SUM(AI:AI)</f>
-        <v>3.9351868999699995E-2</v>
+        <v>7.7109190307324965E-3</v>
       </c>
       <c r="E24" s="4">
         <f t="shared" si="2"/>
@@ -9731,7 +9662,7 @@
       </c>
       <c r="BE24" s="15">
         <f t="shared" ca="1" si="97"/>
-        <v>1.4533654954200002E-4</v>
+        <v>2.3697916666199999E-4</v>
       </c>
       <c r="BF24" s="15">
         <f t="shared" ca="1" si="97"/>
@@ -9759,7 +9690,7 @@
       </c>
       <c r="BL24" s="15">
         <f t="shared" ca="1" si="94"/>
-        <v>-5.7788450453999997E-5</v>
+        <v>3.3854166665999976E-5</v>
       </c>
       <c r="BN24" s="7" t="s">
         <v>115</v>
@@ -9902,7 +9833,7 @@
       </c>
       <c r="C25">
         <f ca="1">ROUND(SUM(AJ:AJ),15)</f>
-        <v>1.2505347740600001E-4</v>
+        <v>0</v>
       </c>
       <c r="E25" s="4" t="str">
         <f t="shared" si="2"/>
@@ -10085,7 +10016,7 @@
       </c>
       <c r="BE25" s="15">
         <f t="shared" ca="1" si="150"/>
-        <v>5.9914319748319997E-2</v>
+        <v>2.8273369779352499E-2</v>
       </c>
       <c r="BF25" s="15">
         <f t="shared" ca="1" si="150"/>
@@ -10113,7 +10044,7 @@
       </c>
       <c r="BL25" s="15">
         <f t="shared" ca="1" si="94"/>
-        <v>3.9351868999699995E-2</v>
+        <v>7.7109190307324965E-3</v>
       </c>
       <c r="BN25" s="7" t="s">
         <v>116</v>
@@ -10426,11 +10357,11 @@
       </c>
       <c r="BD26" s="15">
         <f t="shared" ca="1" si="151"/>
-        <v>-1.5271686862268572E-3</v>
+        <v>-8.2631952713828577E-4</v>
       </c>
       <c r="BE26" s="15">
         <f t="shared" ca="1" si="151"/>
-        <v>1.7752910293768573E-3</v>
+        <v>9.4938839288228596E-4</v>
       </c>
       <c r="BF26" s="15">
         <f t="shared" ca="1" si="151"/>
@@ -10458,7 +10389,7 @@
       </c>
       <c r="BL26" s="15">
         <f t="shared" ca="1" si="94"/>
-        <v>1.2505347740600012E-4</v>
+        <v>2.1684043449710089E-19</v>
       </c>
       <c r="BN26" s="7" t="s">
         <v>117</v>
@@ -10598,7 +10529,7 @@
       </c>
       <c r="C27">
         <f ca="1">SUM(AK:AK)</f>
-        <v>0.1869656882289818</v>
+        <v>0.10117738257952287</v>
       </c>
       <c r="E27" s="4" t="str">
         <f t="shared" si="2"/>
@@ -10779,11 +10710,11 @@
       </c>
       <c r="BD27" s="15">
         <f t="shared" ca="1" si="152"/>
-        <v>0.22222657121618433</v>
+        <v>0.10931809152270286</v>
       </c>
       <c r="BE27" s="15">
         <f t="shared" ca="1" si="152"/>
-        <v>-5.1542300873562499E-2</v>
+        <v>-2.4422126829539998E-2</v>
       </c>
       <c r="BF27" s="15">
         <f t="shared" ca="1" si="152"/>
@@ -10811,7 +10742,7 @@
       </c>
       <c r="BL27" s="15">
         <f t="shared" ca="1" si="94"/>
-        <v>0.18696568822898185</v>
+        <v>0.10117738257952287</v>
       </c>
       <c r="BN27" s="7" t="s">
         <v>33</v>
@@ -10955,7 +10886,7 @@
       </c>
       <c r="C28">
         <f ca="1">SUM(AL:AL)</f>
-        <v>-9.7031046353999998E-5</v>
+        <v>-3.0787037040000023E-6</v>
       </c>
       <c r="E28" s="4">
         <f t="shared" ca="1" si="2"/>
@@ -11035,15 +10966,15 @@
       </c>
       <c r="AB28" s="8">
         <f t="shared" ca="1" si="16"/>
-        <v>1.6226363287499999E-4</v>
+        <v>2.5390624999499999E-4</v>
       </c>
       <c r="AC28" s="15">
         <f t="shared" ca="1" si="17"/>
-        <v>-1.0625E-7</v>
+        <v>0</v>
       </c>
       <c r="AD28" s="15">
         <f t="shared" ca="1" si="18"/>
-        <v>-1.0625E-7</v>
+        <v>0</v>
       </c>
       <c r="AE28" s="15">
         <f t="shared" ca="1" si="19"/>
@@ -11051,7 +10982,7 @@
       </c>
       <c r="AF28" s="15">
         <f t="shared" ca="1" si="20"/>
-        <v>2.125E-7</v>
+        <v>0</v>
       </c>
       <c r="AG28" s="15">
         <f t="shared" ca="1" si="21"/>
@@ -11067,11 +10998,11 @@
       </c>
       <c r="AJ28" s="15">
         <f t="shared" ca="1" si="24"/>
-        <v>-3.1211365449E-4</v>
+        <v>-1.6782118055999999E-4</v>
       </c>
       <c r="AK28" s="15">
         <f t="shared" ca="1" si="25"/>
-        <v>4.5447796947705003E-2</v>
+        <v>2.22019334814E-2</v>
       </c>
       <c r="AL28" s="15">
         <f t="shared" ca="1" si="26"/>
@@ -11079,7 +11010,7 @@
       </c>
       <c r="AM28" s="15">
         <f t="shared" ca="1" si="27"/>
-        <v>3.4314768264E-4</v>
+        <v>2.1371527777500001E-4</v>
       </c>
       <c r="AN28">
         <f t="shared" ca="1" si="28"/>
@@ -11146,7 +11077,7 @@
       </c>
       <c r="BE28" s="15">
         <f t="shared" ca="1" si="153"/>
-        <v>-1.15503268578E-4</v>
+        <v>-2.1550925928000002E-5</v>
       </c>
       <c r="BF28" s="15">
         <f t="shared" ca="1" si="153"/>
@@ -11174,7 +11105,7 @@
       </c>
       <c r="BL28" s="15">
         <f t="shared" ca="1" si="94"/>
-        <v>-9.7031046354000011E-5</v>
+        <v>-3.0787037040000023E-6</v>
       </c>
       <c r="BN28" s="7" t="s">
         <v>34</v>
@@ -11317,7 +11248,7 @@
       </c>
       <c r="C29">
         <f ca="1">ROUND(SUM(AM:AM),15)</f>
-        <v>-1.12174750883E-4</v>
+        <v>0</v>
       </c>
       <c r="E29" s="4" t="str">
         <f t="shared" si="2"/>
@@ -11496,11 +11427,11 @@
       </c>
       <c r="BD29" s="15">
         <f t="shared" ca="1" si="154"/>
-        <v>1.6809650008649999E-3</v>
+        <v>1.052293320092143E-3</v>
       </c>
       <c r="BE29" s="15">
         <f t="shared" ca="1" si="154"/>
-        <v>-1.9498642887830001E-3</v>
+        <v>-1.2090178571271429E-3</v>
       </c>
       <c r="BF29" s="15">
         <f t="shared" ca="1" si="154"/>
@@ -11528,7 +11459,7 @@
       </c>
       <c r="BL29" s="15">
         <f t="shared" ca="1" si="94"/>
-        <v>-1.1217475088300013E-4</v>
+        <v>2.1684043449710089E-19</v>
       </c>
       <c r="BN29" s="7" t="s">
         <v>36</v>
@@ -11748,15 +11679,15 @@
       </c>
       <c r="AB30" s="8">
         <f t="shared" ca="1" si="16"/>
-        <v>3.1293700625892855E-4</v>
+        <v>4.8967633927607141E-4</v>
       </c>
       <c r="AC30" s="15">
         <f t="shared" ca="1" si="17"/>
-        <v>-2.0491071428571429E-7</v>
+        <v>0</v>
       </c>
       <c r="AD30" s="15">
         <f t="shared" ca="1" si="18"/>
-        <v>-2.0491071428571429E-7</v>
+        <v>0</v>
       </c>
       <c r="AE30" s="15">
         <f t="shared" ca="1" si="19"/>
@@ -11764,7 +11695,7 @@
       </c>
       <c r="AF30" s="15">
         <f t="shared" ca="1" si="20"/>
-        <v>4.0982142857142859E-7</v>
+        <v>0</v>
       </c>
       <c r="AG30" s="15">
         <f t="shared" ca="1" si="21"/>
@@ -11780,11 +11711,11 @@
       </c>
       <c r="AJ30" s="15">
         <f t="shared" ca="1" si="24"/>
-        <v>-6.1312155522042855E-4</v>
+        <v>-3.3484321264114285E-4</v>
       </c>
       <c r="AK30" s="15">
         <f t="shared" ca="1" si="25"/>
-        <v>8.9129451583619651E-2</v>
+        <v>4.4298143470031429E-2</v>
       </c>
       <c r="AL30" s="15">
         <f t="shared" ca="1" si="26"/>
@@ -11792,7 +11723,7 @@
       </c>
       <c r="AM30" s="15">
         <f t="shared" ca="1" si="27"/>
-        <v>6.7603250170500005E-4</v>
+        <v>4.2641286375107146E-4</v>
       </c>
       <c r="AN30">
         <f t="shared" ca="1" si="28"/>
@@ -11977,7 +11908,7 @@
       </c>
       <c r="C31">
         <f ca="1">ROUND(SUM(AC:AC),15)</f>
-        <v>0</v>
+        <v>2.0999999999999999E-12</v>
       </c>
       <c r="E31" s="4">
         <f t="shared" ca="1" si="2"/>
@@ -12069,11 +12000,11 @@
       </c>
       <c r="AC31" s="15">
         <f t="shared" ca="1" si="17"/>
-        <v>-2.0491071428571429E-7</v>
+        <v>0</v>
       </c>
       <c r="AD31" s="15">
         <f t="shared" ca="1" si="18"/>
-        <v>-2.0491071428571429E-7</v>
+        <v>0</v>
       </c>
       <c r="AE31" s="15">
         <f t="shared" ca="1" si="19"/>
@@ -12081,11 +12012,11 @@
       </c>
       <c r="AF31" s="15">
         <f t="shared" ca="1" si="20"/>
-        <v>4.0982142857142859E-7</v>
+        <v>0</v>
       </c>
       <c r="AG31" s="15">
         <f t="shared" ca="1" si="21"/>
-        <v>2.2572505368642856E-4</v>
+        <v>4.453125000428571E-5</v>
       </c>
       <c r="AH31" s="15">
         <f t="shared" ca="1" si="22"/>
@@ -12097,11 +12028,11 @@
       </c>
       <c r="AJ31" s="15">
         <f t="shared" ca="1" si="24"/>
-        <v>-6.0193347651642855E-4</v>
+        <v>-3.2365513393714285E-4</v>
       </c>
       <c r="AK31" s="15">
         <f t="shared" ca="1" si="25"/>
-        <v>8.7649322684859657E-2</v>
+        <v>4.2818014571271427E-2</v>
       </c>
       <c r="AL31" s="15">
         <f t="shared" ca="1" si="26"/>
@@ -12109,7 +12040,7 @@
       </c>
       <c r="AM31" s="15">
         <f t="shared" ca="1" si="27"/>
-        <v>6.6178481652000006E-4</v>
+        <v>4.1216517856607147E-4</v>
       </c>
       <c r="AN31">
         <f t="shared" ca="1" si="28"/>
@@ -12223,7 +12154,7 @@
       </c>
       <c r="C32">
         <f ca="1">ROUND(SUM(AD:AD),15)</f>
-        <v>0</v>
+        <v>3.8490000000000003E-12</v>
       </c>
       <c r="E32" s="4" t="str">
         <f t="shared" si="2"/>
@@ -12450,17 +12381,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:113">
+    <row r="33" spans="2:118">
       <c r="B33" t="s">
         <v>130</v>
       </c>
       <c r="C33">
         <f ca="1">ROUND(SUM(AE:AE),15)</f>
-        <v>0</v>
+        <v>2.6249999999999998E-12</v>
       </c>
       <c r="E33" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>8.9347017924020636E-5</v>
+        <v>7.9466049074792083E-5</v>
       </c>
       <c r="F33" s="19" t="s">
         <v>44</v>
@@ -12477,7 +12408,7 @@
         <v>3</v>
       </c>
       <c r="L33" s="38">
-        <v>8.9347017924020636E-5</v>
+        <v>7.9466049074792083E-5</v>
       </c>
       <c r="M33" s="19"/>
       <c r="N33" t="str">
@@ -12498,11 +12429,11 @@
       </c>
       <c r="R33" s="10">
         <f t="shared" ca="1" si="6"/>
-        <v>-4.4673508962010319E-4</v>
+        <v>-3.973302453739604E-4</v>
       </c>
       <c r="S33" s="10">
         <f t="shared" ca="1" si="7"/>
-        <v>-7.5944965235417536E-8</v>
+        <v>-6.7546141713573268E-8</v>
       </c>
       <c r="T33" s="10">
         <f t="shared" ca="1" si="8"/>
@@ -12522,7 +12453,7 @@
       </c>
       <c r="X33" s="10">
         <f t="shared" ca="1" si="12"/>
-        <v>2.2783489570625262E-5</v>
+        <v>2.0263842514071982E-5</v>
       </c>
       <c r="Y33" s="10">
         <f t="shared" ca="1" si="13"/>
@@ -12542,11 +12473,11 @@
       </c>
       <c r="AC33" s="15">
         <f t="shared" ca="1" si="17"/>
-        <v>-1.8986241308854386E-11</v>
+        <v>-1.6886535428393316E-11</v>
       </c>
       <c r="AD33" s="15">
         <f t="shared" ca="1" si="18"/>
-        <v>-1.8986241308854386E-11</v>
+        <v>-1.6886535428393316E-11</v>
       </c>
       <c r="AE33" s="15">
         <f t="shared" ca="1" si="19"/>
@@ -12554,7 +12485,7 @@
       </c>
       <c r="AF33" s="15">
         <f t="shared" ca="1" si="20"/>
-        <v>-2.2783451598142642E-5</v>
+        <v>-2.0263808741001122E-5</v>
       </c>
       <c r="AG33" s="15">
         <f t="shared" ca="1" si="21"/>
@@ -12694,13 +12625,13 @@
       </c>
       <c r="DI33">
         <f>DI30/DI21</f>
-        <v>-0.78238803574241733</v>
+        <v>-0.5</v>
       </c>
     </row>
-    <row r="34" spans="2:113">
+    <row r="34" spans="2:118">
       <c r="E34" s="4">
         <f t="shared" ref="E34:E65" ca="1" si="159">IF(P34="","",IF(AND(G34&gt;=200,G34&lt;300),100%,MIN(L34,AY34)))</f>
-        <v>1.7152242271898735E-5</v>
+        <v>8.9181038514698381E-6</v>
       </c>
       <c r="F34" s="19" t="s">
         <v>46</v>
@@ -12723,7 +12654,7 @@
         <v>3</v>
       </c>
       <c r="L34" s="38">
-        <v>1.7152242271898735E-5</v>
+        <v>8.9181038514698381E-6</v>
       </c>
       <c r="M34" s="19">
         <v>1</v>
@@ -12746,11 +12677,11 @@
       </c>
       <c r="R34" s="10">
         <f t="shared" ref="R34:R65" ca="1" si="161">IF($G34="","",IF(AND(G34&gt;=200,G34&lt;300),1,$J34)*LOOKUP($G34,$BO:$BO,BQ:BQ)*$E34+IF(M34="",IF(O34="",0,O34*LOOKUP(100,BO:BO,BQ:BQ)),0))</f>
-        <v>-2.1440302839873419E-5</v>
+        <v>-1.1147629814337297E-5</v>
       </c>
       <c r="S34" s="10">
         <f t="shared" ref="S34:S65" ca="1" si="162">IF($G34="","",$J34*LOOKUP($G34,$BO:$BO,BR:BR)*$E34)</f>
-        <v>-1.4579405931113924E-8</v>
+        <v>-7.5803882737493625E-9</v>
       </c>
       <c r="T34" s="10">
         <f t="shared" ref="T34:T65" ca="1" si="163">IF($G34="","",IF(AND(G34&gt;=200,G34&lt;300),1,$J34)*LOOKUP($G34,$BO:$BO,BS:BS)*$E34+IF($G34=200,INDEX($BA:$BK,MATCH("Karbonite",$BA:$BA,0),MATCH($K34,$BA$1:$BK$1,0)),0))</f>
@@ -12770,7 +12701,7 @@
       </c>
       <c r="X34" s="10">
         <f t="shared" ref="X34:X65" ca="1" si="167">IF($G34="","",$J34*LOOKUP($G34,$BO:$BO,BW:BW)*$E34)</f>
-        <v>-2.6242930676005065E-6</v>
+        <v>-1.3644698892748852E-6</v>
       </c>
       <c r="Y34" s="10">
         <f t="shared" ref="Y34:Y65" ca="1" si="168">IF($G34="","",$J34*LOOKUP($G34,$BO:$BO,BX:BX)*$E34)</f>
@@ -12790,11 +12721,11 @@
       </c>
       <c r="AC34" s="15">
         <f t="shared" ref="AC34:AC65" ca="1" si="172">IF($G34="","",$J34*LOOKUP($G34,$BO:$BO,CC:CC)*$E34)</f>
-        <v>2.6242894227490232E-6</v>
+        <v>1.3644679941778167E-6</v>
       </c>
       <c r="AD34" s="15">
         <f t="shared" ref="AD34:AD65" ca="1" si="173">IF($G34="","",$J34*LOOKUP($G34,$BO:$BO,CD:CD)*$E34)</f>
-        <v>-3.6448514827784816E-12</v>
+        <v>-1.8950970684373407E-12</v>
       </c>
       <c r="AE34" s="15">
         <f t="shared" ref="AE34:AE65" ca="1" si="174">IF($G34="","",$J34*LOOKUP($G34,$BO:$BO,CE:CE)*$E34)</f>
@@ -12802,7 +12733,7 @@
       </c>
       <c r="AF34" s="15">
         <f t="shared" ref="AF34:AF65" ca="1" si="175">IF($G34="","",$J34*LOOKUP($G34,$BO:$BO,CF:CF)*$E34)</f>
-        <v>7.2897029655569631E-12</v>
+        <v>3.7901941368746813E-12</v>
       </c>
       <c r="AG34" s="15">
         <f t="shared" ref="AG34:AG65" ca="1" si="176">IF($G34="","",$J34*LOOKUP($G34,$BO:$BO,CG:CG)*$E34)</f>
@@ -12946,17 +12877,17 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="35" spans="2:113">
+    <row r="35" spans="2:118">
       <c r="B35" t="s">
         <v>131</v>
       </c>
       <c r="C35">
         <f ca="1">ROUND(SUM(AF:AF),15)</f>
-        <v>0</v>
+        <v>-8.749E-12</v>
       </c>
       <c r="E35" s="4">
         <f t="shared" ca="1" si="159"/>
-        <v>4.8959715407254328E-5</v>
+        <v>3.6608499199366468E-5</v>
       </c>
       <c r="F35" s="19" t="s">
         <v>43</v>
@@ -12979,7 +12910,7 @@
         <v>3</v>
       </c>
       <c r="L35" s="38">
-        <v>4.8959715407254328E-5</v>
+        <v>3.6608499199366468E-5</v>
       </c>
       <c r="M35" s="19">
         <v>1</v>
@@ -13002,11 +12933,11 @@
       </c>
       <c r="R35" s="10">
         <f t="shared" ca="1" si="161"/>
-        <v>-6.119964425906791E-5</v>
+        <v>-4.5760623999208081E-5</v>
       </c>
       <c r="S35" s="10">
         <f t="shared" ca="1" si="162"/>
-        <v>-4.1615758096166174E-8</v>
+        <v>-3.1117224319461499E-8</v>
       </c>
       <c r="T35" s="10">
         <f t="shared" ca="1" si="163"/>
@@ -13030,7 +12961,7 @@
       </c>
       <c r="Y35" s="10">
         <f t="shared" ca="1" si="168"/>
-        <v>-4.9938909715399421E-6</v>
+        <v>-3.7340669183353798E-6</v>
       </c>
       <c r="Z35" s="10">
         <f t="shared" ca="1" si="169"/>
@@ -13050,15 +12981,15 @@
       </c>
       <c r="AD35" s="15">
         <f t="shared" ca="1" si="173"/>
-        <v>4.9938805676004168E-6</v>
+        <v>3.7340591390292998E-6</v>
       </c>
       <c r="AE35" s="15">
         <f t="shared" ca="1" si="174"/>
-        <v>-1.0403939524041544E-11</v>
+        <v>-7.779306079865375E-12</v>
       </c>
       <c r="AF35" s="15">
         <f t="shared" ca="1" si="175"/>
-        <v>2.0807879048083089E-11</v>
+        <v>1.555861215973075E-11</v>
       </c>
       <c r="AG35" s="15">
         <f t="shared" ca="1" si="176"/>
@@ -13201,11 +13132,15 @@
         <f>DH15/DH20</f>
         <v>-1</v>
       </c>
+      <c r="DN35">
+        <f>DK30/DN30</f>
+        <v>-0.78525588955171721</v>
+      </c>
     </row>
-    <row r="36" spans="2:113">
+    <row r="36" spans="2:118">
       <c r="E36" s="4">
         <f t="shared" ca="1" si="159"/>
-        <v>2.973589319899093E-4</v>
+        <v>2.9735893198991413E-4</v>
       </c>
       <c r="F36" s="19" t="s">
         <v>45</v>
@@ -13228,7 +13163,7 @@
         <v>3</v>
       </c>
       <c r="L36" s="38">
-        <v>2.973589319899093E-4</v>
+        <v>2.9735893198991413E-4</v>
       </c>
       <c r="M36" s="19">
         <v>1</v>
@@ -13251,11 +13186,11 @@
       </c>
       <c r="R36" s="10">
         <f t="shared" ca="1" si="161"/>
-        <v>-3.7169866498738661E-4</v>
+        <v>-3.7169866498739268E-4</v>
       </c>
       <c r="S36" s="10">
         <f t="shared" ca="1" si="162"/>
-        <v>-2.5275509219142291E-7</v>
+        <v>-2.5275509219142699E-7</v>
       </c>
       <c r="T36" s="10">
         <f t="shared" ca="1" si="163"/>
@@ -13283,7 +13218,7 @@
       </c>
       <c r="Z36" s="10">
         <f t="shared" ca="1" si="169"/>
-        <v>-1.5165305531485375E-5</v>
+        <v>-1.5165305531485621E-5</v>
       </c>
       <c r="AA36" s="10">
         <f t="shared" ca="1" si="170"/>
@@ -13303,11 +13238,11 @@
       </c>
       <c r="AE36" s="15">
         <f t="shared" ca="1" si="174"/>
-        <v>1.5165179153939278E-5</v>
+        <v>1.5165179153939525E-5</v>
       </c>
       <c r="AF36" s="15">
         <f t="shared" ca="1" si="175"/>
-        <v>1.2637754609571147E-10</v>
+        <v>1.2637754609571351E-10</v>
       </c>
       <c r="AG36" s="15">
         <f t="shared" ca="1" si="176"/>
@@ -13448,10 +13383,14 @@
       </c>
       <c r="DI36">
         <f>DM20/DM30</f>
-        <v>-10.137826971607787</v>
+        <v>-2</v>
+      </c>
+      <c r="DN36">
+        <f>DK14/DN14</f>
+        <v>-0.78525588955171732</v>
       </c>
     </row>
-    <row r="37" spans="2:113">
+    <row r="37" spans="2:118">
       <c r="B37" s="41" t="s">
         <v>88</v>
       </c>
@@ -13685,10 +13624,10 @@
       </c>
       <c r="DI37">
         <f>DI36*DI33</f>
-        <v>7.9317145310127151</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:113">
+    <row r="38" spans="2:118">
       <c r="B38" s="25"/>
       <c r="E38" s="4">
         <f t="shared" ca="1" si="159"/>
@@ -13916,7 +13855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:113">
+    <row r="39" spans="2:118">
       <c r="B39" t="s">
         <v>51</v>
       </c>
@@ -14149,7 +14088,7 @@
       <c r="BN39" s="7"/>
       <c r="BO39" s="7"/>
     </row>
-    <row r="40" spans="2:113">
+    <row r="40" spans="2:118">
       <c r="E40" s="4">
         <f t="shared" ca="1" si="159"/>
         <v>0.5</v>
@@ -14380,13 +14319,13 @@
       <c r="CL40" s="15"/>
       <c r="CM40" s="15"/>
     </row>
-    <row r="41" spans="2:113">
+    <row r="41" spans="2:118">
       <c r="B41" t="s">
         <v>89</v>
       </c>
       <c r="C41" s="18" t="str">
         <f ca="1">CONCATENATE(ROUNDDOWN(C65/(60*60*6),0),"d:",ROUNDDOWN(MOD(C65,60*60*6)/3600,0),"h:",ROUNDDOWN(MOD(C65,3600)/60,0),"m:",ROUNDDOWN(MOD(C65,60),0),"s")</f>
-        <v>1d:5h:17m:36s</v>
+        <v>1d:5h:17m:37s</v>
       </c>
       <c r="E41" s="4" t="str">
         <f t="shared" si="159"/>
@@ -14599,7 +14538,7 @@
       <c r="BO41" s="7"/>
       <c r="CM41" s="15"/>
     </row>
-    <row r="42" spans="2:113">
+    <row r="42" spans="2:118">
       <c r="B42" t="s">
         <v>90</v>
       </c>
@@ -14778,7 +14717,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:113">
+    <row r="43" spans="2:118">
       <c r="B43" t="s">
         <v>91</v>
       </c>
@@ -14963,7 +14902,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="44" spans="2:113">
+    <row r="44" spans="2:118">
       <c r="B44" t="s">
         <v>92</v>
       </c>
@@ -15155,7 +15094,7 @@
       <c r="BJ44" s="19"/>
       <c r="BK44" s="19"/>
     </row>
-    <row r="45" spans="2:113">
+    <row r="45" spans="2:118">
       <c r="E45" s="4">
         <f t="shared" si="159"/>
         <v>1</v>
@@ -15340,13 +15279,13 @@
       <c r="BJ45" s="19"/>
       <c r="BK45" s="19"/>
     </row>
-    <row r="46" spans="2:113">
+    <row r="46" spans="2:118">
       <c r="B46" t="s">
         <v>93</v>
       </c>
       <c r="C46" s="18" t="str">
         <f ca="1">CONCATENATE(ROUNDDOWN(C70/(60*60*6),0),"d:",ROUNDDOWN(MOD(C70,60*60*6)/3600,0),"h:",ROUNDDOWN(MOD(C70,3600)/60,0),"m:",ROUNDDOWN(MOD(C70,60),0),"s")</f>
-        <v>10d:5h:43m:34s</v>
+        <v>10d:5h:43m:44s</v>
       </c>
       <c r="E46" s="4">
         <f t="shared" si="159"/>
@@ -15532,13 +15471,13 @@
       <c r="BJ46" s="19"/>
       <c r="BK46" s="19"/>
     </row>
-    <row r="47" spans="2:113">
+    <row r="47" spans="2:118">
       <c r="B47" t="s">
         <v>94</v>
       </c>
       <c r="C47" s="18" t="str">
         <f ca="1">CONCATENATE(ROUNDDOWN(C71/(60*60*6),0),"d:",ROUNDDOWN(MOD(C71,60*60*6)/3600,0),"h:",ROUNDDOWN(MOD(C71,3600)/60,0),"m:",ROUNDDOWN(MOD(C71,60),0),"s")</f>
-        <v>13d:2h:5m:8s</v>
+        <v>13d:2h:4m:53s</v>
       </c>
       <c r="E47" s="4">
         <f t="shared" si="159"/>
@@ -15724,7 +15663,7 @@
       <c r="BJ47" s="19"/>
       <c r="BK47" s="19"/>
     </row>
-    <row r="48" spans="2:113">
+    <row r="48" spans="2:118">
       <c r="B48" t="s">
         <v>95</v>
       </c>
@@ -17563,7 +17502,7 @@
       </c>
       <c r="C58" s="27">
         <f ca="1">-(SUMIF(G:G,"&lt;&gt;7,1",AM:AM)+SUMIFS(O:O,M:M,"",G:G,7.1)*LOOKUP(100,BO:BO,CM:CM))/LOOKUP(7.1,BO:BO,CM:CM)</f>
-        <v>-5.4483223287412584E-3</v>
+        <v>0</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="4">
@@ -17678,7 +17617,7 @@
       </c>
       <c r="AJ58" s="15">
         <f t="shared" ca="1" si="179"/>
-        <v>2.1506117049858572E-3</v>
+        <v>1.1563678489062859E-3</v>
       </c>
       <c r="AK58" s="15">
         <f t="shared" ca="1" si="180"/>
@@ -17690,7 +17629,7 @@
       </c>
       <c r="AM58" s="15">
         <f t="shared" ca="1" si="182"/>
-        <v>-2.3644509370480001E-3</v>
+        <v>-1.472600033049643E-3</v>
       </c>
       <c r="AN58">
         <f t="shared" ca="1" si="183"/>
@@ -17768,7 +17707,7 @@
       </c>
       <c r="C59" s="27">
         <f ca="1">-(SUMIF(G:G,"&lt;&gt;7,4",AM:AM)+SUMIFS(O:O,M:M,"",G:G,7.4)*LOOKUP(100,BO:BO,CM:CM))/LOOKUP(7.4,BO:BO,CM:CM)</f>
-        <v>4.3757179005011436E-2</v>
+        <v>4.5936507936507942E-2</v>
       </c>
       <c r="E59" s="4">
         <f t="shared" ca="1" si="159"/>
@@ -17856,15 +17795,15 @@
       </c>
       <c r="AB59" s="8">
         <f t="shared" ca="1" si="171"/>
-        <v>1.8930757168750001E-4</v>
+        <v>2.9622395832749996E-4</v>
       </c>
       <c r="AC59" s="15">
         <f t="shared" ca="1" si="172"/>
-        <v>-7.4374999999999997E-7</v>
+        <v>0</v>
       </c>
       <c r="AD59" s="15">
         <f t="shared" ca="1" si="173"/>
-        <v>-7.4374999999999997E-7</v>
+        <v>0</v>
       </c>
       <c r="AE59" s="15">
         <f t="shared" ca="1" si="174"/>
@@ -17872,11 +17811,11 @@
       </c>
       <c r="AF59" s="15">
         <f t="shared" ca="1" si="175"/>
-        <v>1.4874999999999999E-6</v>
+        <v>0</v>
       </c>
       <c r="AG59" s="15">
         <f t="shared" ca="1" si="176"/>
-        <v>-1.3654972383500002E-4</v>
+        <v>-2.6938657410000002E-5</v>
       </c>
       <c r="AH59" s="15">
         <f t="shared" ca="1" si="177"/>
@@ -17884,15 +17823,15 @@
       </c>
       <c r="AI59" s="15">
         <f t="shared" ca="1" si="178"/>
-        <v>6.1627857310704998E-2</v>
+        <v>2.99869073417375E-2</v>
       </c>
       <c r="AJ59" s="15">
         <f t="shared" ca="1" si="179"/>
-        <v>-3.6413259690499996E-4</v>
+        <v>-1.9579137732000002E-4</v>
       </c>
       <c r="AK59" s="15">
         <f t="shared" ca="1" si="180"/>
-        <v>-5.30224297723225E-2</v>
+        <v>-2.5902255728299999E-2</v>
       </c>
       <c r="AL59" s="15">
         <f t="shared" ca="1" si="181"/>
@@ -17900,7 +17839,7 @@
       </c>
       <c r="AM59" s="15">
         <f t="shared" ca="1" si="182"/>
-        <v>4.0033896308E-4</v>
+        <v>2.4933449073750004E-4</v>
       </c>
       <c r="AN59">
         <f t="shared" ca="1" si="183"/>
@@ -17978,7 +17917,7 @@
       </c>
       <c r="C60" s="40">
         <f ca="1">-(SUMIF(G:G,"&lt;&gt;3,4",AF:AF))/LOOKUP(3.4,BO:BO,CF:CF)*(1+$C$57)</f>
-        <v>8.9347017924025867E-5</v>
+        <v>7.946601476581051E-5</v>
       </c>
       <c r="E60" s="4">
         <f t="shared" ca="1" si="159"/>
@@ -18182,7 +18121,7 @@
       </c>
       <c r="C61" s="40">
         <f ca="1">-(SUMIF(G:G,"&lt;&gt;3,1",AC:AC))/LOOKUP(3.1,BO:BO,CC:CC)*(1+$C$57)</f>
-        <v>1.7152242271900188E-5</v>
+        <v>8.9180901278829316E-6</v>
       </c>
       <c r="E61" s="4" t="str">
         <f t="shared" si="159"/>
@@ -18374,7 +18313,7 @@
       </c>
       <c r="C62" s="40">
         <f ca="1">-(SUMIF(G:G,"&lt;&gt;3,2",AD:AD))/LOOKUP(3.2,BO:BO,CD:CD)*(1+$C$57)</f>
-        <v>4.8959715407257384E-5</v>
+        <v>3.6608461459481032E-5</v>
       </c>
       <c r="E62" s="4">
         <f t="shared" ca="1" si="159"/>
@@ -18474,7 +18413,7 @@
       </c>
       <c r="AG62" s="15">
         <f t="shared" ca="1" si="176"/>
-        <v>1.1704262043E-4</v>
+        <v>2.3090277780000002E-5</v>
       </c>
       <c r="AH62" s="15">
         <f t="shared" ca="1" si="177"/>
@@ -18494,7 +18433,7 @@
       </c>
       <c r="AL62" s="15">
         <f t="shared" ca="1" si="181"/>
-        <v>-1.1704262043E-4</v>
+        <v>-2.3090277780000002E-5</v>
       </c>
       <c r="AM62" s="15">
         <f t="shared" ca="1" si="182"/>
@@ -18576,7 +18515,7 @@
       </c>
       <c r="C63" s="40">
         <f ca="1">-(SUMIF(G:G,"&lt;&gt;3,3",AE:AE))/LOOKUP(3.3,BO:BO,CE:CE)*(1+$C$57)</f>
-        <v>2.9735893198991413E-4</v>
+        <v>2.9735888052608435E-4</v>
       </c>
       <c r="E63" s="4">
         <f t="shared" ca="1" si="159"/>
@@ -18664,7 +18603,7 @@
       </c>
       <c r="AB63" s="8">
         <f t="shared" ca="1" si="171"/>
-        <v>-1.6226363287500002E-4</v>
+        <v>-2.5390624999499999E-4</v>
       </c>
       <c r="AC63" s="15">
         <f t="shared" ca="1" si="172"/>
@@ -18688,7 +18627,7 @@
       </c>
       <c r="AH63" s="15">
         <f t="shared" ca="1" si="177"/>
-        <v>1.6226363287500002E-4</v>
+        <v>2.5390624999499999E-4</v>
       </c>
       <c r="AI63" s="15">
         <f t="shared" ca="1" si="178"/>
@@ -18871,10 +18810,7 @@
         <f t="shared" si="176"/>
         <v/>
       </c>
-      <c r="AH64" s="15">
-        <f ca="1">$J63*LOOKUP($G63,$BO:$BO,CH:CH)*$E63</f>
-        <v>1.6226363287500002E-4</v>
-      </c>
+      <c r="AH64" s="15"/>
       <c r="AI64" s="15" t="str">
         <f t="shared" si="178"/>
         <v/>
@@ -18965,7 +18901,7 @@
       </c>
       <c r="C65" s="26">
         <f ca="1">$C$39/C75</f>
-        <v>40656.927775221848</v>
+        <v>40657.522860477809</v>
       </c>
       <c r="E65" s="4">
         <f t="shared" si="159"/>
@@ -19167,22 +19103,16 @@
         <f ca="1">$C$39/C76</f>
         <v>49093.258252002233</v>
       </c>
-      <c r="E66" s="4">
+      <c r="E66" s="4" t="str">
         <f t="shared" ref="E66:E97" si="213">IF(P66="","",IF(AND(G66&gt;=200,G66&lt;300),100%,MIN(L66,AY66)))</f>
-        <v>1</v>
-      </c>
-      <c r="F66" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="G66" s="34">
-        <v>200</v>
-      </c>
+        <v/>
+      </c>
+      <c r="F66" s="19"/>
+      <c r="G66" s="34"/>
       <c r="H66" s="35"/>
       <c r="I66" s="35"/>
       <c r="J66" s="36"/>
-      <c r="K66" s="19">
-        <v>4</v>
-      </c>
+      <c r="K66" s="19"/>
       <c r="L66" s="37"/>
       <c r="M66" s="19"/>
       <c r="N66" t="str">
@@ -19193,101 +19123,101 @@
         <f t="shared" si="39"/>
         <v/>
       </c>
-      <c r="P66">
+      <c r="P66" t="str">
         <f t="shared" si="92"/>
-        <v>0</v>
-      </c>
-      <c r="Q66">
+        <v/>
+      </c>
+      <c r="Q66" t="str">
         <f t="shared" si="40"/>
-        <v>1</v>
-      </c>
-      <c r="R66" s="10">
+        <v/>
+      </c>
+      <c r="R66" s="10" t="str">
         <f t="shared" ref="R66:R97" si="214">IF($G66="","",IF(AND(G66&gt;=200,G66&lt;300),1,$J66)*LOOKUP($G66,$BO:$BO,BQ:BQ)*$E66+IF(M66="",IF(O66="",0,O66*LOOKUP(100,BO:BO,BQ:BQ)),0))</f>
-        <v>-2.5</v>
-      </c>
-      <c r="S66" s="10">
+        <v/>
+      </c>
+      <c r="S66" s="10" t="str">
         <f t="shared" ref="S66:S97" si="215">IF($G66="","",$J66*LOOKUP($G66,$BO:$BO,BR:BR)*$E66)</f>
-        <v>0</v>
-      </c>
-      <c r="T66" s="10">
-        <f t="shared" ref="T66:T97" ca="1" si="216">IF($G66="","",IF(AND(G66&gt;=200,G66&lt;300),1,$J66)*LOOKUP($G66,$BO:$BO,BS:BS)*$E66+IF($G66=200,INDEX($BA:$BK,MATCH("Karbonite",$BA:$BA,0),MATCH($K66,$BA$1:$BK$1,0)),0))</f>
-        <v>0.49951111111111113</v>
-      </c>
-      <c r="U66" s="10">
+        <v/>
+      </c>
+      <c r="T66" s="10" t="str">
+        <f t="shared" ref="T66:T97" si="216">IF($G66="","",IF(AND(G66&gt;=200,G66&lt;300),1,$J66)*LOOKUP($G66,$BO:$BO,BS:BS)*$E66+IF($G66=200,INDEX($BA:$BK,MATCH("Karbonite",$BA:$BA,0),MATCH($K66,$BA$1:$BK$1,0)),0))</f>
+        <v/>
+      </c>
+      <c r="U66" s="10" t="str">
         <f t="shared" ref="U66:U97" si="217">IF($G66="","",$J66*LOOKUP($G66,$BO:$BO,BT:BT)*$E66+IF($G66=201,INDEX($BA:$BK,MATCH("Ore",$BA:$BA,0),MATCH($K66,$BA$1:$BK$1,0)),0))</f>
-        <v>0</v>
-      </c>
-      <c r="V66" s="10">
+        <v/>
+      </c>
+      <c r="V66" s="10" t="str">
         <f t="shared" ref="V66:V97" si="218">IF($G66="","",$J66*LOOKUP($G66,$BO:$BO,BU:BU)*$E66+IF($G66=202,INDEX($BA:$BK,MATCH("Minerals",$BA:$BA,0),MATCH($K66,$BA$1:$BK$1,0)),0))</f>
-        <v>0</v>
-      </c>
-      <c r="W66" s="10">
+        <v/>
+      </c>
+      <c r="W66" s="10" t="str">
         <f t="shared" ref="W66:W97" si="219">IF($G66="","",$J66*LOOKUP($G66,$BO:$BO,BV:BV)*$E66+IF($G66=203,INDEX($BA:$BK,MATCH("Substrate",$BA:$BA,0),MATCH($K66,$BA$1:$BK$1,0)),0))</f>
-        <v>0</v>
-      </c>
-      <c r="X66" s="10">
+        <v/>
+      </c>
+      <c r="X66" s="10" t="str">
         <f t="shared" ref="X66:X97" si="220">IF($G66="","",$J66*LOOKUP($G66,$BO:$BO,BW:BW)*$E66)</f>
-        <v>0</v>
-      </c>
-      <c r="Y66" s="10">
+        <v/>
+      </c>
+      <c r="Y66" s="10" t="str">
         <f t="shared" ref="Y66:Y97" si="221">IF($G66="","",$J66*LOOKUP($G66,$BO:$BO,BX:BX)*$E66)</f>
-        <v>0</v>
-      </c>
-      <c r="Z66" s="10">
+        <v/>
+      </c>
+      <c r="Z66" s="10" t="str">
         <f t="shared" ref="Z66:Z97" si="222">IF($G66="","",$J66*LOOKUP($G66,$BO:$BO,BY:BY)*$E66)</f>
-        <v>0</v>
-      </c>
-      <c r="AA66" s="10">
+        <v/>
+      </c>
+      <c r="AA66" s="10" t="str">
         <f t="shared" ref="AA66:AA97" si="223">IF($G66="","",$J66*LOOKUP($G66,$BO:$BO,BZ:BZ)*$E66)</f>
-        <v>0</v>
-      </c>
-      <c r="AB66" s="8">
+        <v/>
+      </c>
+      <c r="AB66" s="8" t="str">
         <f t="shared" ref="AB66:AB97" si="224">IF($G66="","",$J66*LOOKUP($G66,$BO:$BO,CB:CB)*$E66)</f>
-        <v>0</v>
-      </c>
-      <c r="AC66" s="15">
+        <v/>
+      </c>
+      <c r="AC66" s="15" t="str">
         <f t="shared" ref="AC66:AC97" si="225">IF($G66="","",$J66*LOOKUP($G66,$BO:$BO,CC:CC)*$E66)</f>
-        <v>0</v>
-      </c>
-      <c r="AD66" s="15">
+        <v/>
+      </c>
+      <c r="AD66" s="15" t="str">
         <f t="shared" ref="AD66:AD97" si="226">IF($G66="","",$J66*LOOKUP($G66,$BO:$BO,CD:CD)*$E66)</f>
-        <v>0</v>
-      </c>
-      <c r="AE66" s="15">
+        <v/>
+      </c>
+      <c r="AE66" s="15" t="str">
         <f t="shared" ref="AE66:AE97" si="227">IF($G66="","",$J66*LOOKUP($G66,$BO:$BO,CE:CE)*$E66)</f>
-        <v>0</v>
-      </c>
-      <c r="AF66" s="15">
+        <v/>
+      </c>
+      <c r="AF66" s="15" t="str">
         <f t="shared" ref="AF66:AF97" si="228">IF($G66="","",$J66*LOOKUP($G66,$BO:$BO,CF:CF)*$E66)</f>
-        <v>0</v>
-      </c>
-      <c r="AG66" s="15">
+        <v/>
+      </c>
+      <c r="AG66" s="15" t="str">
         <f t="shared" ref="AG66:AG97" si="229">IF($G66="","",$J66*LOOKUP($G66,$BO:$BO,CG:CG)*$E66)</f>
-        <v>0</v>
-      </c>
-      <c r="AH66" s="15">
+        <v/>
+      </c>
+      <c r="AH66" s="15" t="str">
         <f t="shared" ref="AH66:AH97" si="230">IF($G66="","",$J66*LOOKUP($G66,$BO:$BO,CH:CH)*$E66+IF($M66=1,0,IF($O66="",0,$O66*LOOKUP(100,$BO:$BO,CH:CH))))</f>
-        <v>0</v>
-      </c>
-      <c r="AI66" s="15">
+        <v/>
+      </c>
+      <c r="AI66" s="15" t="str">
         <f t="shared" ref="AI66:AI97" si="231">IF($G66="","",$J66*LOOKUP($G66,$BO:$BO,CI:CI)*$E66+IF($M66=1,0,IF($O66="",0,$O66*LOOKUP(100,$BO:$BO,CI:CI))))</f>
-        <v>0</v>
-      </c>
-      <c r="AJ66" s="15">
+        <v/>
+      </c>
+      <c r="AJ66" s="15" t="str">
         <f t="shared" ref="AJ66:AJ97" si="232">IF($G66="","",$J66*LOOKUP($G66,$BO:$BO,CJ:CJ)*$E66+IF($M66=1,0,IF($O66="",0,$O66*LOOKUP(100,$BO:$BO,CJ:CJ)))+IF($G66=204,INDEX($BA:$BK,MATCH("Water",$BA:$BA,0),MATCH($K66,$BA$1:$BK$1,0)),0))</f>
-        <v>0</v>
-      </c>
-      <c r="AK66" s="15">
+        <v/>
+      </c>
+      <c r="AK66" s="15" t="str">
         <f t="shared" ref="AK66:AK97" si="233">IF($G66="","",$J66*LOOKUP($G66,$BO:$BO,CK:CK)*$E66+IF($M66=1,0,IF($O66="",0,$O66*LOOKUP(100,$BO:$BO,CK:CK))))</f>
-        <v>0</v>
-      </c>
-      <c r="AL66" s="15">
+        <v/>
+      </c>
+      <c r="AL66" s="15" t="str">
         <f t="shared" ref="AL66:AL97" si="234">IF($G66="","",$J66*LOOKUP($G66,$BO:$BO,CL:CL)*$E66+IF($M66=1,0,IF($O66="",0,$O66*LOOKUP(100,$BO:$BO,CL:CL))))</f>
-        <v>0</v>
-      </c>
-      <c r="AM66" s="15">
+        <v/>
+      </c>
+      <c r="AM66" s="15" t="str">
         <f t="shared" ref="AM66:AM97" si="235">IF($G66="","",$J66*LOOKUP($G66,$BO:$BO,CM:CM)*$E66+IF($M66=1,0,IF($O66="",0,$O66*LOOKUP(100,$BO:$BO,CM:CM))))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="AN66" t="str">
         <f t="shared" ref="AN66:AN97" si="236">IF(P66=1,LOOKUP(K66,$BB$1:$BK$1,$BB$32:$BK$32)-IF(O66="",0,O66),"")</f>
@@ -19313,17 +19243,17 @@
         <f t="shared" ref="AS66:AS97" si="241">IF(AQ66="","",IF(LOOKUP(K66,$BB$1:$BK$1,$BB$32:$BK$32)=0,0.25,MAX(MIN(AR66,2.5),0.5)))</f>
         <v/>
       </c>
-      <c r="AT66">
+      <c r="AT66" t="str">
         <f t="shared" si="41"/>
-        <v>200</v>
-      </c>
-      <c r="AU66">
+        <v/>
+      </c>
+      <c r="AU66" t="str">
         <f t="shared" si="42"/>
-        <v>0</v>
-      </c>
-      <c r="AV66">
+        <v/>
+      </c>
+      <c r="AV66" t="str">
         <f t="shared" ref="AV66:AV97" si="242">IF(P66="","",LOOKUP(G66,BO:BO,BP:BP))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="AW66" t="str">
         <f t="shared" ref="AW66:AW97" si="243">IF(OR(AV66="",AV66=0),"",INDEX($BA$1:$BK$7,MATCH(AV66,$BA$1:$BA$7,0),MATCH(K66,$BA$1:$BK$1,0)))</f>
@@ -19693,7 +19623,7 @@
         <v/>
       </c>
       <c r="F69" s="19" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="G69" s="34"/>
       <c r="H69" s="35"/>
@@ -19867,7 +19797,7 @@
       </c>
       <c r="C70" s="10">
         <f ca="1">$C$39/C16*3</f>
-        <v>236614.5022853142</v>
+        <v>236624.58030165161</v>
       </c>
       <c r="E70" s="4">
         <f t="shared" si="213"/>
@@ -20089,7 +20019,7 @@
       </c>
       <c r="C71" s="10">
         <f ca="1">$C$39/C17*3</f>
-        <v>288308.18124480918</v>
+        <v>288293.22008376435</v>
       </c>
       <c r="E71" s="4">
         <f t="shared" si="213"/>
@@ -20962,7 +20892,7 @@
       </c>
       <c r="C75">
         <f ca="1">SUMIF(X:X,"&gt;0",X:X)/3</f>
-        <v>5.7382594496523533E-2</v>
+        <v>5.7381754614171353E-2</v>
       </c>
       <c r="E75" s="4" t="str">
         <f t="shared" si="213"/>
@@ -22583,7 +22513,7 @@
       </c>
       <c r="C83" s="10">
         <f ca="1">SUMIF(AJ:AJ,"&lt;0")*60*60*6</f>
-        <v>-43.752057715724916</v>
+        <v>-24.977545536375775</v>
       </c>
       <c r="E83" s="4" t="str">
         <f t="shared" si="213"/>
@@ -28994,114 +28924,4 @@
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:G7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="3" spans="2:7">
-      <c r="B3" t="s">
-        <v>213</v>
-      </c>
-      <c r="C3" t="s">
-        <v>214</v>
-      </c>
-      <c r="D3" t="s">
-        <v>215</v>
-      </c>
-      <c r="E3" t="s">
-        <v>216</v>
-      </c>
-      <c r="F3" t="s">
-        <v>217</v>
-      </c>
-      <c r="G3" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7">
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>16</v>
-      </c>
-      <c r="D4">
-        <f>C4+60*B4</f>
-        <v>76</v>
-      </c>
-      <c r="E4">
-        <v>962</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7">
-      <c r="B5">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>28</v>
-      </c>
-      <c r="D5">
-        <f>C5+60*B5</f>
-        <v>628</v>
-      </c>
-      <c r="E5">
-        <v>971</v>
-      </c>
-      <c r="F5">
-        <f>D5-D4</f>
-        <v>552</v>
-      </c>
-      <c r="G5">
-        <f>E5-E4</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7">
-      <c r="B6">
-        <v>14</v>
-      </c>
-      <c r="C6">
-        <v>39</v>
-      </c>
-      <c r="D6">
-        <f>C6+60*B6</f>
-        <v>879</v>
-      </c>
-      <c r="E6">
-        <v>975</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7">
-      <c r="B7">
-        <v>23</v>
-      </c>
-      <c r="C7">
-        <v>45</v>
-      </c>
-      <c r="D7">
-        <f>C7+60*B7</f>
-        <v>1425</v>
-      </c>
-      <c r="E7">
-        <v>985</v>
-      </c>
-      <c r="F7" t="s">
-        <v>219</v>
-      </c>
-      <c r="G7">
-        <f>E7-E6</f>
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>